<commit_message>
added more categories to the expertise column
</commit_message>
<xml_diff>
--- a/data/Walnut_grain_veg_tub.xlsx
+++ b/data/Walnut_grain_veg_tub.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\belgium_app\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mjimenez\Documents\Stakeholder process\ReForest\Belgium\Dynamic-Shiny - MarcosEdited\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08881748-4685-49DB-A62D-D6743DB00530}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21D71331-C3C7-4170-99AB-A785FF834B4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1905" yWindow="1905" windowWidth="21600" windowHeight="11295" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sheet_names" sheetId="17" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="865" uniqueCount="315">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="865" uniqueCount="314">
   <si>
     <t>variable</t>
   </si>
@@ -974,9 +974,6 @@
   </si>
   <si>
     <t>Market analysis</t>
-  </si>
-  <si>
-    <t>Decision maker;Data analyst</t>
   </si>
 </sst>
 </file>
@@ -1474,48 +1471,48 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
-    <cellStyle name="20 % - Akzent1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20 % - Akzent2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20 % - Akzent3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20 % - Akzent4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20 % - Akzent5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20 % - Akzent6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40 % - Akzent1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40 % - Akzent2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40 % - Akzent3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40 % - Akzent4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40 % - Akzent5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40 % - Akzent6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60 % - Akzent1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60 % - Akzent2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60 % - Akzent3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60 % - Akzent4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60 % - Akzent5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60 % - Akzent6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Akzent1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Akzent2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Akzent3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Akzent4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Akzent5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Akzent6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Ausgabe" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Berechnung" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Eingabe" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Ergebnis" xfId="17" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Erklärender Text" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Gut" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
-    <cellStyle name="Notiz" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Schlecht" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
-    <cellStyle name="Überschrift" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Überschrift 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Überschrift 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Überschrift 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Überschrift 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Verknüpfte Zelle" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Warnender Text" xfId="14" builtinId="11" customBuiltin="1"/>
-    <cellStyle name="Zelle überprüfen" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1531,7 +1528,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1829,76 +1826,76 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6B894F3-1BBC-4877-818A-ECEC60560258}">
   <dimension ref="A1:A13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="37.140625" customWidth="1"/>
+    <col min="1" max="1" width="37.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>162</v>
       </c>
@@ -1917,16 +1914,16 @@
       <selection activeCell="I1" sqref="I1:I1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="28.28515625" customWidth="1"/>
-    <col min="2" max="2" width="11.42578125" customWidth="1"/>
-    <col min="3" max="3" width="10.85546875" customWidth="1"/>
-    <col min="6" max="6" width="94.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.42578125" customWidth="1"/>
+    <col min="1" max="1" width="28.26953125" customWidth="1"/>
+    <col min="2" max="2" width="11.453125" customWidth="1"/>
+    <col min="3" max="3" width="10.81640625" customWidth="1"/>
+    <col min="6" max="6" width="94.08984375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1955,7 +1952,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>57</v>
       </c>
@@ -1984,7 +1981,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>58</v>
       </c>
@@ -2013,7 +2010,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>59</v>
       </c>
@@ -2042,7 +2039,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>61</v>
       </c>
@@ -2084,14 +2081,14 @@
       <selection activeCell="I1" sqref="I1:I1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="38.85546875" customWidth="1"/>
-    <col min="6" max="6" width="160.5703125" customWidth="1"/>
-    <col min="9" max="9" width="18.42578125" customWidth="1"/>
+    <col min="1" max="1" width="38.81640625" customWidth="1"/>
+    <col min="6" max="6" width="160.54296875" customWidth="1"/>
+    <col min="9" max="9" width="18.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2120,7 +2117,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>104</v>
       </c>
@@ -2149,7 +2146,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>106</v>
       </c>
@@ -2178,7 +2175,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>107</v>
       </c>
@@ -2207,7 +2204,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>108</v>
       </c>
@@ -2236,7 +2233,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>150</v>
       </c>
@@ -2265,7 +2262,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>111</v>
       </c>
@@ -2294,7 +2291,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>112</v>
       </c>
@@ -2323,7 +2320,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>113</v>
       </c>
@@ -2352,7 +2349,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>114</v>
       </c>
@@ -2381,7 +2378,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>116</v>
       </c>
@@ -2410,7 +2407,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>117</v>
       </c>
@@ -2439,7 +2436,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>118</v>
       </c>
@@ -2468,7 +2465,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>119</v>
       </c>
@@ -2497,7 +2494,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>149</v>
       </c>
@@ -2526,7 +2523,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>148</v>
       </c>
@@ -2555,7 +2552,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>121</v>
       </c>
@@ -2584,7 +2581,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>123</v>
       </c>
@@ -2613,7 +2610,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>147</v>
       </c>
@@ -2655,14 +2652,14 @@
       <selection activeCell="I1" sqref="I1:I1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="29.140625" customWidth="1"/>
-    <col min="6" max="6" width="52.85546875" customWidth="1"/>
-    <col min="9" max="9" width="18.42578125" customWidth="1"/>
+    <col min="1" max="1" width="29.08984375" customWidth="1"/>
+    <col min="6" max="6" width="52.90625" customWidth="1"/>
+    <col min="9" max="9" width="18.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2691,7 +2688,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>157</v>
       </c>
@@ -2720,483 +2717,483 @@
         <v>313</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
     </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
     </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
     </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
     </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
     </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
     </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
     </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
     </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
     </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
     </row>
-    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
     </row>
-    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
     </row>
-    <row r="29" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
     </row>
-    <row r="30" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
     </row>
-    <row r="31" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
     </row>
-    <row r="32" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
     </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
     </row>
-    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
     </row>
-    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
     </row>
-    <row r="36" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
     </row>
-    <row r="37" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
     </row>
-    <row r="38" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
     </row>
-    <row r="39" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
     </row>
-    <row r="40" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
     </row>
-    <row r="41" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
     </row>
-    <row r="42" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
     </row>
-    <row r="43" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
     </row>
-    <row r="44" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
     </row>
-    <row r="45" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
     </row>
-    <row r="46" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>
     </row>
-    <row r="47" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
     </row>
-    <row r="48" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B48" s="1"/>
       <c r="C48" s="1"/>
     </row>
-    <row r="49" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B49" s="1"/>
       <c r="C49" s="1"/>
     </row>
-    <row r="50" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B50" s="1"/>
       <c r="C50" s="1"/>
     </row>
-    <row r="51" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B51" s="1"/>
       <c r="C51" s="1"/>
     </row>
-    <row r="52" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B52" s="1"/>
       <c r="C52" s="1"/>
     </row>
-    <row r="53" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B53" s="1"/>
       <c r="C53" s="1"/>
     </row>
-    <row r="54" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B54" s="1"/>
       <c r="C54" s="1"/>
     </row>
-    <row r="55" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B55" s="1"/>
       <c r="C55" s="1"/>
     </row>
-    <row r="56" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B56" s="1"/>
       <c r="C56" s="1"/>
     </row>
-    <row r="57" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B57" s="1"/>
       <c r="C57" s="1"/>
     </row>
-    <row r="58" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B58" s="1"/>
       <c r="C58" s="1"/>
     </row>
-    <row r="59" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B59" s="1"/>
       <c r="C59" s="1"/>
     </row>
-    <row r="60" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B60" s="1"/>
       <c r="C60" s="1"/>
     </row>
-    <row r="61" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B61" s="1"/>
       <c r="C61" s="1"/>
     </row>
-    <row r="62" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B62" s="1"/>
       <c r="C62" s="1"/>
     </row>
-    <row r="63" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B63" s="1"/>
       <c r="C63" s="1"/>
     </row>
-    <row r="64" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B64" s="1"/>
       <c r="C64" s="1"/>
     </row>
-    <row r="65" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B65" s="1"/>
       <c r="C65" s="1"/>
     </row>
-    <row r="66" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B66" s="1"/>
       <c r="C66" s="1"/>
     </row>
-    <row r="67" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B67" s="1"/>
       <c r="C67" s="1"/>
     </row>
-    <row r="68" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B68" s="1"/>
       <c r="C68" s="1"/>
     </row>
-    <row r="69" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B69" s="1"/>
       <c r="C69" s="1"/>
     </row>
-    <row r="70" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B70" s="1"/>
       <c r="C70" s="1"/>
     </row>
-    <row r="71" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B71" s="1"/>
       <c r="C71" s="1"/>
     </row>
-    <row r="72" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B72" s="1"/>
       <c r="C72" s="1"/>
     </row>
-    <row r="73" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="73" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B73" s="1"/>
       <c r="C73" s="1"/>
     </row>
-    <row r="74" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B74" s="1"/>
       <c r="C74" s="1"/>
     </row>
-    <row r="75" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="75" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B75" s="1"/>
       <c r="C75" s="1"/>
     </row>
-    <row r="76" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="76" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B76" s="1"/>
       <c r="C76" s="1"/>
     </row>
-    <row r="77" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="77" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B77" s="1"/>
       <c r="C77" s="1"/>
     </row>
-    <row r="78" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="78" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B78" s="1"/>
       <c r="C78" s="1"/>
     </row>
-    <row r="79" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="79" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B79" s="1"/>
       <c r="C79" s="1"/>
     </row>
-    <row r="80" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="80" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B80" s="1"/>
       <c r="C80" s="1"/>
     </row>
-    <row r="81" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="81" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B81" s="1"/>
       <c r="C81" s="1"/>
     </row>
-    <row r="82" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="82" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B82" s="1"/>
       <c r="C82" s="1"/>
     </row>
-    <row r="83" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="83" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B83" s="1"/>
       <c r="C83" s="1"/>
     </row>
-    <row r="84" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="84" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B84" s="1"/>
       <c r="C84" s="1"/>
     </row>
-    <row r="85" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="85" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B85" s="1"/>
       <c r="C85" s="1"/>
     </row>
-    <row r="86" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="86" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B86" s="1"/>
       <c r="C86" s="1"/>
     </row>
-    <row r="87" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="87" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B87" s="1"/>
       <c r="C87" s="1"/>
     </row>
-    <row r="88" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="88" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B88" s="1"/>
       <c r="C88" s="1"/>
     </row>
-    <row r="89" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="89" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B89" s="1"/>
       <c r="C89" s="1"/>
     </row>
-    <row r="90" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="90" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B90" s="1"/>
       <c r="C90" s="1"/>
     </row>
-    <row r="91" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="91" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B91" s="1"/>
       <c r="C91" s="1"/>
     </row>
-    <row r="92" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="92" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B92" s="1"/>
       <c r="C92" s="1"/>
     </row>
-    <row r="93" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="93" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B93" s="1"/>
       <c r="C93" s="1"/>
     </row>
-    <row r="94" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="94" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B94" s="1"/>
       <c r="C94" s="1"/>
     </row>
-    <row r="95" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="95" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B95" s="1"/>
       <c r="C95" s="1"/>
     </row>
-    <row r="96" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="96" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B96" s="1"/>
       <c r="C96" s="1"/>
     </row>
-    <row r="97" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="97" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B97" s="1"/>
       <c r="C97" s="1"/>
     </row>
-    <row r="98" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="98" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B98" s="1"/>
       <c r="C98" s="1"/>
     </row>
-    <row r="99" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="99" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B99" s="1"/>
       <c r="C99" s="1"/>
     </row>
-    <row r="100" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="100" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B100" s="1"/>
       <c r="C100" s="1"/>
     </row>
-    <row r="101" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="101" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B101" s="1"/>
       <c r="C101" s="1"/>
     </row>
-    <row r="102" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="102" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B102" s="1"/>
       <c r="C102" s="1"/>
     </row>
-    <row r="103" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="103" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B103" s="1"/>
       <c r="C103" s="1"/>
     </row>
-    <row r="104" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="104" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B104" s="1"/>
       <c r="C104" s="1"/>
     </row>
-    <row r="105" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="105" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B105" s="1"/>
       <c r="C105" s="1"/>
     </row>
-    <row r="106" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="106" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B106" s="1"/>
       <c r="C106" s="1"/>
     </row>
-    <row r="107" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="107" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B107" s="1"/>
       <c r="C107" s="1"/>
     </row>
-    <row r="108" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="108" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B108" s="1"/>
       <c r="C108" s="1"/>
     </row>
-    <row r="109" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="109" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B109" s="1"/>
       <c r="C109" s="1"/>
     </row>
-    <row r="110" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="110" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B110" s="1"/>
       <c r="C110" s="1"/>
     </row>
-    <row r="111" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="111" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B111" s="1"/>
       <c r="C111" s="1"/>
     </row>
-    <row r="112" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="112" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B112" s="1"/>
       <c r="C112" s="1"/>
     </row>
-    <row r="113" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="113" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B113" s="1"/>
       <c r="C113" s="1"/>
     </row>
-    <row r="114" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="114" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B114" s="1"/>
       <c r="C114" s="1"/>
     </row>
-    <row r="115" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="115" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B115" s="1"/>
       <c r="C115" s="1"/>
     </row>
-    <row r="116" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="116" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B116" s="1"/>
       <c r="C116" s="1"/>
     </row>
-    <row r="117" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="117" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B117" s="1"/>
       <c r="C117" s="1"/>
     </row>
-    <row r="118" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="118" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B118" s="1"/>
       <c r="C118" s="1"/>
     </row>
-    <row r="119" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="119" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B119" s="1"/>
       <c r="C119" s="1"/>
     </row>
-    <row r="120" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="120" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B120" s="1"/>
       <c r="C120" s="1"/>
     </row>
-    <row r="121" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="121" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B121" s="1"/>
       <c r="C121" s="1"/>
     </row>
-    <row r="122" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="122" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B122" s="1"/>
       <c r="C122" s="1"/>
     </row>
@@ -3213,17 +3210,17 @@
       <selection activeCell="I1" sqref="I1:I1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="27" customWidth="1"/>
-    <col min="2" max="2" width="13.140625" customWidth="1"/>
-    <col min="3" max="3" width="8.7109375" customWidth="1"/>
-    <col min="6" max="6" width="59.42578125" customWidth="1"/>
-    <col min="7" max="7" width="33.5703125" customWidth="1"/>
-    <col min="9" max="9" width="10.85546875" customWidth="1"/>
+    <col min="2" max="2" width="13.08984375" customWidth="1"/>
+    <col min="3" max="3" width="8.7265625" customWidth="1"/>
+    <col min="6" max="6" width="59.453125" customWidth="1"/>
+    <col min="7" max="7" width="33.54296875" customWidth="1"/>
+    <col min="9" max="9" width="10.90625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3252,7 +3249,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>37</v>
       </c>
@@ -3281,7 +3278,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>39</v>
       </c>
@@ -3310,7 +3307,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>156</v>
       </c>
@@ -3339,7 +3336,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>155</v>
       </c>
@@ -3378,19 +3375,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06826C72-96B8-4DB0-B8A1-5FBF5F35F3F2}">
   <dimension ref="A1:I121"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1:I1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="36.7109375" customWidth="1"/>
-    <col min="2" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="55.42578125" customWidth="1"/>
-    <col min="9" max="9" width="18.42578125" customWidth="1"/>
+    <col min="1" max="1" width="36.7265625" customWidth="1"/>
+    <col min="2" max="3" width="10.36328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="55.36328125" customWidth="1"/>
+    <col min="9" max="9" width="18.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3419,7 +3416,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -3445,10 +3442,10 @@
         <v>1</v>
       </c>
       <c r="I2" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -3477,7 +3474,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>54</v>
       </c>
@@ -3506,7 +3503,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>56</v>
       </c>
@@ -3535,7 +3532,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -3564,7 +3561,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -3593,459 +3590,459 @@
         <v>311</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
     </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
     </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
     </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
     </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
     </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
     </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
     </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
     </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
     </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
     </row>
-    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
     </row>
-    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
     </row>
-    <row r="29" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
     </row>
-    <row r="30" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
     </row>
-    <row r="31" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
     </row>
-    <row r="32" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
     </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
     </row>
-    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
     </row>
-    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
     </row>
-    <row r="36" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
     </row>
-    <row r="37" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
     </row>
-    <row r="38" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
     </row>
-    <row r="39" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
     </row>
-    <row r="40" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
     </row>
-    <row r="41" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
     </row>
-    <row r="42" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
     </row>
-    <row r="43" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
     </row>
-    <row r="44" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
     </row>
-    <row r="45" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
     </row>
-    <row r="46" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>
     </row>
-    <row r="47" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
     </row>
-    <row r="48" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B48" s="1"/>
       <c r="C48" s="1"/>
     </row>
-    <row r="49" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B49" s="1"/>
       <c r="C49" s="1"/>
     </row>
-    <row r="50" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B50" s="1"/>
       <c r="C50" s="1"/>
     </row>
-    <row r="51" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B51" s="1"/>
       <c r="C51" s="1"/>
     </row>
-    <row r="52" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B52" s="1"/>
       <c r="C52" s="1"/>
     </row>
-    <row r="53" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B53" s="1"/>
       <c r="C53" s="1"/>
     </row>
-    <row r="54" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B54" s="1"/>
       <c r="C54" s="1"/>
     </row>
-    <row r="55" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B55" s="1"/>
       <c r="C55" s="1"/>
     </row>
-    <row r="56" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B56" s="1"/>
       <c r="C56" s="1"/>
     </row>
-    <row r="57" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B57" s="1"/>
       <c r="C57" s="1"/>
     </row>
-    <row r="58" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B58" s="1"/>
       <c r="C58" s="1"/>
     </row>
-    <row r="59" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B59" s="1"/>
       <c r="C59" s="1"/>
     </row>
-    <row r="60" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B60" s="1"/>
       <c r="C60" s="1"/>
     </row>
-    <row r="61" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B61" s="1"/>
       <c r="C61" s="1"/>
     </row>
-    <row r="62" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B62" s="1"/>
       <c r="C62" s="1"/>
     </row>
-    <row r="63" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B63" s="1"/>
       <c r="C63" s="1"/>
     </row>
-    <row r="64" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B64" s="1"/>
       <c r="C64" s="1"/>
     </row>
-    <row r="65" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B65" s="1"/>
       <c r="C65" s="1"/>
     </row>
-    <row r="66" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B66" s="1"/>
       <c r="C66" s="1"/>
     </row>
-    <row r="67" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B67" s="1"/>
       <c r="C67" s="1"/>
     </row>
-    <row r="68" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B68" s="1"/>
       <c r="C68" s="1"/>
     </row>
-    <row r="69" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B69" s="1"/>
       <c r="C69" s="1"/>
     </row>
-    <row r="70" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B70" s="1"/>
       <c r="C70" s="1"/>
     </row>
-    <row r="71" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B71" s="1"/>
       <c r="C71" s="1"/>
     </row>
-    <row r="72" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B72" s="1"/>
       <c r="C72" s="1"/>
     </row>
-    <row r="73" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="73" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B73" s="1"/>
       <c r="C73" s="1"/>
     </row>
-    <row r="74" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B74" s="1"/>
       <c r="C74" s="1"/>
     </row>
-    <row r="75" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="75" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B75" s="1"/>
       <c r="C75" s="1"/>
     </row>
-    <row r="76" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="76" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B76" s="1"/>
       <c r="C76" s="1"/>
     </row>
-    <row r="77" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="77" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B77" s="1"/>
       <c r="C77" s="1"/>
     </row>
-    <row r="78" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="78" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B78" s="1"/>
       <c r="C78" s="1"/>
     </row>
-    <row r="79" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="79" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B79" s="1"/>
       <c r="C79" s="1"/>
     </row>
-    <row r="80" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="80" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B80" s="1"/>
       <c r="C80" s="1"/>
     </row>
-    <row r="81" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="81" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B81" s="1"/>
       <c r="C81" s="1"/>
     </row>
-    <row r="82" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="82" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B82" s="1"/>
       <c r="C82" s="1"/>
     </row>
-    <row r="83" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="83" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B83" s="1"/>
       <c r="C83" s="1"/>
     </row>
-    <row r="84" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="84" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B84" s="1"/>
       <c r="C84" s="1"/>
     </row>
-    <row r="85" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="85" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B85" s="1"/>
       <c r="C85" s="1"/>
     </row>
-    <row r="86" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="86" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B86" s="1"/>
       <c r="C86" s="1"/>
     </row>
-    <row r="87" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="87" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B87" s="1"/>
       <c r="C87" s="1"/>
     </row>
-    <row r="88" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="88" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B88" s="1"/>
       <c r="C88" s="1"/>
     </row>
-    <row r="89" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="89" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B89" s="1"/>
       <c r="C89" s="1"/>
     </row>
-    <row r="90" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="90" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B90" s="1"/>
       <c r="C90" s="1"/>
     </row>
-    <row r="91" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="91" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B91" s="1"/>
       <c r="C91" s="1"/>
     </row>
-    <row r="92" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="92" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B92" s="1"/>
       <c r="C92" s="1"/>
     </row>
-    <row r="93" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="93" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B93" s="1"/>
       <c r="C93" s="1"/>
     </row>
-    <row r="94" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="94" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B94" s="1"/>
       <c r="C94" s="1"/>
     </row>
-    <row r="95" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="95" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B95" s="1"/>
       <c r="C95" s="1"/>
     </row>
-    <row r="96" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="96" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B96" s="1"/>
       <c r="C96" s="1"/>
     </row>
-    <row r="97" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="97" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B97" s="1"/>
       <c r="C97" s="1"/>
     </row>
-    <row r="98" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="98" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B98" s="1"/>
       <c r="C98" s="1"/>
     </row>
-    <row r="99" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="99" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B99" s="1"/>
       <c r="C99" s="1"/>
     </row>
-    <row r="100" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="100" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B100" s="1"/>
       <c r="C100" s="1"/>
     </row>
-    <row r="101" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="101" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B101" s="1"/>
       <c r="C101" s="1"/>
     </row>
-    <row r="102" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="102" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B102" s="1"/>
       <c r="C102" s="1"/>
     </row>
-    <row r="103" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="103" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B103" s="1"/>
       <c r="C103" s="1"/>
     </row>
-    <row r="104" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="104" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B104" s="1"/>
       <c r="C104" s="1"/>
     </row>
-    <row r="105" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="105" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B105" s="1"/>
       <c r="C105" s="1"/>
     </row>
-    <row r="106" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="106" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B106" s="1"/>
       <c r="C106" s="1"/>
     </row>
-    <row r="107" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="107" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B107" s="1"/>
       <c r="C107" s="1"/>
     </row>
-    <row r="108" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="108" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B108" s="1"/>
       <c r="C108" s="1"/>
     </row>
-    <row r="109" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="109" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B109" s="1"/>
       <c r="C109" s="1"/>
     </row>
-    <row r="110" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="110" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B110" s="1"/>
       <c r="C110" s="1"/>
     </row>
-    <row r="111" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="111" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B111" s="1"/>
       <c r="C111" s="1"/>
     </row>
-    <row r="112" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="112" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B112" s="1"/>
       <c r="C112" s="1"/>
     </row>
-    <row r="113" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="113" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B113" s="1"/>
       <c r="C113" s="1"/>
     </row>
-    <row r="114" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="114" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B114" s="1"/>
       <c r="C114" s="1"/>
     </row>
-    <row r="115" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="115" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B115" s="1"/>
       <c r="C115" s="1"/>
     </row>
-    <row r="116" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="116" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B116" s="1"/>
       <c r="C116" s="1"/>
     </row>
-    <row r="117" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="117" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B117" s="1"/>
       <c r="C117" s="1"/>
     </row>
-    <row r="118" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="118" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B118" s="1"/>
       <c r="C118" s="1"/>
     </row>
-    <row r="119" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="119" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B119" s="1"/>
       <c r="C119" s="1"/>
     </row>
-    <row r="120" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="120" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B120" s="1"/>
       <c r="C120" s="1"/>
     </row>
-    <row r="121" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="121" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B121" s="1"/>
       <c r="C121" s="1"/>
     </row>
@@ -4062,14 +4059,14 @@
       <selection activeCell="I1" sqref="I1:I1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="42.28515625" customWidth="1"/>
-    <col min="6" max="6" width="68.42578125" customWidth="1"/>
-    <col min="9" max="9" width="18.42578125" customWidth="1"/>
+    <col min="1" max="1" width="42.26953125" customWidth="1"/>
+    <col min="6" max="6" width="68.453125" customWidth="1"/>
+    <col min="9" max="9" width="18.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4098,7 +4095,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -4127,7 +4124,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -4157,7 +4154,7 @@
       </c>
       <c r="K3" s="1"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>17</v>
       </c>
@@ -4186,7 +4183,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -4215,455 +4212,455 @@
         <v>310</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
     </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
     </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
     </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
     </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
     </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
     </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
     </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
     </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
     </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
     </row>
-    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
     </row>
-    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
     </row>
-    <row r="29" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
     </row>
-    <row r="30" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
     </row>
-    <row r="31" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
     </row>
-    <row r="32" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
     </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
     </row>
-    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
     </row>
-    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
     </row>
-    <row r="36" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
     </row>
-    <row r="37" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
     </row>
-    <row r="38" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
     </row>
-    <row r="39" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
     </row>
-    <row r="40" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
     </row>
-    <row r="41" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
     </row>
-    <row r="42" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
     </row>
-    <row r="43" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
     </row>
-    <row r="44" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
     </row>
-    <row r="45" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
     </row>
-    <row r="46" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>
     </row>
-    <row r="47" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
     </row>
-    <row r="48" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B48" s="1"/>
       <c r="C48" s="1"/>
     </row>
-    <row r="49" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B49" s="1"/>
       <c r="C49" s="1"/>
     </row>
-    <row r="50" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B50" s="1"/>
       <c r="C50" s="1"/>
     </row>
-    <row r="51" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B51" s="1"/>
       <c r="C51" s="1"/>
     </row>
-    <row r="52" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B52" s="1"/>
       <c r="C52" s="1"/>
     </row>
-    <row r="53" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B53" s="1"/>
       <c r="C53" s="1"/>
     </row>
-    <row r="54" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B54" s="1"/>
       <c r="C54" s="1"/>
     </row>
-    <row r="55" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B55" s="1"/>
       <c r="C55" s="1"/>
     </row>
-    <row r="56" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B56" s="1"/>
       <c r="C56" s="1"/>
     </row>
-    <row r="57" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B57" s="1"/>
       <c r="C57" s="1"/>
     </row>
-    <row r="58" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B58" s="1"/>
       <c r="C58" s="1"/>
     </row>
-    <row r="59" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B59" s="1"/>
       <c r="C59" s="1"/>
     </row>
-    <row r="60" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B60" s="1"/>
       <c r="C60" s="1"/>
     </row>
-    <row r="61" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B61" s="1"/>
       <c r="C61" s="1"/>
     </row>
-    <row r="62" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B62" s="1"/>
       <c r="C62" s="1"/>
     </row>
-    <row r="63" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B63" s="1"/>
       <c r="C63" s="1"/>
     </row>
-    <row r="64" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B64" s="1"/>
       <c r="C64" s="1"/>
     </row>
-    <row r="65" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B65" s="1"/>
       <c r="C65" s="1"/>
     </row>
-    <row r="66" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B66" s="1"/>
       <c r="C66" s="1"/>
     </row>
-    <row r="67" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B67" s="1"/>
       <c r="C67" s="1"/>
     </row>
-    <row r="68" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B68" s="1"/>
       <c r="C68" s="1"/>
     </row>
-    <row r="69" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B69" s="1"/>
       <c r="C69" s="1"/>
     </row>
-    <row r="70" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B70" s="1"/>
       <c r="C70" s="1"/>
     </row>
-    <row r="71" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B71" s="1"/>
       <c r="C71" s="1"/>
     </row>
-    <row r="72" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B72" s="1"/>
       <c r="C72" s="1"/>
     </row>
-    <row r="73" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="73" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B73" s="1"/>
       <c r="C73" s="1"/>
     </row>
-    <row r="74" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B74" s="1"/>
       <c r="C74" s="1"/>
     </row>
-    <row r="75" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="75" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B75" s="1"/>
       <c r="C75" s="1"/>
     </row>
-    <row r="76" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="76" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B76" s="1"/>
       <c r="C76" s="1"/>
     </row>
-    <row r="77" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="77" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B77" s="1"/>
       <c r="C77" s="1"/>
     </row>
-    <row r="78" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="78" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B78" s="1"/>
       <c r="C78" s="1"/>
     </row>
-    <row r="79" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="79" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B79" s="1"/>
       <c r="C79" s="1"/>
     </row>
-    <row r="80" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="80" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B80" s="1"/>
       <c r="C80" s="1"/>
     </row>
-    <row r="81" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="81" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B81" s="1"/>
       <c r="C81" s="1"/>
     </row>
-    <row r="82" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="82" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B82" s="1"/>
       <c r="C82" s="1"/>
     </row>
-    <row r="83" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="83" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B83" s="1"/>
       <c r="C83" s="1"/>
     </row>
-    <row r="84" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="84" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B84" s="1"/>
       <c r="C84" s="1"/>
     </row>
-    <row r="85" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="85" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B85" s="1"/>
       <c r="C85" s="1"/>
     </row>
-    <row r="86" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="86" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B86" s="1"/>
       <c r="C86" s="1"/>
     </row>
-    <row r="87" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="87" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B87" s="1"/>
       <c r="C87" s="1"/>
     </row>
-    <row r="88" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="88" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B88" s="1"/>
       <c r="C88" s="1"/>
     </row>
-    <row r="89" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="89" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B89" s="1"/>
       <c r="C89" s="1"/>
     </row>
-    <row r="90" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="90" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B90" s="1"/>
       <c r="C90" s="1"/>
     </row>
-    <row r="91" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="91" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B91" s="1"/>
       <c r="C91" s="1"/>
     </row>
-    <row r="92" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="92" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B92" s="1"/>
       <c r="C92" s="1"/>
     </row>
-    <row r="93" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="93" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B93" s="1"/>
       <c r="C93" s="1"/>
     </row>
-    <row r="94" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="94" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B94" s="1"/>
       <c r="C94" s="1"/>
     </row>
-    <row r="95" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="95" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B95" s="1"/>
       <c r="C95" s="1"/>
     </row>
-    <row r="96" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="96" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B96" s="1"/>
       <c r="C96" s="1"/>
     </row>
-    <row r="97" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="97" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B97" s="1"/>
       <c r="C97" s="1"/>
     </row>
-    <row r="98" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="98" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B98" s="1"/>
       <c r="C98" s="1"/>
     </row>
-    <row r="99" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="99" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B99" s="1"/>
       <c r="C99" s="1"/>
     </row>
-    <row r="100" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="100" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B100" s="1"/>
       <c r="C100" s="1"/>
     </row>
-    <row r="101" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="101" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B101" s="1"/>
       <c r="C101" s="1"/>
     </row>
-    <row r="102" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="102" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B102" s="1"/>
       <c r="C102" s="1"/>
     </row>
-    <row r="103" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="103" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B103" s="1"/>
       <c r="C103" s="1"/>
     </row>
-    <row r="104" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="104" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B104" s="1"/>
       <c r="C104" s="1"/>
     </row>
-    <row r="105" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="105" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B105" s="1"/>
       <c r="C105" s="1"/>
     </row>
-    <row r="106" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="106" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B106" s="1"/>
       <c r="C106" s="1"/>
     </row>
-    <row r="107" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="107" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B107" s="1"/>
       <c r="C107" s="1"/>
     </row>
-    <row r="108" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="108" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B108" s="1"/>
       <c r="C108" s="1"/>
     </row>
-    <row r="109" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="109" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B109" s="1"/>
       <c r="C109" s="1"/>
     </row>
-    <row r="110" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="110" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B110" s="1"/>
       <c r="C110" s="1"/>
     </row>
-    <row r="111" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="111" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B111" s="1"/>
       <c r="C111" s="1"/>
     </row>
-    <row r="112" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="112" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B112" s="1"/>
       <c r="C112" s="1"/>
     </row>
-    <row r="113" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="113" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B113" s="1"/>
       <c r="C113" s="1"/>
     </row>
-    <row r="114" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="114" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B114" s="1"/>
       <c r="C114" s="1"/>
     </row>
-    <row r="115" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="115" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B115" s="1"/>
       <c r="C115" s="1"/>
     </row>
-    <row r="116" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="116" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B116" s="1"/>
       <c r="C116" s="1"/>
     </row>
-    <row r="117" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="117" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B117" s="1"/>
       <c r="C117" s="1"/>
     </row>
-    <row r="118" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="118" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B118" s="1"/>
       <c r="C118" s="1"/>
     </row>
@@ -4680,16 +4677,16 @@
       <selection activeCell="I1" sqref="I1:I1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="32.5703125" customWidth="1"/>
-    <col min="2" max="2" width="14.140625" customWidth="1"/>
-    <col min="3" max="3" width="10.85546875" customWidth="1"/>
-    <col min="6" max="6" width="128.85546875" customWidth="1"/>
-    <col min="9" max="9" width="18.42578125" customWidth="1"/>
+    <col min="1" max="1" width="32.54296875" customWidth="1"/>
+    <col min="2" max="2" width="14.08984375" customWidth="1"/>
+    <col min="3" max="3" width="10.81640625" customWidth="1"/>
+    <col min="6" max="6" width="128.90625" customWidth="1"/>
+    <col min="9" max="9" width="18.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4718,7 +4715,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>19</v>
       </c>
@@ -4747,7 +4744,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -4776,7 +4773,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>21</v>
       </c>
@@ -4818,17 +4815,17 @@
       <selection activeCell="I1" sqref="I1:I1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="47.42578125" customWidth="1"/>
-    <col min="2" max="2" width="11.5703125" customWidth="1"/>
-    <col min="3" max="3" width="12.28515625" customWidth="1"/>
-    <col min="4" max="4" width="12.140625" customWidth="1"/>
-    <col min="6" max="6" width="63.7109375" customWidth="1"/>
-    <col min="9" max="9" width="18.42578125" customWidth="1"/>
+    <col min="1" max="1" width="47.36328125" customWidth="1"/>
+    <col min="2" max="2" width="11.6328125" customWidth="1"/>
+    <col min="3" max="3" width="12.26953125" customWidth="1"/>
+    <col min="4" max="4" width="12.1796875" customWidth="1"/>
+    <col min="6" max="6" width="63.7265625" customWidth="1"/>
+    <col min="9" max="9" width="18.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4857,7 +4854,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>22</v>
       </c>
@@ -4886,7 +4883,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>63</v>
       </c>
@@ -4915,7 +4912,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>65</v>
       </c>
@@ -4944,7 +4941,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>67</v>
       </c>
@@ -4973,7 +4970,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>69</v>
       </c>
@@ -5002,7 +4999,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>71</v>
       </c>
@@ -5031,7 +5028,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>73</v>
       </c>
@@ -5060,7 +5057,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>75</v>
       </c>
@@ -5089,7 +5086,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>36</v>
       </c>
@@ -5118,7 +5115,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>23</v>
       </c>
@@ -5147,7 +5144,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>26</v>
       </c>
@@ -5176,7 +5173,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>27</v>
       </c>
@@ -5205,7 +5202,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>29</v>
       </c>
@@ -5234,7 +5231,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>31</v>
       </c>
@@ -5263,7 +5260,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>32</v>
       </c>
@@ -5292,7 +5289,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>33</v>
       </c>
@@ -5321,7 +5318,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>34</v>
       </c>
@@ -5350,7 +5347,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>35</v>
       </c>
@@ -5379,7 +5376,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>98</v>
       </c>
@@ -5408,7 +5405,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>100</v>
       </c>
@@ -5437,7 +5434,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>101</v>
       </c>
@@ -5466,7 +5463,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>102</v>
       </c>
@@ -5495,7 +5492,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>103</v>
       </c>
@@ -5524,7 +5521,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>134</v>
       </c>
@@ -5553,7 +5550,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>143</v>
       </c>
@@ -5582,7 +5579,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
     </row>
@@ -5599,15 +5596,15 @@
       <selection activeCell="I1" sqref="I1:I1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="23.42578125" customWidth="1"/>
-    <col min="2" max="3" width="12.5703125" customWidth="1"/>
+    <col min="1" max="1" width="23.36328125" customWidth="1"/>
+    <col min="2" max="3" width="12.54296875" customWidth="1"/>
     <col min="6" max="6" width="87" customWidth="1"/>
-    <col min="9" max="9" width="18.42578125" customWidth="1"/>
+    <col min="9" max="9" width="18.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -5636,7 +5633,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>64</v>
       </c>
@@ -5665,7 +5662,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>42</v>
       </c>
@@ -5694,7 +5691,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>43</v>
       </c>
@@ -5723,7 +5720,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>66</v>
       </c>
@@ -5752,7 +5749,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>44</v>
       </c>
@@ -5781,7 +5778,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>45</v>
       </c>
@@ -5810,7 +5807,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>68</v>
       </c>
@@ -5839,7 +5836,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>46</v>
       </c>
@@ -5868,7 +5865,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>47</v>
       </c>
@@ -5897,7 +5894,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>70</v>
       </c>
@@ -5926,7 +5923,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>48</v>
       </c>
@@ -5955,7 +5952,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>49</v>
       </c>
@@ -5984,7 +5981,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>72</v>
       </c>
@@ -6013,7 +6010,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>50</v>
       </c>
@@ -6042,7 +6039,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>51</v>
       </c>
@@ -6071,7 +6068,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>74</v>
       </c>
@@ -6100,7 +6097,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>52</v>
       </c>
@@ -6129,7 +6126,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>53</v>
       </c>
@@ -6158,7 +6155,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>62</v>
       </c>
@@ -6187,7 +6184,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>40</v>
       </c>
@@ -6216,7 +6213,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>41</v>
       </c>
@@ -6258,15 +6255,15 @@
       <selection activeCell="I1" sqref="I1:I1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="25.140625" customWidth="1"/>
-    <col min="3" max="4" width="12.42578125" customWidth="1"/>
-    <col min="6" max="6" width="107.42578125" customWidth="1"/>
-    <col min="9" max="9" width="18.42578125" customWidth="1"/>
+    <col min="1" max="1" width="25.1796875" customWidth="1"/>
+    <col min="3" max="4" width="12.453125" customWidth="1"/>
+    <col min="6" max="6" width="107.453125" customWidth="1"/>
+    <col min="9" max="9" width="18.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -6295,7 +6292,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>76</v>
       </c>
@@ -6324,7 +6321,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>78</v>
       </c>
@@ -6353,7 +6350,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>80</v>
       </c>
@@ -6382,7 +6379,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>81</v>
       </c>
@@ -6411,7 +6408,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>82</v>
       </c>
@@ -6440,7 +6437,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>83</v>
       </c>
@@ -6469,7 +6466,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>84</v>
       </c>
@@ -6498,7 +6495,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>97</v>
       </c>
@@ -6527,7 +6524,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>85</v>
       </c>
@@ -6556,7 +6553,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>87</v>
       </c>
@@ -6585,7 +6582,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>88</v>
       </c>
@@ -6614,7 +6611,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>89</v>
       </c>
@@ -6643,7 +6640,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>90</v>
       </c>
@@ -6672,7 +6669,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>92</v>
       </c>
@@ -6701,7 +6698,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>153</v>
       </c>
@@ -6730,7 +6727,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>154</v>
       </c>
@@ -6759,7 +6756,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>93</v>
       </c>
@@ -6788,7 +6785,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>96</v>
       </c>
@@ -6817,7 +6814,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>95</v>
       </c>
@@ -6846,7 +6843,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>94</v>
       </c>
@@ -6875,7 +6872,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>152</v>
       </c>
@@ -6904,7 +6901,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>151</v>
       </c>
@@ -6946,15 +6943,15 @@
       <selection activeCell="I1" sqref="I1:I1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="39.85546875" customWidth="1"/>
-    <col min="4" max="4" width="12.28515625" customWidth="1"/>
-    <col min="6" max="6" width="156.7109375" customWidth="1"/>
-    <col min="9" max="9" width="18.42578125" customWidth="1"/>
+    <col min="1" max="1" width="39.81640625" customWidth="1"/>
+    <col min="4" max="4" width="12.26953125" customWidth="1"/>
+    <col min="6" max="6" width="156.7265625" customWidth="1"/>
+    <col min="9" max="9" width="18.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -6983,7 +6980,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>141</v>
       </c>
@@ -7012,7 +7009,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>142</v>
       </c>
@@ -7041,7 +7038,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>124</v>
       </c>
@@ -7070,7 +7067,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>125</v>
       </c>
@@ -7099,7 +7096,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>126</v>
       </c>
@@ -7128,7 +7125,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>127</v>
       </c>
@@ -7157,7 +7154,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>128</v>
       </c>
@@ -7186,7 +7183,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>146</v>
       </c>
@@ -7215,7 +7212,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>129</v>
       </c>
@@ -7244,7 +7241,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>145</v>
       </c>
@@ -7273,7 +7270,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>144</v>
       </c>
@@ -7302,7 +7299,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>130</v>
       </c>
@@ -7331,7 +7328,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>131</v>
       </c>
@@ -7360,7 +7357,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>132</v>
       </c>
@@ -7389,7 +7386,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>133</v>
       </c>
@@ -7431,16 +7428,16 @@
       <selection activeCell="I1" sqref="I1:I1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="21.28515625" customWidth="1"/>
-    <col min="2" max="2" width="10.5703125" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" customWidth="1"/>
-    <col min="6" max="6" width="47.85546875" customWidth="1"/>
-    <col min="9" max="9" width="18.42578125" customWidth="1"/>
+    <col min="1" max="1" width="21.26953125" customWidth="1"/>
+    <col min="2" max="2" width="10.54296875" customWidth="1"/>
+    <col min="3" max="3" width="11.6328125" customWidth="1"/>
+    <col min="6" max="6" width="47.90625" customWidth="1"/>
+    <col min="9" max="9" width="18.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -7469,7 +7466,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>25</v>
       </c>

</xml_diff>

<commit_message>
added relevant render conditions to html elements in xlsx file
</commit_message>
<xml_diff>
--- a/data/Walnut_grain_veg_tub.xlsx
+++ b/data/Walnut_grain_veg_tub.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\belgium_app\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1967C82-C3E8-44B6-BF04-B52F2A7643EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C09B67C2-9E27-4774-9AF6-DEC59D8B7174}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="3" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="3" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sheet_names" sheetId="17" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="901" uniqueCount="323">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="931" uniqueCount="323">
   <si>
     <t>variable</t>
   </si>
@@ -2104,8 +2104,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{724F1830-3430-4657-920D-E95506196AA8}">
   <dimension ref="A1:I29"/>
   <sheetViews>
-    <sheetView topLeftCell="F7" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2179,6 +2179,9 @@
       <c r="G3" t="s">
         <v>322</v>
       </c>
+      <c r="I3" t="s">
+        <v>308</v>
+      </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B4" s="1"/>
@@ -2189,6 +2192,9 @@
       <c r="G4" t="s">
         <v>315</v>
       </c>
+      <c r="I4" t="s">
+        <v>308</v>
+      </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B5" s="1"/>
@@ -2196,6 +2202,9 @@
       <c r="G5" t="s">
         <v>316</v>
       </c>
+      <c r="I5" t="s">
+        <v>308</v>
+      </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -2290,6 +2299,9 @@
       <c r="G9" t="s">
         <v>316</v>
       </c>
+      <c r="I9" t="s">
+        <v>308</v>
+      </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B10" s="1"/>
@@ -2297,6 +2309,9 @@
       <c r="G10" t="s">
         <v>322</v>
       </c>
+      <c r="I10" t="s">
+        <v>308</v>
+      </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
@@ -2362,6 +2377,9 @@
       <c r="G13" t="s">
         <v>322</v>
       </c>
+      <c r="I13" t="s">
+        <v>312</v>
+      </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B14" s="1"/>
@@ -2372,6 +2390,9 @@
       <c r="G14" t="s">
         <v>315</v>
       </c>
+      <c r="I14" t="s">
+        <v>312</v>
+      </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B15" s="1"/>
@@ -2379,6 +2400,9 @@
       <c r="G15" t="s">
         <v>316</v>
       </c>
+      <c r="I15" t="s">
+        <v>312</v>
+      </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
@@ -2560,12 +2584,18 @@
       <c r="G22" t="s">
         <v>316</v>
       </c>
+      <c r="I22" t="s">
+        <v>312</v>
+      </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
       <c r="G23" t="s">
         <v>322</v>
+      </c>
+      <c r="I23" t="s">
+        <v>312</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
@@ -6354,8 +6384,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5B46F03-BBFE-4EF0-AFCA-0F4C3592A7D1}">
   <dimension ref="A1:I33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6401,6 +6431,9 @@
       <c r="G2" t="s">
         <v>322</v>
       </c>
+      <c r="I2" t="s">
+        <v>308</v>
+      </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
@@ -6411,6 +6444,9 @@
       <c r="G3" t="s">
         <v>315</v>
       </c>
+      <c r="I3" t="s">
+        <v>308</v>
+      </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B4" s="1"/>
@@ -6418,6 +6454,9 @@
       <c r="G4" t="s">
         <v>316</v>
       </c>
+      <c r="I4" t="s">
+        <v>308</v>
+      </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -6570,6 +6609,9 @@
       <c r="G10" t="s">
         <v>316</v>
       </c>
+      <c r="I10" t="s">
+        <v>308</v>
+      </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B11" s="1"/>
@@ -6577,6 +6619,9 @@
       <c r="G11" t="s">
         <v>322</v>
       </c>
+      <c r="I11" t="s">
+        <v>308</v>
+      </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
@@ -6671,6 +6716,9 @@
       <c r="G15" t="s">
         <v>322</v>
       </c>
+      <c r="I15" t="s">
+        <v>309</v>
+      </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B16" s="1"/>
@@ -6681,6 +6729,9 @@
       <c r="G16" t="s">
         <v>315</v>
       </c>
+      <c r="I16" t="s">
+        <v>309</v>
+      </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B17" s="1"/>
@@ -6688,6 +6739,9 @@
       <c r="G17" t="s">
         <v>316</v>
       </c>
+      <c r="I17" t="s">
+        <v>309</v>
+      </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
@@ -6869,12 +6923,18 @@
       <c r="G24" t="s">
         <v>316</v>
       </c>
+      <c r="I24" t="s">
+        <v>309</v>
+      </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
       <c r="G25" t="s">
         <v>322</v>
+      </c>
+      <c r="I25" t="s">
+        <v>309</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
@@ -7118,8 +7178,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7AD55CD1-0195-43C4-85D0-979B3B5F4C61}">
   <dimension ref="A1:I26"/>
   <sheetViews>
-    <sheetView topLeftCell="F6" workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6:I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7223,6 +7283,9 @@
       <c r="G4" t="s">
         <v>322</v>
       </c>
+      <c r="I4" t="s">
+        <v>307</v>
+      </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B5" s="1"/>
@@ -7233,6 +7296,9 @@
       <c r="G5" t="s">
         <v>315</v>
       </c>
+      <c r="I5" t="s">
+        <v>307</v>
+      </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B6" s="1"/>
@@ -7240,6 +7306,9 @@
       <c r="G6" t="s">
         <v>316</v>
       </c>
+      <c r="I6" t="s">
+        <v>307</v>
+      </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -7392,6 +7461,9 @@
       <c r="G12" t="s">
         <v>316</v>
       </c>
+      <c r="I12" t="s">
+        <v>307</v>
+      </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B13" s="1"/>
@@ -7399,6 +7471,9 @@
       <c r="G13" t="s">
         <v>322</v>
       </c>
+      <c r="I13" t="s">
+        <v>307</v>
+      </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
@@ -7493,6 +7568,9 @@
       <c r="G17" t="s">
         <v>322</v>
       </c>
+      <c r="I17" t="s">
+        <v>307</v>
+      </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B18" s="1"/>
@@ -7503,6 +7581,9 @@
       <c r="G18" t="s">
         <v>315</v>
       </c>
+      <c r="I18" t="s">
+        <v>307</v>
+      </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B19" s="1"/>
@@ -7510,6 +7591,9 @@
       <c r="G19" t="s">
         <v>316</v>
       </c>
+      <c r="I19" t="s">
+        <v>307</v>
+      </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
@@ -7660,10 +7744,16 @@
       <c r="G25" t="s">
         <v>316</v>
       </c>
+      <c r="I25" t="s">
+        <v>307</v>
+      </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="G26" t="s">
         <v>322</v>
+      </c>
+      <c r="I26" t="s">
+        <v>307</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changed how the dynamic ui is built - now the whole accordion panel gets build by a helper and can be hidden if no element in it is visible (checkbox filter at the top)
</commit_message>
<xml_diff>
--- a/data/Walnut_grain_veg_tub.xlsx
+++ b/data/Walnut_grain_veg_tub.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\belgium_app\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C09B67C2-9E27-4774-9AF6-DEC59D8B7174}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A1EFF3C-A2EA-40D1-AE25-9046D3C4AAB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="3" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sheet_names" sheetId="17" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="931" uniqueCount="323">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="944" uniqueCount="336">
   <si>
     <t>variable</t>
   </si>
@@ -1001,6 +1001,45 @@
   </si>
   <si>
     <t>break</t>
+  </si>
+  <si>
+    <t>icon</t>
+  </si>
+  <si>
+    <t>bullseye</t>
+  </si>
+  <si>
+    <t>grip</t>
+  </si>
+  <si>
+    <t>cart-shopping</t>
+  </si>
+  <si>
+    <t>people-group</t>
+  </si>
+  <si>
+    <t>seedling</t>
+  </si>
+  <si>
+    <t>tree</t>
+  </si>
+  <si>
+    <t>route</t>
+  </si>
+  <si>
+    <t>person-chalkboard</t>
+  </si>
+  <si>
+    <t>check-double</t>
+  </si>
+  <si>
+    <t>atom</t>
+  </si>
+  <si>
+    <t>square-poll-vertical</t>
+  </si>
+  <si>
+    <t>water</t>
   </si>
 </sst>
 </file>
@@ -1851,10 +1890,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6B894F3-1BBC-4877-818A-ECEC60560258}">
-  <dimension ref="A1:A13"/>
+  <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1862,69 +1901,108 @@
     <col min="1" max="1" width="37.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>162</v>
+      </c>
+      <c r="B13" t="s">
+        <v>335</v>
       </c>
     </row>
   </sheetData>
@@ -2104,8 +2182,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{724F1830-3430-4657-920D-E95506196AA8}">
   <dimension ref="A1:I29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="J21" sqref="J21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
added multiple categories in expertise column.
</commit_message>
<xml_diff>
--- a/data/Walnut_grain_veg_tub.xlsx
+++ b/data/Walnut_grain_veg_tub.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\belgium_app\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A1EFF3C-A2EA-40D1-AE25-9046D3C4AAB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFF53BD4-D5AF-4AE1-9595-9DD5608C8F4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1905" yWindow="1905" windowWidth="21600" windowHeight="11295" firstSheet="8" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sheet_names" sheetId="17" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="944" uniqueCount="336">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="944" uniqueCount="346">
   <si>
     <t>variable</t>
   </si>
@@ -961,9 +961,6 @@
     <t>Silviculture</t>
   </si>
   <si>
-    <t>Fruit/Nuts production</t>
-  </si>
-  <si>
     <t>Decision maker</t>
   </si>
   <si>
@@ -973,9 +970,6 @@
     <t>Soil science</t>
   </si>
   <si>
-    <t>Market analysis</t>
-  </si>
-  <si>
     <t>Tree growth model</t>
   </si>
   <si>
@@ -1040,6 +1034,42 @@
   </si>
   <si>
     <t>water</t>
+  </si>
+  <si>
+    <t>Agroforestry farming;Silviculture</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Agroforestry farming;Policy analysis </t>
+  </si>
+  <si>
+    <t>Agroforestry farming;Fruit/Nuts production</t>
+  </si>
+  <si>
+    <t>Market analysis;Treeless farming</t>
+  </si>
+  <si>
+    <t>Silviculture;Agroforestry farming</t>
+  </si>
+  <si>
+    <t>Fruit/Nuts production;Agroforestry farming</t>
+  </si>
+  <si>
+    <t>Fruit/Nuts production;Agroforestry farming;Data analyst</t>
+  </si>
+  <si>
+    <t>Fruits/Nuts production;Market analysis;Agroforestry farming</t>
+  </si>
+  <si>
+    <t>Silviculture;Market analysis;Agroforestry farming</t>
+  </si>
+  <si>
+    <t>Policy analysis;Agroforestry farming</t>
+  </si>
+  <si>
+    <t>Market analysis;Policy analysis</t>
+  </si>
+  <si>
+    <t>Soil science;Policy analysis ;Data analyst</t>
   </si>
 </sst>
 </file>
@@ -1893,7 +1923,7 @@
   <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="B1" sqref="B1:B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1906,7 +1936,7 @@
         <v>158</v>
       </c>
       <c r="B1" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -1914,7 +1944,7 @@
         <v>159</v>
       </c>
       <c r="B2" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -1922,7 +1952,7 @@
         <v>163</v>
       </c>
       <c r="B3" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -1930,7 +1960,7 @@
         <v>164</v>
       </c>
       <c r="B4" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -1938,7 +1968,7 @@
         <v>160</v>
       </c>
       <c r="B5" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -1946,7 +1976,7 @@
         <v>167</v>
       </c>
       <c r="B6" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -1954,7 +1984,7 @@
         <v>165</v>
       </c>
       <c r="B7" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -1962,7 +1992,7 @@
         <v>166</v>
       </c>
       <c r="B8" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -1970,7 +2000,7 @@
         <v>168</v>
       </c>
       <c r="B9" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -1978,7 +2008,7 @@
         <v>169</v>
       </c>
       <c r="B10" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -1986,7 +2016,7 @@
         <v>161</v>
       </c>
       <c r="B11" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -1994,7 +2024,7 @@
         <v>170</v>
       </c>
       <c r="B12" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -2002,7 +2032,7 @@
         <v>162</v>
       </c>
       <c r="B13" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
     </row>
   </sheetData>
@@ -2015,8 +2045,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E807E7F-DCAE-400C-B9F4-3C0EDF692711}">
   <dimension ref="A1:I5"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1:I1048576"/>
+    <sheetView topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2:I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2083,7 +2113,7 @@
         <v>1</v>
       </c>
       <c r="I2" t="s">
-        <v>307</v>
+        <v>343</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -2112,7 +2142,7 @@
         <v>1</v>
       </c>
       <c r="I3" t="s">
-        <v>307</v>
+        <v>343</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -2141,7 +2171,7 @@
         <v>1E-3</v>
       </c>
       <c r="I4" t="s">
-        <v>307</v>
+        <v>343</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -2170,7 +2200,7 @@
         <v>1</v>
       </c>
       <c r="I5" t="s">
-        <v>307</v>
+        <v>343</v>
       </c>
     </row>
   </sheetData>
@@ -2182,8 +2212,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{724F1830-3430-4657-920D-E95506196AA8}">
   <dimension ref="A1:I29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2255,33 +2285,33 @@
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="G3" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="I3" t="s">
-        <v>308</v>
+        <v>338</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="F4" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="G4" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="I4" t="s">
-        <v>308</v>
+        <v>338</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
       <c r="G5" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="I5" t="s">
-        <v>308</v>
+        <v>338</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -2310,7 +2340,7 @@
         <v>1E-3</v>
       </c>
       <c r="I6" t="s">
-        <v>308</v>
+        <v>338</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -2339,7 +2369,7 @@
         <v>0.01</v>
       </c>
       <c r="I7" t="s">
-        <v>308</v>
+        <v>338</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -2368,27 +2398,27 @@
         <v>1</v>
       </c>
       <c r="I8" t="s">
-        <v>308</v>
+        <v>338</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="G9" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="I9" t="s">
-        <v>308</v>
+        <v>338</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="G10" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="I10" t="s">
-        <v>308</v>
+        <v>338</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -2417,7 +2447,7 @@
         <v>1</v>
       </c>
       <c r="I11" t="s">
-        <v>308</v>
+        <v>338</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -2453,33 +2483,33 @@
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="G13" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="I13" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="F14" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="G14" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="I14" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
       <c r="G15" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="I15" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
@@ -2508,7 +2538,7 @@
         <v>1</v>
       </c>
       <c r="I16" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
@@ -2537,7 +2567,7 @@
         <v>1</v>
       </c>
       <c r="I17" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
@@ -2566,7 +2596,7 @@
         <v>1E-3</v>
       </c>
       <c r="I18" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
@@ -2595,7 +2625,7 @@
         <v>1E-4</v>
       </c>
       <c r="I19" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
@@ -2624,7 +2654,7 @@
         <v>1</v>
       </c>
       <c r="I20" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
@@ -2653,27 +2683,27 @@
         <v>1</v>
       </c>
       <c r="I21" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
       <c r="G22" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="I22" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
       <c r="G23" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="I23" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
@@ -2702,7 +2732,7 @@
         <v>1</v>
       </c>
       <c r="I24" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
@@ -2731,7 +2761,7 @@
         <v>0.01</v>
       </c>
       <c r="I25" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
@@ -2760,7 +2790,7 @@
         <v>0.01</v>
       </c>
       <c r="I26" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
@@ -2789,7 +2819,7 @@
         <v>1E-3</v>
       </c>
       <c r="I27" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
@@ -2818,7 +2848,7 @@
         <v>0.01</v>
       </c>
       <c r="I28" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
@@ -2847,7 +2877,7 @@
         <v>1E-3</v>
       </c>
       <c r="I29" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
   </sheetData>
@@ -2859,8 +2889,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2682F285-7B44-4D8F-A7EA-4445FB570320}">
   <dimension ref="A1:I122"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I1" sqref="I1:I1048576"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2925,7 +2955,7 @@
         <v>1</v>
       </c>
       <c r="I2" t="s">
-        <v>313</v>
+        <v>344</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -3417,8 +3447,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0AACA546-DF26-443B-AA33-3E83721C2724}">
   <dimension ref="A1:I5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I1" sqref="I1:I1048576"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="O10" sqref="O10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3428,7 +3458,7 @@
     <col min="3" max="3" width="8.7109375" customWidth="1"/>
     <col min="6" max="6" width="59.42578125" customWidth="1"/>
     <col min="7" max="7" width="33.5703125" customWidth="1"/>
-    <col min="9" max="9" width="10.85546875" customWidth="1"/>
+    <col min="9" max="9" width="37" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -3486,7 +3516,7 @@
         <v>0.01</v>
       </c>
       <c r="I2" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -3515,7 +3545,7 @@
         <v>1E-3</v>
       </c>
       <c r="I3" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -3544,7 +3574,7 @@
         <v>1</v>
       </c>
       <c r="I4" t="s">
-        <v>312</v>
+        <v>345</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -3573,7 +3603,7 @@
         <v>1</v>
       </c>
       <c r="I5" t="s">
-        <v>312</v>
+        <v>345</v>
       </c>
     </row>
   </sheetData>
@@ -3586,8 +3616,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06826C72-96B8-4DB0-B8A1-5FBF5F35F3F2}">
   <dimension ref="A1:I121"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1:I1048576"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3653,7 +3683,7 @@
         <v>1</v>
       </c>
       <c r="I2" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -3682,7 +3712,7 @@
         <v>1</v>
       </c>
       <c r="I3" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -3769,7 +3799,7 @@
         <v>1</v>
       </c>
       <c r="I6" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -3798,7 +3828,7 @@
         <v>1</v>
       </c>
       <c r="I7" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -4266,8 +4296,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B046A6C-AF4B-434A-AE31-2F62785AB96F}">
   <dimension ref="A1:K118"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1:I1048576"/>
+    <sheetView topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4332,7 +4362,7 @@
         <v>0.01</v>
       </c>
       <c r="I2" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -4361,7 +4391,7 @@
         <v>1E-4</v>
       </c>
       <c r="I3" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="K3" s="1"/>
     </row>
@@ -4391,7 +4421,7 @@
         <v>1</v>
       </c>
       <c r="I4" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -4420,7 +4450,7 @@
         <v>1E-3</v>
       </c>
       <c r="I5" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -4884,8 +4914,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FF733DD-E084-451A-AEBD-87D8A1F2D1F6}">
   <dimension ref="A1:I4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I1" sqref="I1:I1048576"/>
+    <sheetView topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2:I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4952,7 +4982,7 @@
         <v>1</v>
       </c>
       <c r="I2" t="s">
-        <v>307</v>
+        <v>334</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -4981,7 +5011,7 @@
         <v>1</v>
       </c>
       <c r="I3" t="s">
-        <v>307</v>
+        <v>334</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -5010,7 +5040,7 @@
         <v>1</v>
       </c>
       <c r="I4" t="s">
-        <v>307</v>
+        <v>334</v>
       </c>
     </row>
   </sheetData>
@@ -5022,8 +5052,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8D4214A-8AE9-4396-ABE5-C95E3D310602}">
   <dimension ref="A1:I27"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1:I1048576"/>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2:I26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5352,7 +5382,7 @@
         <v>1</v>
       </c>
       <c r="I11" t="s">
-        <v>307</v>
+        <v>335</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -5381,7 +5411,7 @@
         <v>1</v>
       </c>
       <c r="I12" t="s">
-        <v>307</v>
+        <v>335</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -5613,7 +5643,7 @@
         <v>1E-3</v>
       </c>
       <c r="I20" t="s">
-        <v>308</v>
+        <v>334</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
@@ -5642,7 +5672,7 @@
         <v>1E-4</v>
       </c>
       <c r="I21" t="s">
-        <v>308</v>
+        <v>334</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
@@ -5671,7 +5701,7 @@
         <v>0.01</v>
       </c>
       <c r="I22" t="s">
-        <v>308</v>
+        <v>334</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
@@ -5700,7 +5730,7 @@
         <v>1</v>
       </c>
       <c r="I23" t="s">
-        <v>309</v>
+        <v>336</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
@@ -5729,7 +5759,7 @@
         <v>1</v>
       </c>
       <c r="I24" t="s">
-        <v>309</v>
+        <v>336</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
@@ -5758,7 +5788,7 @@
         <v>1</v>
       </c>
       <c r="I25" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
@@ -5787,7 +5817,7 @@
         <v>1E-3</v>
       </c>
       <c r="I26" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
@@ -5803,8 +5833,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C0D7C64-12CB-4A85-A4CD-D098869794C1}">
   <dimension ref="A1:I22"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1:I1048576"/>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2:I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5928,7 +5958,7 @@
         <v>1</v>
       </c>
       <c r="I4" t="s">
-        <v>306</v>
+        <v>337</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -6015,7 +6045,7 @@
         <v>1</v>
       </c>
       <c r="I7" t="s">
-        <v>306</v>
+        <v>337</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -6102,7 +6132,7 @@
         <v>1</v>
       </c>
       <c r="I10" t="s">
-        <v>306</v>
+        <v>337</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -6189,7 +6219,7 @@
         <v>1</v>
       </c>
       <c r="I13" t="s">
-        <v>306</v>
+        <v>337</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -6276,7 +6306,7 @@
         <v>1</v>
       </c>
       <c r="I16" t="s">
-        <v>306</v>
+        <v>337</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
@@ -6363,7 +6393,7 @@
         <v>1</v>
       </c>
       <c r="I19" t="s">
-        <v>306</v>
+        <v>337</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
@@ -6450,7 +6480,7 @@
         <v>1</v>
       </c>
       <c r="I22" t="s">
-        <v>306</v>
+        <v>337</v>
       </c>
     </row>
   </sheetData>
@@ -6462,7 +6492,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5B46F03-BBFE-4EF0-AFCA-0F4C3592A7D1}">
   <dimension ref="A1:I33"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="G1" workbookViewId="0">
       <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
@@ -6507,33 +6537,33 @@
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
       <c r="G2" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="I2" t="s">
-        <v>308</v>
+        <v>338</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="F3" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="G3" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="I3" t="s">
-        <v>308</v>
+        <v>338</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="G4" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="I4" t="s">
-        <v>308</v>
+        <v>338</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -6562,7 +6592,7 @@
         <v>1</v>
       </c>
       <c r="I5" t="s">
-        <v>308</v>
+        <v>338</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -6591,7 +6621,7 @@
         <v>1</v>
       </c>
       <c r="I6" t="s">
-        <v>308</v>
+        <v>338</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -6620,7 +6650,7 @@
         <v>1</v>
       </c>
       <c r="I7" t="s">
-        <v>308</v>
+        <v>338</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -6649,7 +6679,7 @@
         <v>1</v>
       </c>
       <c r="I8" t="s">
-        <v>308</v>
+        <v>338</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -6678,27 +6708,27 @@
         <v>1</v>
       </c>
       <c r="I9" t="s">
-        <v>308</v>
+        <v>338</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="G10" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="I10" t="s">
-        <v>308</v>
+        <v>338</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="G11" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="I11" t="s">
-        <v>308</v>
+        <v>338</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -6727,7 +6757,7 @@
         <v>1</v>
       </c>
       <c r="I12" t="s">
-        <v>307</v>
+        <v>338</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -6756,7 +6786,7 @@
         <v>1</v>
       </c>
       <c r="I13" t="s">
-        <v>308</v>
+        <v>338</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -6785,40 +6815,40 @@
         <v>1E-3</v>
       </c>
       <c r="I14" t="s">
-        <v>307</v>
+        <v>338</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
       <c r="G15" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="I15" t="s">
-        <v>309</v>
+        <v>340</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
       <c r="F16" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="G16" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="I16" t="s">
-        <v>309</v>
+        <v>340</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
       <c r="G17" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="I17" t="s">
-        <v>309</v>
+        <v>340</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
@@ -6847,7 +6877,7 @@
         <v>1</v>
       </c>
       <c r="I18" t="s">
-        <v>309</v>
+        <v>339</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
@@ -6876,7 +6906,7 @@
         <v>1</v>
       </c>
       <c r="I19" t="s">
-        <v>309</v>
+        <v>339</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
@@ -6905,7 +6935,7 @@
         <v>1</v>
       </c>
       <c r="I20" t="s">
-        <v>309</v>
+        <v>339</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
@@ -6934,7 +6964,7 @@
         <v>1</v>
       </c>
       <c r="I21" t="s">
-        <v>309</v>
+        <v>339</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
@@ -6963,7 +6993,7 @@
         <v>1</v>
       </c>
       <c r="I22" t="s">
-        <v>309</v>
+        <v>339</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
@@ -6992,27 +7022,27 @@
         <v>1</v>
       </c>
       <c r="I23" t="s">
-        <v>309</v>
+        <v>340</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
       <c r="G24" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="I24" t="s">
-        <v>309</v>
+        <v>340</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
       <c r="G25" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="I25" t="s">
-        <v>309</v>
+        <v>340</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
@@ -7041,7 +7071,7 @@
         <v>0.01</v>
       </c>
       <c r="I26" t="s">
-        <v>309</v>
+        <v>339</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
@@ -7070,7 +7100,7 @@
         <v>0.01</v>
       </c>
       <c r="I27" t="s">
-        <v>309</v>
+        <v>339</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
@@ -7099,7 +7129,7 @@
         <v>1</v>
       </c>
       <c r="I28" t="s">
-        <v>309</v>
+        <v>341</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
@@ -7128,7 +7158,7 @@
         <v>1</v>
       </c>
       <c r="I29" t="s">
-        <v>308</v>
+        <v>342</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
@@ -7157,7 +7187,7 @@
         <v>1</v>
       </c>
       <c r="I30" t="s">
-        <v>308</v>
+        <v>342</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
@@ -7186,7 +7216,7 @@
         <v>1</v>
       </c>
       <c r="I31" t="s">
-        <v>308</v>
+        <v>342</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
@@ -7215,7 +7245,7 @@
         <v>0.01</v>
       </c>
       <c r="I32" t="s">
-        <v>308</v>
+        <v>338</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
@@ -7244,7 +7274,7 @@
         <v>0.01</v>
       </c>
       <c r="I33" t="s">
-        <v>308</v>
+        <v>338</v>
       </c>
     </row>
   </sheetData>
@@ -7359,7 +7389,7 @@
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="G4" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="I4" t="s">
         <v>307</v>
@@ -7369,10 +7399,10 @@
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
       <c r="F5" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="G5" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="I5" t="s">
         <v>307</v>
@@ -7382,7 +7412,7 @@
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
       <c r="G6" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="I6" t="s">
         <v>307</v>
@@ -7537,7 +7567,7 @@
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="G12" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="I12" t="s">
         <v>307</v>
@@ -7547,7 +7577,7 @@
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="G13" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="I13" t="s">
         <v>307</v>
@@ -7644,7 +7674,7 @@
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
       <c r="G17" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="I17" t="s">
         <v>307</v>
@@ -7654,10 +7684,10 @@
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
       <c r="F18" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="G18" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="I18" t="s">
         <v>307</v>
@@ -7667,7 +7697,7 @@
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
       <c r="G19" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="I19" t="s">
         <v>307</v>
@@ -7820,7 +7850,7 @@
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="G25" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="I25" t="s">
         <v>307</v>
@@ -7828,7 +7858,7 @@
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="G26" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="I26" t="s">
         <v>307</v>

</xml_diff>

<commit_message>
added missing "name" column in Sheet12 and Sheet13
</commit_message>
<xml_diff>
--- a/data/Walnut_grain_veg_tub.xlsx
+++ b/data/Walnut_grain_veg_tub.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mjimenez\Documents\ReForest\Living Labs for Mitigating Climate Change in Agriculture\DualPurpose_Trees\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F68B87DA-8B41-4E8C-A3AD-4D8C92D3D52A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4435E1BD-B3C2-4CA4-B2AC-51D2F79711C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" firstSheet="6" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" firstSheet="6" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sheet_names" sheetId="17" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1073" uniqueCount="464">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1079" uniqueCount="465">
   <si>
     <t>variable</t>
   </si>
@@ -718,9 +718,6 @@
     <t>Annual maintenance support: Lump sum of funds received annually from external sources in order to maintain the agroforestry system [€]</t>
   </si>
   <si>
-    <t>The price of one tone of certified CO2 sequestration [t CO2eq]</t>
-  </si>
-  <si>
     <t>Mean annual soil loss due to water erosion [t/ha]</t>
   </si>
   <si>
@@ -1424,6 +1421,12 @@
   </si>
   <si>
     <t>Impact of crop production difference between alley and treeless cropping on SOC change</t>
+  </si>
+  <si>
+    <t>Carbon certificate price</t>
+  </si>
+  <si>
+    <t>The income received by the farmer for one tone of certified CO2 sequestration [t CO2eq]</t>
   </si>
 </sst>
 </file>
@@ -2290,7 +2293,7 @@
         <v>158</v>
       </c>
       <c r="B1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
@@ -2298,7 +2301,7 @@
         <v>159</v>
       </c>
       <c r="B2" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
@@ -2306,7 +2309,7 @@
         <v>163</v>
       </c>
       <c r="B3" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
@@ -2314,7 +2317,7 @@
         <v>164</v>
       </c>
       <c r="B4" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
@@ -2322,7 +2325,7 @@
         <v>160</v>
       </c>
       <c r="B5" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
@@ -2330,7 +2333,7 @@
         <v>167</v>
       </c>
       <c r="B6" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
@@ -2338,7 +2341,7 @@
         <v>165</v>
       </c>
       <c r="B7" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
@@ -2346,7 +2349,7 @@
         <v>166</v>
       </c>
       <c r="B8" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
@@ -2354,7 +2357,7 @@
         <v>168</v>
       </c>
       <c r="B9" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
@@ -2362,7 +2365,7 @@
         <v>169</v>
       </c>
       <c r="B10" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
@@ -2370,7 +2373,7 @@
         <v>161</v>
       </c>
       <c r="B11" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
@@ -2378,7 +2381,7 @@
         <v>170</v>
       </c>
       <c r="B12" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
@@ -2386,7 +2389,7 @@
         <v>162</v>
       </c>
       <c r="B13" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
   </sheetData>
@@ -2429,7 +2432,7 @@
         <v>135</v>
       </c>
       <c r="F1" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="G1" t="s">
         <v>136</v>
@@ -2441,7 +2444,7 @@
         <v>139</v>
       </c>
       <c r="J1" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.35">
@@ -2461,7 +2464,7 @@
         <v>171</v>
       </c>
       <c r="F2" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="G2" t="s">
         <v>227</v>
@@ -2473,7 +2476,7 @@
         <v>1</v>
       </c>
       <c r="J2" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.35">
@@ -2493,7 +2496,7 @@
         <v>55</v>
       </c>
       <c r="F3" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="G3" t="s">
         <v>225</v>
@@ -2505,7 +2508,7 @@
         <v>1</v>
       </c>
       <c r="J3" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.35">
@@ -2525,7 +2528,7 @@
         <v>60</v>
       </c>
       <c r="F4" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="G4" t="s">
         <v>224</v>
@@ -2537,7 +2540,7 @@
         <v>1E-3</v>
       </c>
       <c r="J4" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.35">
@@ -2557,7 +2560,7 @@
         <v>171</v>
       </c>
       <c r="F5" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="G5" t="s">
         <v>226</v>
@@ -2569,7 +2572,7 @@
         <v>1</v>
       </c>
       <c r="J5" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
   </sheetData>
@@ -2581,9 +2584,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{724F1830-3430-4657-920D-E95506196AA8}">
   <dimension ref="A1:J29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -2609,7 +2610,7 @@
         <v>135</v>
       </c>
       <c r="F1" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="G1" t="s">
         <v>136</v>
@@ -2621,7 +2622,7 @@
         <v>139</v>
       </c>
       <c r="J1" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.35">
@@ -2641,10 +2642,10 @@
         <v>105</v>
       </c>
       <c r="F2" t="s">
+        <v>442</v>
+      </c>
+      <c r="G2" t="s">
         <v>443</v>
-      </c>
-      <c r="G2" t="s">
-        <v>444</v>
       </c>
       <c r="H2" t="s">
         <v>138</v>
@@ -2653,7 +2654,7 @@
         <v>0.01</v>
       </c>
       <c r="J2" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.35">
@@ -2673,10 +2674,10 @@
         <v>60</v>
       </c>
       <c r="F3" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="G3" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="H3" t="s">
         <v>138</v>
@@ -2685,43 +2686,43 @@
         <v>1E-3</v>
       </c>
       <c r="J3" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="H4" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="J4" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
       <c r="F5" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="G5" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="H5" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="J5" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
       <c r="H6" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="J6" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.35">
@@ -2741,10 +2742,10 @@
         <v>60</v>
       </c>
       <c r="F7" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="G7" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="H7" t="s">
         <v>138</v>
@@ -2753,7 +2754,7 @@
         <v>1</v>
       </c>
       <c r="J7" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.35">
@@ -2773,16 +2774,16 @@
         <v>60</v>
       </c>
       <c r="F8" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="G8" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="H8" t="s">
         <v>138</v>
       </c>
       <c r="J8" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.35">
@@ -2802,16 +2803,16 @@
         <v>60</v>
       </c>
       <c r="F9" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="G9" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="H9" t="s">
         <v>138</v>
       </c>
       <c r="J9" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.35">
@@ -2831,52 +2832,52 @@
         <v>110</v>
       </c>
       <c r="F10" t="s">
+        <v>446</v>
+      </c>
+      <c r="G10" t="s">
         <v>447</v>
       </c>
-      <c r="G10" t="s">
-        <v>448</v>
-      </c>
       <c r="H10" t="s">
         <v>138</v>
       </c>
       <c r="J10" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="H11" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="J11" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="F12" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="G12" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="H12" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="J12" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="H13" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="J13" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.35">
@@ -2896,10 +2897,10 @@
         <v>38</v>
       </c>
       <c r="F14" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="G14" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="H14" t="s">
         <v>138</v>
@@ -2908,7 +2909,7 @@
         <v>1</v>
       </c>
       <c r="J14" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.35">
@@ -2928,10 +2929,10 @@
         <v>38</v>
       </c>
       <c r="F15" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="G15" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="H15" t="s">
         <v>138</v>
@@ -2940,7 +2941,7 @@
         <v>1</v>
       </c>
       <c r="J15" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.35">
@@ -2960,10 +2961,10 @@
         <v>115</v>
       </c>
       <c r="F16" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="G16" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="H16" t="s">
         <v>138</v>
@@ -2972,7 +2973,7 @@
         <v>1</v>
       </c>
       <c r="J16" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.35">
@@ -2992,10 +2993,10 @@
         <v>115</v>
       </c>
       <c r="F17" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="G17" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="H17" t="s">
         <v>138</v>
@@ -3004,7 +3005,7 @@
         <v>1</v>
       </c>
       <c r="J17" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.35">
@@ -3024,16 +3025,16 @@
         <v>110</v>
       </c>
       <c r="F18" t="s">
+        <v>453</v>
+      </c>
+      <c r="G18" t="s">
         <v>454</v>
       </c>
-      <c r="G18" t="s">
-        <v>455</v>
-      </c>
       <c r="H18" t="s">
         <v>138</v>
       </c>
       <c r="J18" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.35">
@@ -3053,16 +3054,16 @@
         <v>110</v>
       </c>
       <c r="F19" t="s">
+        <v>455</v>
+      </c>
+      <c r="G19" t="s">
         <v>456</v>
       </c>
-      <c r="G19" t="s">
-        <v>457</v>
-      </c>
       <c r="H19" t="s">
         <v>138</v>
       </c>
       <c r="J19" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.35">
@@ -3082,10 +3083,10 @@
         <v>120</v>
       </c>
       <c r="F20" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="G20" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="H20" t="s">
         <v>138</v>
@@ -3094,7 +3095,7 @@
         <v>0.01</v>
       </c>
       <c r="J20" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.35">
@@ -3114,10 +3115,10 @@
         <v>60</v>
       </c>
       <c r="F21" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="G21" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="H21" t="s">
         <v>138</v>
@@ -3126,7 +3127,7 @@
         <v>1E-3</v>
       </c>
       <c r="J21" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.35">
@@ -3146,10 +3147,10 @@
         <v>60</v>
       </c>
       <c r="F22" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="G22" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="H22" t="s">
         <v>140</v>
@@ -3158,7 +3159,7 @@
         <v>1E-3</v>
       </c>
       <c r="J22" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.35">
@@ -3178,16 +3179,16 @@
         <v>122</v>
       </c>
       <c r="F23" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="G23" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="H23" t="s">
         <v>138</v>
       </c>
       <c r="J23" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.35">
@@ -3207,16 +3208,16 @@
         <v>13</v>
       </c>
       <c r="F24" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="G24" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="H24" t="s">
         <v>138</v>
       </c>
       <c r="J24" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.35">
@@ -3236,30 +3237,30 @@
         <v>60</v>
       </c>
       <c r="F25" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="G25" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="H25" t="s">
         <v>138</v>
       </c>
       <c r="J25" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
       <c r="H26" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
       <c r="H27" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.35">
@@ -3277,10 +3278,10 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2682F285-7B44-4D8F-A7EA-4445FB570320}">
-  <dimension ref="A1:I122"/>
+  <dimension ref="A1:J122"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3290,7 +3291,7 @@
     <col min="9" max="9" width="18.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3307,19 +3308,22 @@
         <v>135</v>
       </c>
       <c r="F1" t="s">
+        <v>287</v>
+      </c>
+      <c r="G1" t="s">
         <v>136</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>137</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>139</v>
       </c>
-      <c r="I1" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J1" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>157</v>
       </c>
@@ -3336,71 +3340,74 @@
         <v>172</v>
       </c>
       <c r="F2" t="s">
-        <v>228</v>
+        <v>463</v>
       </c>
       <c r="G2" t="s">
-        <v>138</v>
-      </c>
-      <c r="H2">
-        <v>1</v>
-      </c>
-      <c r="I2" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+        <v>464</v>
+      </c>
+      <c r="H2" t="s">
+        <v>138</v>
+      </c>
+      <c r="I2">
+        <v>1</v>
+      </c>
+      <c r="J2" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
     </row>
@@ -3835,10 +3842,10 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0AACA546-DF26-443B-AA33-3E83721C2724}">
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:J5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O10" sqref="O10"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2:F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3851,7 +3858,7 @@
     <col min="9" max="9" width="37" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3867,20 +3874,20 @@
       <c r="E1" t="s">
         <v>135</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>136</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>137</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>139</v>
       </c>
-      <c r="I1" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J1" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>37</v>
       </c>
@@ -3897,19 +3904,22 @@
         <v>38</v>
       </c>
       <c r="F2" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="G2" t="s">
-        <v>138</v>
-      </c>
-      <c r="H2">
+        <v>228</v>
+      </c>
+      <c r="H2" t="s">
+        <v>138</v>
+      </c>
+      <c r="I2">
         <v>0.01</v>
       </c>
-      <c r="I2" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J2" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>39</v>
       </c>
@@ -3926,19 +3936,22 @@
         <v>38</v>
       </c>
       <c r="F3" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="G3" t="s">
-        <v>138</v>
-      </c>
-      <c r="H3">
+        <v>229</v>
+      </c>
+      <c r="H3" t="s">
+        <v>138</v>
+      </c>
+      <c r="I3">
         <v>1E-3</v>
       </c>
-      <c r="I3" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J3" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>156</v>
       </c>
@@ -3955,19 +3968,22 @@
         <v>173</v>
       </c>
       <c r="F4" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="G4" t="s">
+        <v>230</v>
+      </c>
+      <c r="H4" t="s">
         <v>140</v>
       </c>
-      <c r="H4">
-        <v>1</v>
-      </c>
-      <c r="I4" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I4">
+        <v>1</v>
+      </c>
+      <c r="J4" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>155</v>
       </c>
@@ -3984,16 +4000,19 @@
         <v>174</v>
       </c>
       <c r="F5" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="G5" t="s">
+        <v>231</v>
+      </c>
+      <c r="H5" t="s">
         <v>140</v>
       </c>
-      <c r="H5">
-        <v>1</v>
-      </c>
-      <c r="I5" t="s">
-        <v>287</v>
+      <c r="I5">
+        <v>1</v>
+      </c>
+      <c r="J5" t="s">
+        <v>286</v>
       </c>
     </row>
   </sheetData>
@@ -4035,7 +4054,7 @@
         <v>135</v>
       </c>
       <c r="F1" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="G1" t="s">
         <v>136</v>
@@ -4047,7 +4066,7 @@
         <v>139</v>
       </c>
       <c r="J1" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.35">
@@ -4067,10 +4086,10 @@
         <v>8</v>
       </c>
       <c r="F2" t="s">
+        <v>288</v>
+      </c>
+      <c r="G2" t="s">
         <v>289</v>
-      </c>
-      <c r="G2" t="s">
-        <v>290</v>
       </c>
       <c r="H2" t="s">
         <v>140</v>
@@ -4079,7 +4098,7 @@
         <v>1</v>
       </c>
       <c r="J2" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.35">
@@ -4099,11 +4118,11 @@
         <v>13</v>
       </c>
       <c r="F3" t="s">
+        <v>290</v>
+      </c>
+      <c r="G3" t="s">
         <v>291</v>
       </c>
-      <c r="G3" t="s">
-        <v>292</v>
-      </c>
       <c r="H3" t="s">
         <v>138</v>
       </c>
@@ -4111,7 +4130,7 @@
         <v>1</v>
       </c>
       <c r="J3" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.35">
@@ -4131,10 +4150,10 @@
         <v>55</v>
       </c>
       <c r="F4" t="s">
+        <v>292</v>
+      </c>
+      <c r="G4" t="s">
         <v>293</v>
-      </c>
-      <c r="G4" t="s">
-        <v>294</v>
       </c>
       <c r="H4" t="s">
         <v>140</v>
@@ -4143,7 +4162,7 @@
         <v>1</v>
       </c>
       <c r="J4" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.35">
@@ -4163,10 +4182,10 @@
         <v>55</v>
       </c>
       <c r="F5" t="s">
+        <v>294</v>
+      </c>
+      <c r="G5" t="s">
         <v>295</v>
-      </c>
-      <c r="G5" t="s">
-        <v>296</v>
       </c>
       <c r="H5" t="s">
         <v>140</v>
@@ -4175,7 +4194,7 @@
         <v>1</v>
       </c>
       <c r="J5" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.35">
@@ -4195,7 +4214,7 @@
         <v>6</v>
       </c>
       <c r="F6" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="G6" t="s">
         <v>179</v>
@@ -4207,7 +4226,7 @@
         <v>1</v>
       </c>
       <c r="J6" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.35">
@@ -4227,11 +4246,11 @@
         <v>13</v>
       </c>
       <c r="F7" t="s">
+        <v>297</v>
+      </c>
+      <c r="G7" t="s">
         <v>298</v>
       </c>
-      <c r="G7" t="s">
-        <v>299</v>
-      </c>
       <c r="H7" t="s">
         <v>138</v>
       </c>
@@ -4239,7 +4258,7 @@
         <v>1</v>
       </c>
       <c r="J7" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.35">
@@ -4735,7 +4754,7 @@
         <v>135</v>
       </c>
       <c r="F1" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="G1" t="s">
         <v>136</v>
@@ -4747,7 +4766,7 @@
         <v>139</v>
       </c>
       <c r="J1" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.35">
@@ -4767,10 +4786,10 @@
         <v>10</v>
       </c>
       <c r="F2" t="s">
+        <v>299</v>
+      </c>
+      <c r="G2" t="s">
         <v>300</v>
-      </c>
-      <c r="G2" t="s">
-        <v>301</v>
       </c>
       <c r="H2" t="s">
         <v>140</v>
@@ -4779,7 +4798,7 @@
         <v>0.01</v>
       </c>
       <c r="J2" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.35">
@@ -4799,10 +4818,10 @@
         <v>10</v>
       </c>
       <c r="F3" t="s">
+        <v>301</v>
+      </c>
+      <c r="G3" t="s">
         <v>302</v>
-      </c>
-      <c r="G3" t="s">
-        <v>303</v>
       </c>
       <c r="H3" t="s">
         <v>140</v>
@@ -4811,7 +4830,7 @@
         <v>1E-4</v>
       </c>
       <c r="J3" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="K3" s="1"/>
     </row>
@@ -4832,10 +4851,10 @@
         <v>18</v>
       </c>
       <c r="F4" t="s">
+        <v>303</v>
+      </c>
+      <c r="G4" t="s">
         <v>304</v>
-      </c>
-      <c r="G4" t="s">
-        <v>305</v>
       </c>
       <c r="H4" t="s">
         <v>140</v>
@@ -4844,7 +4863,7 @@
         <v>1</v>
       </c>
       <c r="J4" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.35">
@@ -4864,10 +4883,10 @@
         <v>10</v>
       </c>
       <c r="F5" t="s">
+        <v>305</v>
+      </c>
+      <c r="G5" t="s">
         <v>306</v>
-      </c>
-      <c r="G5" t="s">
-        <v>307</v>
       </c>
       <c r="H5" t="s">
         <v>140</v>
@@ -4876,7 +4895,7 @@
         <v>1E-3</v>
       </c>
       <c r="J5" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.35">
@@ -5370,7 +5389,7 @@
         <v>135</v>
       </c>
       <c r="F1" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="G1" t="s">
         <v>136</v>
@@ -5382,7 +5401,7 @@
         <v>139</v>
       </c>
       <c r="J1" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.35">
@@ -5402,11 +5421,11 @@
         <v>178</v>
       </c>
       <c r="F2" t="s">
+        <v>307</v>
+      </c>
+      <c r="G2" t="s">
         <v>308</v>
       </c>
-      <c r="G2" t="s">
-        <v>309</v>
-      </c>
       <c r="H2" t="s">
         <v>138</v>
       </c>
@@ -5414,7 +5433,7 @@
         <v>1</v>
       </c>
       <c r="J2" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.35">
@@ -5434,11 +5453,11 @@
         <v>171</v>
       </c>
       <c r="F3" t="s">
+        <v>309</v>
+      </c>
+      <c r="G3" t="s">
         <v>310</v>
       </c>
-      <c r="G3" t="s">
-        <v>311</v>
-      </c>
       <c r="H3" t="s">
         <v>138</v>
       </c>
@@ -5446,7 +5465,7 @@
         <v>1</v>
       </c>
       <c r="J3" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.35">
@@ -5466,11 +5485,11 @@
         <v>171</v>
       </c>
       <c r="F4" t="s">
+        <v>311</v>
+      </c>
+      <c r="G4" t="s">
         <v>312</v>
       </c>
-      <c r="G4" t="s">
-        <v>313</v>
-      </c>
       <c r="H4" t="s">
         <v>138</v>
       </c>
@@ -5478,7 +5497,7 @@
         <v>1</v>
       </c>
       <c r="J4" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
   </sheetData>
@@ -5521,7 +5540,7 @@
         <v>135</v>
       </c>
       <c r="F1" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="G1" t="s">
         <v>136</v>
@@ -5533,7 +5552,7 @@
         <v>139</v>
       </c>
       <c r="J1" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.35">
@@ -5553,11 +5572,11 @@
         <v>177</v>
       </c>
       <c r="F2" t="s">
+        <v>313</v>
+      </c>
+      <c r="G2" t="s">
         <v>314</v>
       </c>
-      <c r="G2" t="s">
-        <v>315</v>
-      </c>
       <c r="H2" t="s">
         <v>138</v>
       </c>
@@ -5565,7 +5584,7 @@
         <v>1</v>
       </c>
       <c r="J2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.35">
@@ -5585,11 +5604,11 @@
         <v>180</v>
       </c>
       <c r="F3" t="s">
+        <v>315</v>
+      </c>
+      <c r="G3" t="s">
         <v>316</v>
       </c>
-      <c r="G3" t="s">
-        <v>317</v>
-      </c>
       <c r="H3" t="s">
         <v>138</v>
       </c>
@@ -5597,7 +5616,7 @@
         <v>1</v>
       </c>
       <c r="J3" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.35">
@@ -5617,11 +5636,11 @@
         <v>180</v>
       </c>
       <c r="F4" t="s">
+        <v>317</v>
+      </c>
+      <c r="G4" t="s">
         <v>318</v>
       </c>
-      <c r="G4" t="s">
-        <v>319</v>
-      </c>
       <c r="H4" t="s">
         <v>138</v>
       </c>
@@ -5629,7 +5648,7 @@
         <v>1</v>
       </c>
       <c r="J4" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.35">
@@ -5649,11 +5668,11 @@
         <v>180</v>
       </c>
       <c r="F5" t="s">
+        <v>319</v>
+      </c>
+      <c r="G5" t="s">
         <v>320</v>
       </c>
-      <c r="G5" t="s">
-        <v>321</v>
-      </c>
       <c r="H5" t="s">
         <v>138</v>
       </c>
@@ -5661,7 +5680,7 @@
         <v>1</v>
       </c>
       <c r="J5" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.35">
@@ -5681,11 +5700,11 @@
         <v>180</v>
       </c>
       <c r="F6" t="s">
+        <v>321</v>
+      </c>
+      <c r="G6" t="s">
         <v>322</v>
       </c>
-      <c r="G6" t="s">
-        <v>323</v>
-      </c>
       <c r="H6" t="s">
         <v>138</v>
       </c>
@@ -5693,7 +5712,7 @@
         <v>1</v>
       </c>
       <c r="J6" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.35">
@@ -5713,11 +5732,11 @@
         <v>180</v>
       </c>
       <c r="F7" t="s">
+        <v>323</v>
+      </c>
+      <c r="G7" t="s">
         <v>324</v>
       </c>
-      <c r="G7" t="s">
-        <v>325</v>
-      </c>
       <c r="H7" t="s">
         <v>138</v>
       </c>
@@ -5725,7 +5744,7 @@
         <v>1</v>
       </c>
       <c r="J7" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.35">
@@ -5745,11 +5764,11 @@
         <v>180</v>
       </c>
       <c r="F8" t="s">
+        <v>325</v>
+      </c>
+      <c r="G8" t="s">
         <v>326</v>
       </c>
-      <c r="G8" t="s">
-        <v>327</v>
-      </c>
       <c r="H8" t="s">
         <v>138</v>
       </c>
@@ -5757,7 +5776,7 @@
         <v>1</v>
       </c>
       <c r="J8" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.35">
@@ -5777,11 +5796,11 @@
         <v>180</v>
       </c>
       <c r="F9" t="s">
+        <v>327</v>
+      </c>
+      <c r="G9" t="s">
         <v>328</v>
       </c>
-      <c r="G9" t="s">
-        <v>329</v>
-      </c>
       <c r="H9" t="s">
         <v>138</v>
       </c>
@@ -5789,7 +5808,7 @@
         <v>1</v>
       </c>
       <c r="J9" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.35">
@@ -5809,10 +5828,10 @@
         <v>60</v>
       </c>
       <c r="F10" t="s">
+        <v>329</v>
+      </c>
+      <c r="G10" t="s">
         <v>330</v>
-      </c>
-      <c r="G10" t="s">
-        <v>331</v>
       </c>
       <c r="H10" t="s">
         <v>138</v>
@@ -5821,7 +5840,7 @@
         <v>1E-3</v>
       </c>
       <c r="J10" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.35">
@@ -5841,11 +5860,11 @@
         <v>24</v>
       </c>
       <c r="F11" t="s">
+        <v>331</v>
+      </c>
+      <c r="G11" t="s">
         <v>332</v>
       </c>
-      <c r="G11" t="s">
-        <v>333</v>
-      </c>
       <c r="H11" t="s">
         <v>138</v>
       </c>
@@ -5853,7 +5872,7 @@
         <v>1</v>
       </c>
       <c r="J11" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.35">
@@ -5873,11 +5892,11 @@
         <v>181</v>
       </c>
       <c r="F12" t="s">
+        <v>333</v>
+      </c>
+      <c r="G12" t="s">
         <v>334</v>
       </c>
-      <c r="G12" t="s">
-        <v>335</v>
-      </c>
       <c r="H12" t="s">
         <v>138</v>
       </c>
@@ -5885,7 +5904,7 @@
         <v>1</v>
       </c>
       <c r="J12" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.35">
@@ -5905,11 +5924,11 @@
         <v>28</v>
       </c>
       <c r="F13" t="s">
+        <v>335</v>
+      </c>
+      <c r="G13" t="s">
         <v>336</v>
       </c>
-      <c r="G13" t="s">
-        <v>337</v>
-      </c>
       <c r="H13" t="s">
         <v>138</v>
       </c>
@@ -5917,7 +5936,7 @@
         <v>1</v>
       </c>
       <c r="J13" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.35">
@@ -5937,10 +5956,10 @@
         <v>30</v>
       </c>
       <c r="F14" t="s">
+        <v>337</v>
+      </c>
+      <c r="G14" t="s">
         <v>338</v>
-      </c>
-      <c r="G14" t="s">
-        <v>339</v>
       </c>
       <c r="H14" t="s">
         <v>138</v>
@@ -5949,7 +5968,7 @@
         <v>0.01</v>
       </c>
       <c r="J14" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.35">
@@ -5969,11 +5988,11 @@
         <v>24</v>
       </c>
       <c r="F15" t="s">
+        <v>339</v>
+      </c>
+      <c r="G15" t="s">
         <v>340</v>
       </c>
-      <c r="G15" t="s">
-        <v>341</v>
-      </c>
       <c r="H15" t="s">
         <v>138</v>
       </c>
@@ -5981,7 +6000,7 @@
         <v>1</v>
       </c>
       <c r="J15" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.35">
@@ -6001,11 +6020,11 @@
         <v>28</v>
       </c>
       <c r="F16" t="s">
+        <v>341</v>
+      </c>
+      <c r="G16" t="s">
         <v>342</v>
       </c>
-      <c r="G16" t="s">
-        <v>343</v>
-      </c>
       <c r="H16" t="s">
         <v>138</v>
       </c>
@@ -6013,7 +6032,7 @@
         <v>1</v>
       </c>
       <c r="J16" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.35">
@@ -6033,10 +6052,10 @@
         <v>180</v>
       </c>
       <c r="F17" t="s">
+        <v>343</v>
+      </c>
+      <c r="G17" t="s">
         <v>344</v>
-      </c>
-      <c r="G17" t="s">
-        <v>345</v>
       </c>
       <c r="H17" t="s">
         <v>138</v>
@@ -6045,7 +6064,7 @@
         <v>1E-3</v>
       </c>
       <c r="J17" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.35">
@@ -6065,10 +6084,10 @@
         <v>30</v>
       </c>
       <c r="F18" t="s">
+        <v>345</v>
+      </c>
+      <c r="G18" t="s">
         <v>346</v>
-      </c>
-      <c r="G18" t="s">
-        <v>347</v>
       </c>
       <c r="H18" t="s">
         <v>138</v>
@@ -6077,7 +6096,7 @@
         <v>1E-3</v>
       </c>
       <c r="J18" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.35">
@@ -6097,10 +6116,10 @@
         <v>30</v>
       </c>
       <c r="F19" t="s">
+        <v>347</v>
+      </c>
+      <c r="G19" t="s">
         <v>348</v>
-      </c>
-      <c r="G19" t="s">
-        <v>349</v>
       </c>
       <c r="H19" t="s">
         <v>138</v>
@@ -6109,7 +6128,7 @@
         <v>1E-3</v>
       </c>
       <c r="J19" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.35">
@@ -6129,10 +6148,10 @@
         <v>99</v>
       </c>
       <c r="F20" t="s">
+        <v>349</v>
+      </c>
+      <c r="G20" t="s">
         <v>350</v>
-      </c>
-      <c r="G20" t="s">
-        <v>351</v>
       </c>
       <c r="H20" t="s">
         <v>138</v>
@@ -6141,7 +6160,7 @@
         <v>1E-3</v>
       </c>
       <c r="J20" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.35">
@@ -6161,10 +6180,10 @@
         <v>30</v>
       </c>
       <c r="F21" t="s">
+        <v>351</v>
+      </c>
+      <c r="G21" t="s">
         <v>352</v>
-      </c>
-      <c r="G21" t="s">
-        <v>353</v>
       </c>
       <c r="H21" t="s">
         <v>138</v>
@@ -6173,7 +6192,7 @@
         <v>1E-4</v>
       </c>
       <c r="J21" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.35">
@@ -6193,10 +6212,10 @@
         <v>28</v>
       </c>
       <c r="F22" t="s">
+        <v>353</v>
+      </c>
+      <c r="G22" t="s">
         <v>354</v>
-      </c>
-      <c r="G22" t="s">
-        <v>355</v>
       </c>
       <c r="H22" t="s">
         <v>138</v>
@@ -6205,7 +6224,7 @@
         <v>0.01</v>
       </c>
       <c r="J22" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.35">
@@ -6225,11 +6244,11 @@
         <v>174</v>
       </c>
       <c r="F23" t="s">
+        <v>355</v>
+      </c>
+      <c r="G23" t="s">
         <v>356</v>
       </c>
-      <c r="G23" t="s">
-        <v>357</v>
-      </c>
       <c r="H23" t="s">
         <v>138</v>
       </c>
@@ -6237,7 +6256,7 @@
         <v>1</v>
       </c>
       <c r="J23" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.35">
@@ -6257,11 +6276,11 @@
         <v>174</v>
       </c>
       <c r="F24" t="s">
+        <v>357</v>
+      </c>
+      <c r="G24" t="s">
         <v>358</v>
       </c>
-      <c r="G24" t="s">
-        <v>359</v>
-      </c>
       <c r="H24" t="s">
         <v>138</v>
       </c>
@@ -6269,7 +6288,7 @@
         <v>1</v>
       </c>
       <c r="J24" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.35">
@@ -6289,11 +6308,11 @@
         <v>24</v>
       </c>
       <c r="F25" t="s">
+        <v>359</v>
+      </c>
+      <c r="G25" t="s">
         <v>360</v>
       </c>
-      <c r="G25" t="s">
-        <v>361</v>
-      </c>
       <c r="H25" t="s">
         <v>138</v>
       </c>
@@ -6301,7 +6320,7 @@
         <v>1</v>
       </c>
       <c r="J25" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.35">
@@ -6321,10 +6340,10 @@
         <v>60</v>
       </c>
       <c r="F26" t="s">
+        <v>361</v>
+      </c>
+      <c r="G26" t="s">
         <v>362</v>
-      </c>
-      <c r="G26" t="s">
-        <v>363</v>
       </c>
       <c r="H26" t="s">
         <v>138</v>
@@ -6333,7 +6352,7 @@
         <v>1E-3</v>
       </c>
       <c r="J26" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.35">
@@ -6378,7 +6397,7 @@
         <v>135</v>
       </c>
       <c r="F1" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="G1" t="s">
         <v>136</v>
@@ -6390,7 +6409,7 @@
         <v>139</v>
       </c>
       <c r="J1" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.35">
@@ -6410,11 +6429,11 @@
         <v>174</v>
       </c>
       <c r="F2" t="s">
+        <v>363</v>
+      </c>
+      <c r="G2" t="s">
         <v>364</v>
       </c>
-      <c r="G2" t="s">
-        <v>365</v>
-      </c>
       <c r="H2" t="s">
         <v>138</v>
       </c>
@@ -6422,7 +6441,7 @@
         <v>1</v>
       </c>
       <c r="J2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.35">
@@ -6442,7 +6461,7 @@
         <v>38</v>
       </c>
       <c r="F3" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="G3" t="s">
         <v>182</v>
@@ -6454,7 +6473,7 @@
         <v>1</v>
       </c>
       <c r="J3" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.35">
@@ -6474,11 +6493,11 @@
         <v>173</v>
       </c>
       <c r="F4" t="s">
+        <v>366</v>
+      </c>
+      <c r="G4" t="s">
         <v>367</v>
       </c>
-      <c r="G4" t="s">
-        <v>368</v>
-      </c>
       <c r="H4" t="s">
         <v>138</v>
       </c>
@@ -6486,7 +6505,7 @@
         <v>1</v>
       </c>
       <c r="J4" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.35">
@@ -6506,7 +6525,7 @@
         <v>174</v>
       </c>
       <c r="F5" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="G5" t="s">
         <v>186</v>
@@ -6518,7 +6537,7 @@
         <v>1</v>
       </c>
       <c r="J5" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.35">
@@ -6538,7 +6557,7 @@
         <v>38</v>
       </c>
       <c r="F6" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="G6" t="s">
         <v>183</v>
@@ -6550,7 +6569,7 @@
         <v>1</v>
       </c>
       <c r="J6" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.35">
@@ -6570,7 +6589,7 @@
         <v>173</v>
       </c>
       <c r="F7" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="G7" t="s">
         <v>184</v>
@@ -6582,7 +6601,7 @@
         <v>1</v>
       </c>
       <c r="J7" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.35">
@@ -6602,11 +6621,11 @@
         <v>174</v>
       </c>
       <c r="F8" t="s">
+        <v>371</v>
+      </c>
+      <c r="G8" t="s">
         <v>372</v>
       </c>
-      <c r="G8" t="s">
-        <v>373</v>
-      </c>
       <c r="H8" t="s">
         <v>138</v>
       </c>
@@ -6614,7 +6633,7 @@
         <v>1</v>
       </c>
       <c r="J8" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.35">
@@ -6634,7 +6653,7 @@
         <v>38</v>
       </c>
       <c r="F9" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="G9" t="s">
         <v>185</v>
@@ -6646,7 +6665,7 @@
         <v>1</v>
       </c>
       <c r="J9" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.35">
@@ -6666,11 +6685,11 @@
         <v>173</v>
       </c>
       <c r="F10" t="s">
+        <v>374</v>
+      </c>
+      <c r="G10" t="s">
         <v>375</v>
       </c>
-      <c r="G10" t="s">
-        <v>376</v>
-      </c>
       <c r="H10" t="s">
         <v>138</v>
       </c>
@@ -6678,7 +6697,7 @@
         <v>1</v>
       </c>
       <c r="J10" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.35">
@@ -6698,11 +6717,11 @@
         <v>174</v>
       </c>
       <c r="F11" t="s">
+        <v>376</v>
+      </c>
+      <c r="G11" t="s">
         <v>377</v>
       </c>
-      <c r="G11" t="s">
-        <v>378</v>
-      </c>
       <c r="H11" t="s">
         <v>138</v>
       </c>
@@ -6710,7 +6729,7 @@
         <v>1</v>
       </c>
       <c r="J11" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.35">
@@ -6730,11 +6749,11 @@
         <v>38</v>
       </c>
       <c r="F12" t="s">
+        <v>378</v>
+      </c>
+      <c r="G12" t="s">
         <v>379</v>
       </c>
-      <c r="G12" t="s">
-        <v>380</v>
-      </c>
       <c r="H12" t="s">
         <v>138</v>
       </c>
@@ -6742,7 +6761,7 @@
         <v>1</v>
       </c>
       <c r="J12" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.35">
@@ -6762,11 +6781,11 @@
         <v>173</v>
       </c>
       <c r="F13" t="s">
+        <v>380</v>
+      </c>
+      <c r="G13" t="s">
         <v>381</v>
       </c>
-      <c r="G13" t="s">
-        <v>382</v>
-      </c>
       <c r="H13" t="s">
         <v>138</v>
       </c>
@@ -6774,7 +6793,7 @@
         <v>1</v>
       </c>
       <c r="J13" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.35">
@@ -6794,11 +6813,11 @@
         <v>174</v>
       </c>
       <c r="F14" t="s">
+        <v>382</v>
+      </c>
+      <c r="G14" t="s">
         <v>383</v>
       </c>
-      <c r="G14" t="s">
-        <v>384</v>
-      </c>
       <c r="H14" t="s">
         <v>138</v>
       </c>
@@ -6806,7 +6825,7 @@
         <v>1</v>
       </c>
       <c r="J14" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.35">
@@ -6826,7 +6845,7 @@
         <v>38</v>
       </c>
       <c r="F15" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="G15" t="s">
         <v>187</v>
@@ -6838,7 +6857,7 @@
         <v>1</v>
       </c>
       <c r="J15" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.35">
@@ -6858,11 +6877,11 @@
         <v>173</v>
       </c>
       <c r="F16" t="s">
+        <v>385</v>
+      </c>
+      <c r="G16" t="s">
         <v>386</v>
       </c>
-      <c r="G16" t="s">
-        <v>387</v>
-      </c>
       <c r="H16" t="s">
         <v>138</v>
       </c>
@@ -6870,7 +6889,7 @@
         <v>1</v>
       </c>
       <c r="J16" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.35">
@@ -6890,11 +6909,11 @@
         <v>174</v>
       </c>
       <c r="F17" t="s">
+        <v>387</v>
+      </c>
+      <c r="G17" t="s">
         <v>388</v>
       </c>
-      <c r="G17" t="s">
-        <v>389</v>
-      </c>
       <c r="H17" t="s">
         <v>138</v>
       </c>
@@ -6902,7 +6921,7 @@
         <v>1</v>
       </c>
       <c r="J17" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.35">
@@ -6922,7 +6941,7 @@
         <v>38</v>
       </c>
       <c r="F18" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="G18" t="s">
         <v>188</v>
@@ -6934,7 +6953,7 @@
         <v>0.01</v>
       </c>
       <c r="J18" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.35">
@@ -6954,11 +6973,11 @@
         <v>173</v>
       </c>
       <c r="F19" t="s">
+        <v>390</v>
+      </c>
+      <c r="G19" t="s">
         <v>391</v>
       </c>
-      <c r="G19" t="s">
-        <v>392</v>
-      </c>
       <c r="H19" t="s">
         <v>138</v>
       </c>
@@ -6966,7 +6985,7 @@
         <v>1</v>
       </c>
       <c r="J19" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.35">
@@ -6986,10 +7005,10 @@
         <v>174</v>
       </c>
       <c r="F20" t="s">
+        <v>392</v>
+      </c>
+      <c r="G20" t="s">
         <v>393</v>
-      </c>
-      <c r="G20" t="s">
-        <v>394</v>
       </c>
       <c r="H20" t="s">
         <v>138</v>
@@ -6998,7 +7017,7 @@
         <v>0.01</v>
       </c>
       <c r="J20" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.35">
@@ -7018,7 +7037,7 @@
         <v>38</v>
       </c>
       <c r="F21" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="G21" t="s">
         <v>189</v>
@@ -7030,7 +7049,7 @@
         <v>1</v>
       </c>
       <c r="J21" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.35">
@@ -7050,11 +7069,11 @@
         <v>173</v>
       </c>
       <c r="F22" t="s">
+        <v>395</v>
+      </c>
+      <c r="G22" t="s">
         <v>396</v>
       </c>
-      <c r="G22" t="s">
-        <v>397</v>
-      </c>
       <c r="H22" t="s">
         <v>138</v>
       </c>
@@ -7062,7 +7081,7 @@
         <v>1</v>
       </c>
       <c r="J22" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
   </sheetData>
@@ -7103,7 +7122,7 @@
         <v>135</v>
       </c>
       <c r="F1" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="G1" t="s">
         <v>136</v>
@@ -7115,43 +7134,43 @@
         <v>139</v>
       </c>
       <c r="J1" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
       <c r="H2" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="J2" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="F3" t="s">
+        <v>253</v>
+      </c>
+      <c r="G3" t="s">
+        <v>253</v>
+      </c>
+      <c r="H3" t="s">
         <v>254</v>
       </c>
-      <c r="G3" t="s">
-        <v>254</v>
-      </c>
-      <c r="H3" t="s">
-        <v>255</v>
-      </c>
       <c r="J3" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="H4" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="J4" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.35">
@@ -7171,7 +7190,7 @@
         <v>77</v>
       </c>
       <c r="F5" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="G5" t="s">
         <v>190</v>
@@ -7183,7 +7202,7 @@
         <v>1</v>
       </c>
       <c r="J5" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.35">
@@ -7203,7 +7222,7 @@
         <v>79</v>
       </c>
       <c r="F6" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="G6" t="s">
         <v>191</v>
@@ -7215,7 +7234,7 @@
         <v>1</v>
       </c>
       <c r="J6" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.35">
@@ -7235,7 +7254,7 @@
         <v>79</v>
       </c>
       <c r="F7" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="G7" t="s">
         <v>192</v>
@@ -7247,7 +7266,7 @@
         <v>1</v>
       </c>
       <c r="J7" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.35">
@@ -7267,7 +7286,7 @@
         <v>13</v>
       </c>
       <c r="F8" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="G8" t="s">
         <v>193</v>
@@ -7279,7 +7298,7 @@
         <v>1</v>
       </c>
       <c r="J8" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.35">
@@ -7299,7 +7318,7 @@
         <v>13</v>
       </c>
       <c r="F9" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="G9" t="s">
         <v>194</v>
@@ -7311,27 +7330,27 @@
         <v>1</v>
       </c>
       <c r="J9" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="H10" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="J10" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="H11" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="J11" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.35">
@@ -7351,7 +7370,7 @@
         <v>79</v>
       </c>
       <c r="F12" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="G12" t="s">
         <v>195</v>
@@ -7363,7 +7382,7 @@
         <v>1</v>
       </c>
       <c r="J12" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.35">
@@ -7383,10 +7402,10 @@
         <v>79</v>
       </c>
       <c r="F13" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="G13" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="H13" t="s">
         <v>138</v>
@@ -7395,7 +7414,7 @@
         <v>1</v>
       </c>
       <c r="J13" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.35">
@@ -7415,7 +7434,7 @@
         <v>60</v>
       </c>
       <c r="F14" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="G14" t="s">
         <v>206</v>
@@ -7427,43 +7446,43 @@
         <v>1E-3</v>
       </c>
       <c r="J14" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
       <c r="H15" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="J15" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
       <c r="F16" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="G16" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="H16" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="J16" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
       <c r="H17" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="J17" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.35">
@@ -7483,7 +7502,7 @@
         <v>86</v>
       </c>
       <c r="F18" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="G18" t="s">
         <v>198</v>
@@ -7495,7 +7514,7 @@
         <v>1</v>
       </c>
       <c r="J18" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.35">
@@ -7515,7 +7534,7 @@
         <v>79</v>
       </c>
       <c r="F19" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="G19" t="s">
         <v>196</v>
@@ -7527,7 +7546,7 @@
         <v>1</v>
       </c>
       <c r="J19" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.35">
@@ -7547,7 +7566,7 @@
         <v>79</v>
       </c>
       <c r="F20" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="G20" t="s">
         <v>197</v>
@@ -7559,7 +7578,7 @@
         <v>1</v>
       </c>
       <c r="J20" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.35">
@@ -7579,7 +7598,7 @@
         <v>13</v>
       </c>
       <c r="F21" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="G21" t="s">
         <v>199</v>
@@ -7591,7 +7610,7 @@
         <v>1</v>
       </c>
       <c r="J21" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.35">
@@ -7611,7 +7630,7 @@
         <v>13</v>
       </c>
       <c r="F22" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="G22" t="s">
         <v>200</v>
@@ -7623,7 +7642,7 @@
         <v>1</v>
       </c>
       <c r="J22" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.35">
@@ -7643,11 +7662,11 @@
         <v>13</v>
       </c>
       <c r="F23" t="s">
+        <v>410</v>
+      </c>
+      <c r="G23" t="s">
         <v>411</v>
       </c>
-      <c r="G23" t="s">
-        <v>412</v>
-      </c>
       <c r="H23" t="s">
         <v>138</v>
       </c>
@@ -7655,27 +7674,27 @@
         <v>1</v>
       </c>
       <c r="J23" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
       <c r="H24" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="J24" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
       <c r="H25" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="J25" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.35">
@@ -7695,7 +7714,7 @@
         <v>60</v>
       </c>
       <c r="F26" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="G26" t="s">
         <v>201</v>
@@ -7707,7 +7726,7 @@
         <v>0.01</v>
       </c>
       <c r="J26" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.35">
@@ -7727,7 +7746,7 @@
         <v>60</v>
       </c>
       <c r="F27" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="G27" t="s">
         <v>214</v>
@@ -7739,7 +7758,7 @@
         <v>0.01</v>
       </c>
       <c r="J27" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.35">
@@ -7759,7 +7778,7 @@
         <v>175</v>
       </c>
       <c r="F28" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="G28" t="s">
         <v>202</v>
@@ -7771,7 +7790,7 @@
         <v>1</v>
       </c>
       <c r="J28" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.35">
@@ -7791,7 +7810,7 @@
         <v>173</v>
       </c>
       <c r="F29" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="G29" t="s">
         <v>207</v>
@@ -7803,7 +7822,7 @@
         <v>1</v>
       </c>
       <c r="J29" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.35">
@@ -7823,11 +7842,11 @@
         <v>176</v>
       </c>
       <c r="F30" t="s">
+        <v>416</v>
+      </c>
+      <c r="G30" t="s">
         <v>417</v>
       </c>
-      <c r="G30" t="s">
-        <v>418</v>
-      </c>
       <c r="H30" t="s">
         <v>138</v>
       </c>
@@ -7835,7 +7854,7 @@
         <v>1</v>
       </c>
       <c r="J30" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.35">
@@ -7855,7 +7874,7 @@
         <v>176</v>
       </c>
       <c r="F31" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="G31" t="s">
         <v>204</v>
@@ -7867,7 +7886,7 @@
         <v>1</v>
       </c>
       <c r="J31" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.35">
@@ -7887,7 +7906,7 @@
         <v>60</v>
       </c>
       <c r="F32" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="G32" t="s">
         <v>203</v>
@@ -7899,7 +7918,7 @@
         <v>0.01</v>
       </c>
       <c r="J32" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.35">
@@ -7919,7 +7938,7 @@
         <v>60</v>
       </c>
       <c r="F33" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="G33" t="s">
         <v>205</v>
@@ -7931,7 +7950,7 @@
         <v>0.01</v>
       </c>
       <c r="J33" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
   </sheetData>
@@ -7972,7 +7991,7 @@
         <v>135</v>
       </c>
       <c r="F1" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="G1" t="s">
         <v>136</v>
@@ -7984,43 +8003,43 @@
         <v>139</v>
       </c>
       <c r="J1" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
       <c r="H2" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="J2" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="F3" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="G3" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="H3" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="J3" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="H4" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="J4" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.35">
@@ -8040,10 +8059,10 @@
         <v>60</v>
       </c>
       <c r="F5" t="s">
+        <v>423</v>
+      </c>
+      <c r="G5" t="s">
         <v>424</v>
-      </c>
-      <c r="G5" t="s">
-        <v>425</v>
       </c>
       <c r="H5" t="s">
         <v>138</v>
@@ -8052,7 +8071,7 @@
         <v>1E-3</v>
       </c>
       <c r="J5" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.35">
@@ -8072,7 +8091,7 @@
         <v>55</v>
       </c>
       <c r="F6" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="G6" t="s">
         <v>210</v>
@@ -8084,7 +8103,7 @@
         <v>1</v>
       </c>
       <c r="J6" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.35">
@@ -8104,7 +8123,7 @@
         <v>55</v>
       </c>
       <c r="F7" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="G7" t="s">
         <v>211</v>
@@ -8116,7 +8135,7 @@
         <v>1</v>
       </c>
       <c r="J7" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.35">
@@ -8136,7 +8155,7 @@
         <v>13</v>
       </c>
       <c r="F8" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="G8" t="s">
         <v>212</v>
@@ -8148,7 +8167,7 @@
         <v>1</v>
       </c>
       <c r="J8" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.35">
@@ -8168,7 +8187,7 @@
         <v>13</v>
       </c>
       <c r="F9" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="G9" t="s">
         <v>213</v>
@@ -8180,27 +8199,27 @@
         <v>1</v>
       </c>
       <c r="J9" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="H10" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="J10" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="H11" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="J11" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.35">
@@ -8220,7 +8239,7 @@
         <v>60</v>
       </c>
       <c r="F12" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="G12" t="s">
         <v>216</v>
@@ -8232,7 +8251,7 @@
         <v>0.01</v>
       </c>
       <c r="J12" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.35">
@@ -8252,7 +8271,7 @@
         <v>60</v>
       </c>
       <c r="F13" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="G13" t="s">
         <v>215</v>
@@ -8264,7 +8283,7 @@
         <v>1E-3</v>
       </c>
       <c r="J13" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.35">
@@ -8284,7 +8303,7 @@
         <v>60</v>
       </c>
       <c r="F14" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="G14" t="s">
         <v>221</v>
@@ -8296,43 +8315,43 @@
         <v>1E-3</v>
       </c>
       <c r="J14" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
       <c r="H15" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="J15" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
       <c r="F16" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="G16" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="H16" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="J16" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
       <c r="H17" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="J17" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.35">
@@ -8352,7 +8371,7 @@
         <v>60</v>
       </c>
       <c r="F18" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="G18" t="s">
         <v>222</v>
@@ -8364,7 +8383,7 @@
         <v>0.01</v>
       </c>
       <c r="J18" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.35">
@@ -8384,7 +8403,7 @@
         <v>79</v>
       </c>
       <c r="F19" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="G19" t="s">
         <v>220</v>
@@ -8396,7 +8415,7 @@
         <v>1</v>
       </c>
       <c r="J19" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.35">
@@ -8416,7 +8435,7 @@
         <v>79</v>
       </c>
       <c r="F20" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="G20" t="s">
         <v>219</v>
@@ -8428,7 +8447,7 @@
         <v>1</v>
       </c>
       <c r="J20" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.35">
@@ -8448,7 +8467,7 @@
         <v>13</v>
       </c>
       <c r="F21" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="G21" t="s">
         <v>217</v>
@@ -8460,7 +8479,7 @@
         <v>1</v>
       </c>
       <c r="J21" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.35">
@@ -8480,7 +8499,7 @@
         <v>13</v>
       </c>
       <c r="F22" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="G22" t="s">
         <v>218</v>
@@ -8492,27 +8511,27 @@
         <v>1</v>
       </c>
       <c r="J22" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
       <c r="H23" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="J23" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
       <c r="H24" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="J24" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.35">
@@ -8532,7 +8551,7 @@
         <v>60</v>
       </c>
       <c r="F25" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="G25" t="s">
         <v>208</v>
@@ -8544,7 +8563,7 @@
         <v>0.01</v>
       </c>
       <c r="J25" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.35">
@@ -8564,7 +8583,7 @@
         <v>55</v>
       </c>
       <c r="F26" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="G26" t="s">
         <v>209</v>
@@ -8576,7 +8595,7 @@
         <v>1</v>
       </c>
       <c r="J26" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
   </sheetData>
@@ -8619,7 +8638,7 @@
         <v>135</v>
       </c>
       <c r="F1" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="G1" t="s">
         <v>136</v>
@@ -8631,7 +8650,7 @@
         <v>139</v>
       </c>
       <c r="J1" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.35">
@@ -8651,7 +8670,7 @@
         <v>171</v>
       </c>
       <c r="F2" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="G2" t="s">
         <v>223</v>
@@ -8663,7 +8682,7 @@
         <v>1</v>
       </c>
       <c r="J2" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
In the UI, the generic concept "nuts/fruit" has substituted the more specific "walnut", in order to show people that this model can be used for any dual-purpose (food and timber) tree
</commit_message>
<xml_diff>
--- a/data/Walnut_grain_veg_tub.xlsx
+++ b/data/Walnut_grain_veg_tub.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mjimenez\Documents\ReForest\Living Labs for Mitigating Climate Change in Agriculture\DualPurpose_Trees\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4435E1BD-B3C2-4CA4-B2AC-51D2F79711C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06417455-764A-4C7D-86E9-0B56CE35ED1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" firstSheet="6" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" firstSheet="5" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sheet_names" sheetId="17" r:id="rId1"/>
@@ -802,9 +802,6 @@
     <t>horizontal line</t>
   </si>
   <si>
-    <t>Walnut yield model</t>
-  </si>
-  <si>
     <t>Tree impact on alley crop yield</t>
   </si>
   <si>
@@ -1427,6 +1424,9 @@
   </si>
   <si>
     <t>The income received by the farmer for one tone of certified CO2 sequestration [t CO2eq]</t>
+  </si>
+  <si>
+    <t>Nuts/fruit yield model</t>
   </si>
 </sst>
 </file>
@@ -2293,7 +2293,7 @@
         <v>158</v>
       </c>
       <c r="B1" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
@@ -2301,7 +2301,7 @@
         <v>159</v>
       </c>
       <c r="B2" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
@@ -2309,7 +2309,7 @@
         <v>163</v>
       </c>
       <c r="B3" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
@@ -2317,7 +2317,7 @@
         <v>164</v>
       </c>
       <c r="B4" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
@@ -2325,7 +2325,7 @@
         <v>160</v>
       </c>
       <c r="B5" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
@@ -2333,7 +2333,7 @@
         <v>167</v>
       </c>
       <c r="B6" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
@@ -2341,7 +2341,7 @@
         <v>165</v>
       </c>
       <c r="B7" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
@@ -2349,7 +2349,7 @@
         <v>166</v>
       </c>
       <c r="B8" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
@@ -2357,7 +2357,7 @@
         <v>168</v>
       </c>
       <c r="B9" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
@@ -2365,7 +2365,7 @@
         <v>169</v>
       </c>
       <c r="B10" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
@@ -2373,7 +2373,7 @@
         <v>161</v>
       </c>
       <c r="B11" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
@@ -2381,7 +2381,7 @@
         <v>170</v>
       </c>
       <c r="B12" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
@@ -2389,7 +2389,7 @@
         <v>162</v>
       </c>
       <c r="B13" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
   </sheetData>
@@ -2402,8 +2402,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E807E7F-DCAE-400C-B9F4-3C0EDF692711}">
   <dimension ref="A1:J5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="D1" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2432,7 +2432,7 @@
         <v>135</v>
       </c>
       <c r="F1" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="G1" t="s">
         <v>136</v>
@@ -2464,7 +2464,7 @@
         <v>171</v>
       </c>
       <c r="F2" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="G2" t="s">
         <v>227</v>
@@ -2476,7 +2476,7 @@
         <v>1</v>
       </c>
       <c r="J2" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.35">
@@ -2496,7 +2496,7 @@
         <v>55</v>
       </c>
       <c r="F3" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="G3" t="s">
         <v>225</v>
@@ -2508,7 +2508,7 @@
         <v>1</v>
       </c>
       <c r="J3" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.35">
@@ -2528,7 +2528,7 @@
         <v>60</v>
       </c>
       <c r="F4" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="G4" t="s">
         <v>224</v>
@@ -2540,7 +2540,7 @@
         <v>1E-3</v>
       </c>
       <c r="J4" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.35">
@@ -2560,7 +2560,7 @@
         <v>171</v>
       </c>
       <c r="F5" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="G5" t="s">
         <v>226</v>
@@ -2572,7 +2572,7 @@
         <v>1</v>
       </c>
       <c r="J5" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
   </sheetData>
@@ -2584,7 +2584,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{724F1830-3430-4657-920D-E95506196AA8}">
   <dimension ref="A1:J29"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="B19" workbookViewId="0">
+      <selection activeCell="B19" sqref="A1:XFD1048576"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -2610,7 +2612,7 @@
         <v>135</v>
       </c>
       <c r="F1" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="G1" t="s">
         <v>136</v>
@@ -2642,10 +2644,10 @@
         <v>105</v>
       </c>
       <c r="F2" t="s">
+        <v>441</v>
+      </c>
+      <c r="G2" t="s">
         <v>442</v>
-      </c>
-      <c r="G2" t="s">
-        <v>443</v>
       </c>
       <c r="H2" t="s">
         <v>138</v>
@@ -2674,7 +2676,7 @@
         <v>60</v>
       </c>
       <c r="F3" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="G3" t="s">
         <v>240</v>
@@ -2693,26 +2695,26 @@
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="H4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="J4" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
       <c r="F5" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="G5" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="H5" t="s">
         <v>254</v>
       </c>
       <c r="J5" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.35">
@@ -2722,7 +2724,7 @@
         <v>255</v>
       </c>
       <c r="J6" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.35">
@@ -2742,7 +2744,7 @@
         <v>60</v>
       </c>
       <c r="F7" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="G7" t="s">
         <v>233</v>
@@ -2774,7 +2776,7 @@
         <v>60</v>
       </c>
       <c r="F8" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="G8" t="s">
         <v>234</v>
@@ -2832,10 +2834,10 @@
         <v>110</v>
       </c>
       <c r="F10" t="s">
+        <v>445</v>
+      </c>
+      <c r="G10" t="s">
         <v>446</v>
-      </c>
-      <c r="G10" t="s">
-        <v>447</v>
       </c>
       <c r="H10" t="s">
         <v>138</v>
@@ -2848,7 +2850,7 @@
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="H11" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="J11" t="s">
         <v>252</v>
@@ -2858,10 +2860,10 @@
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="F12" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="G12" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="H12" t="s">
         <v>254</v>
@@ -2897,7 +2899,7 @@
         <v>38</v>
       </c>
       <c r="F14" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="G14" t="s">
         <v>239</v>
@@ -2929,7 +2931,7 @@
         <v>38</v>
       </c>
       <c r="F15" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="G15" t="s">
         <v>238</v>
@@ -2961,7 +2963,7 @@
         <v>115</v>
       </c>
       <c r="F16" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="G16" t="s">
         <v>237</v>
@@ -2993,7 +2995,7 @@
         <v>115</v>
       </c>
       <c r="F17" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="G17" t="s">
         <v>236</v>
@@ -3025,10 +3027,10 @@
         <v>110</v>
       </c>
       <c r="F18" t="s">
+        <v>452</v>
+      </c>
+      <c r="G18" t="s">
         <v>453</v>
-      </c>
-      <c r="G18" t="s">
-        <v>454</v>
       </c>
       <c r="H18" t="s">
         <v>138</v>
@@ -3054,10 +3056,10 @@
         <v>110</v>
       </c>
       <c r="F19" t="s">
+        <v>454</v>
+      </c>
+      <c r="G19" t="s">
         <v>455</v>
-      </c>
-      <c r="G19" t="s">
-        <v>456</v>
       </c>
       <c r="H19" t="s">
         <v>138</v>
@@ -3083,7 +3085,7 @@
         <v>120</v>
       </c>
       <c r="F20" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="G20" t="s">
         <v>245</v>
@@ -3115,7 +3117,7 @@
         <v>60</v>
       </c>
       <c r="F21" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="G21" t="s">
         <v>241</v>
@@ -3147,7 +3149,7 @@
         <v>60</v>
       </c>
       <c r="F22" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="G22" t="s">
         <v>242</v>
@@ -3179,7 +3181,7 @@
         <v>122</v>
       </c>
       <c r="F23" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="G23" t="s">
         <v>246</v>
@@ -3208,7 +3210,7 @@
         <v>13</v>
       </c>
       <c r="F24" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="G24" t="s">
         <v>243</v>
@@ -3237,7 +3239,7 @@
         <v>60</v>
       </c>
       <c r="F25" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="G25" t="s">
         <v>244</v>
@@ -3260,7 +3262,7 @@
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
       <c r="H27" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.35">
@@ -3281,7 +3283,7 @@
   <dimension ref="A1:J122"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
+      <selection activeCell="C1" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3308,7 +3310,7 @@
         <v>135</v>
       </c>
       <c r="F1" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="G1" t="s">
         <v>136</v>
@@ -3340,11 +3342,11 @@
         <v>172</v>
       </c>
       <c r="F2" t="s">
+        <v>462</v>
+      </c>
+      <c r="G2" t="s">
         <v>463</v>
       </c>
-      <c r="G2" t="s">
-        <v>464</v>
-      </c>
       <c r="H2" t="s">
         <v>138</v>
       </c>
@@ -3352,7 +3354,7 @@
         <v>1</v>
       </c>
       <c r="J2" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.35">
@@ -3845,7 +3847,7 @@
   <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:F5"/>
+      <selection activeCell="D1" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3980,7 +3982,7 @@
         <v>1</v>
       </c>
       <c r="J4" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.35">
@@ -4012,7 +4014,7 @@
         <v>1</v>
       </c>
       <c r="J5" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
   </sheetData>
@@ -4025,15 +4027,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06826C72-96B8-4DB0-B8A1-5FBF5F35F3F2}">
   <dimension ref="A1:J121"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B1" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="36.7265625" customWidth="1"/>
     <col min="2" max="3" width="10.453125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="55.453125" customWidth="1"/>
+    <col min="6" max="6" width="31.90625" customWidth="1"/>
+    <col min="7" max="7" width="30.453125" customWidth="1"/>
     <col min="9" max="9" width="18.453125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -4054,7 +4057,7 @@
         <v>135</v>
       </c>
       <c r="F1" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="G1" t="s">
         <v>136</v>
@@ -4086,10 +4089,10 @@
         <v>8</v>
       </c>
       <c r="F2" t="s">
+        <v>287</v>
+      </c>
+      <c r="G2" t="s">
         <v>288</v>
-      </c>
-      <c r="G2" t="s">
-        <v>289</v>
       </c>
       <c r="H2" t="s">
         <v>140</v>
@@ -4118,10 +4121,10 @@
         <v>13</v>
       </c>
       <c r="F3" t="s">
+        <v>289</v>
+      </c>
+      <c r="G3" t="s">
         <v>290</v>
-      </c>
-      <c r="G3" t="s">
-        <v>291</v>
       </c>
       <c r="H3" t="s">
         <v>138</v>
@@ -4150,10 +4153,10 @@
         <v>55</v>
       </c>
       <c r="F4" t="s">
+        <v>291</v>
+      </c>
+      <c r="G4" t="s">
         <v>292</v>
-      </c>
-      <c r="G4" t="s">
-        <v>293</v>
       </c>
       <c r="H4" t="s">
         <v>140</v>
@@ -4182,10 +4185,10 @@
         <v>55</v>
       </c>
       <c r="F5" t="s">
+        <v>293</v>
+      </c>
+      <c r="G5" t="s">
         <v>294</v>
-      </c>
-      <c r="G5" t="s">
-        <v>295</v>
       </c>
       <c r="H5" t="s">
         <v>140</v>
@@ -4214,7 +4217,7 @@
         <v>6</v>
       </c>
       <c r="F6" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="G6" t="s">
         <v>179</v>
@@ -4246,10 +4249,10 @@
         <v>13</v>
       </c>
       <c r="F7" t="s">
+        <v>296</v>
+      </c>
+      <c r="G7" t="s">
         <v>297</v>
-      </c>
-      <c r="G7" t="s">
-        <v>298</v>
       </c>
       <c r="H7" t="s">
         <v>138</v>
@@ -4726,7 +4729,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B046A6C-AF4B-434A-AE31-2F62785AB96F}">
   <dimension ref="A1:K118"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:J5"/>
     </sheetView>
   </sheetViews>
@@ -4754,7 +4757,7 @@
         <v>135</v>
       </c>
       <c r="F1" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="G1" t="s">
         <v>136</v>
@@ -4786,10 +4789,10 @@
         <v>10</v>
       </c>
       <c r="F2" t="s">
+        <v>298</v>
+      </c>
+      <c r="G2" t="s">
         <v>299</v>
-      </c>
-      <c r="G2" t="s">
-        <v>300</v>
       </c>
       <c r="H2" t="s">
         <v>140</v>
@@ -4818,10 +4821,10 @@
         <v>10</v>
       </c>
       <c r="F3" t="s">
+        <v>300</v>
+      </c>
+      <c r="G3" t="s">
         <v>301</v>
-      </c>
-      <c r="G3" t="s">
-        <v>302</v>
       </c>
       <c r="H3" t="s">
         <v>140</v>
@@ -4851,10 +4854,10 @@
         <v>18</v>
       </c>
       <c r="F4" t="s">
+        <v>302</v>
+      </c>
+      <c r="G4" t="s">
         <v>303</v>
-      </c>
-      <c r="G4" t="s">
-        <v>304</v>
       </c>
       <c r="H4" t="s">
         <v>140</v>
@@ -4883,10 +4886,10 @@
         <v>10</v>
       </c>
       <c r="F5" t="s">
+        <v>304</v>
+      </c>
+      <c r="G5" t="s">
         <v>305</v>
-      </c>
-      <c r="G5" t="s">
-        <v>306</v>
       </c>
       <c r="H5" t="s">
         <v>140</v>
@@ -5360,7 +5363,7 @@
   <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:L4"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5389,7 +5392,7 @@
         <v>135</v>
       </c>
       <c r="F1" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="G1" t="s">
         <v>136</v>
@@ -5421,11 +5424,11 @@
         <v>178</v>
       </c>
       <c r="F2" t="s">
+        <v>306</v>
+      </c>
+      <c r="G2" t="s">
         <v>307</v>
       </c>
-      <c r="G2" t="s">
-        <v>308</v>
-      </c>
       <c r="H2" t="s">
         <v>138</v>
       </c>
@@ -5433,7 +5436,7 @@
         <v>1</v>
       </c>
       <c r="J2" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.35">
@@ -5453,11 +5456,11 @@
         <v>171</v>
       </c>
       <c r="F3" t="s">
+        <v>308</v>
+      </c>
+      <c r="G3" t="s">
         <v>309</v>
       </c>
-      <c r="G3" t="s">
-        <v>310</v>
-      </c>
       <c r="H3" t="s">
         <v>138</v>
       </c>
@@ -5465,7 +5468,7 @@
         <v>1</v>
       </c>
       <c r="J3" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.35">
@@ -5485,11 +5488,11 @@
         <v>171</v>
       </c>
       <c r="F4" t="s">
+        <v>310</v>
+      </c>
+      <c r="G4" t="s">
         <v>311</v>
       </c>
-      <c r="G4" t="s">
-        <v>312</v>
-      </c>
       <c r="H4" t="s">
         <v>138</v>
       </c>
@@ -5497,7 +5500,7 @@
         <v>1</v>
       </c>
       <c r="J4" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
   </sheetData>
@@ -5509,8 +5512,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8D4214A-8AE9-4396-ABE5-C95E3D310602}">
   <dimension ref="A1:J27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:J26"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A24" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5540,7 +5543,7 @@
         <v>135</v>
       </c>
       <c r="F1" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="G1" t="s">
         <v>136</v>
@@ -5572,10 +5575,10 @@
         <v>177</v>
       </c>
       <c r="F2" t="s">
+        <v>312</v>
+      </c>
+      <c r="G2" t="s">
         <v>313</v>
-      </c>
-      <c r="G2" t="s">
-        <v>314</v>
       </c>
       <c r="H2" t="s">
         <v>138</v>
@@ -5604,10 +5607,10 @@
         <v>180</v>
       </c>
       <c r="F3" t="s">
+        <v>314</v>
+      </c>
+      <c r="G3" t="s">
         <v>315</v>
-      </c>
-      <c r="G3" t="s">
-        <v>316</v>
       </c>
       <c r="H3" t="s">
         <v>138</v>
@@ -5636,10 +5639,10 @@
         <v>180</v>
       </c>
       <c r="F4" t="s">
+        <v>316</v>
+      </c>
+      <c r="G4" t="s">
         <v>317</v>
-      </c>
-      <c r="G4" t="s">
-        <v>318</v>
       </c>
       <c r="H4" t="s">
         <v>138</v>
@@ -5668,10 +5671,10 @@
         <v>180</v>
       </c>
       <c r="F5" t="s">
+        <v>318</v>
+      </c>
+      <c r="G5" t="s">
         <v>319</v>
-      </c>
-      <c r="G5" t="s">
-        <v>320</v>
       </c>
       <c r="H5" t="s">
         <v>138</v>
@@ -5700,10 +5703,10 @@
         <v>180</v>
       </c>
       <c r="F6" t="s">
+        <v>320</v>
+      </c>
+      <c r="G6" t="s">
         <v>321</v>
-      </c>
-      <c r="G6" t="s">
-        <v>322</v>
       </c>
       <c r="H6" t="s">
         <v>138</v>
@@ -5732,10 +5735,10 @@
         <v>180</v>
       </c>
       <c r="F7" t="s">
+        <v>322</v>
+      </c>
+      <c r="G7" t="s">
         <v>323</v>
-      </c>
-      <c r="G7" t="s">
-        <v>324</v>
       </c>
       <c r="H7" t="s">
         <v>138</v>
@@ -5764,10 +5767,10 @@
         <v>180</v>
       </c>
       <c r="F8" t="s">
+        <v>324</v>
+      </c>
+      <c r="G8" t="s">
         <v>325</v>
-      </c>
-      <c r="G8" t="s">
-        <v>326</v>
       </c>
       <c r="H8" t="s">
         <v>138</v>
@@ -5796,10 +5799,10 @@
         <v>180</v>
       </c>
       <c r="F9" t="s">
+        <v>326</v>
+      </c>
+      <c r="G9" t="s">
         <v>327</v>
-      </c>
-      <c r="G9" t="s">
-        <v>328</v>
       </c>
       <c r="H9" t="s">
         <v>138</v>
@@ -5828,10 +5831,10 @@
         <v>60</v>
       </c>
       <c r="F10" t="s">
+        <v>328</v>
+      </c>
+      <c r="G10" t="s">
         <v>329</v>
-      </c>
-      <c r="G10" t="s">
-        <v>330</v>
       </c>
       <c r="H10" t="s">
         <v>138</v>
@@ -5860,11 +5863,11 @@
         <v>24</v>
       </c>
       <c r="F11" t="s">
+        <v>330</v>
+      </c>
+      <c r="G11" t="s">
         <v>331</v>
       </c>
-      <c r="G11" t="s">
-        <v>332</v>
-      </c>
       <c r="H11" t="s">
         <v>138</v>
       </c>
@@ -5872,7 +5875,7 @@
         <v>1</v>
       </c>
       <c r="J11" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.35">
@@ -5892,11 +5895,11 @@
         <v>181</v>
       </c>
       <c r="F12" t="s">
+        <v>332</v>
+      </c>
+      <c r="G12" t="s">
         <v>333</v>
       </c>
-      <c r="G12" t="s">
-        <v>334</v>
-      </c>
       <c r="H12" t="s">
         <v>138</v>
       </c>
@@ -5904,7 +5907,7 @@
         <v>1</v>
       </c>
       <c r="J12" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.35">
@@ -5924,10 +5927,10 @@
         <v>28</v>
       </c>
       <c r="F13" t="s">
+        <v>334</v>
+      </c>
+      <c r="G13" t="s">
         <v>335</v>
-      </c>
-      <c r="G13" t="s">
-        <v>336</v>
       </c>
       <c r="H13" t="s">
         <v>138</v>
@@ -5956,10 +5959,10 @@
         <v>30</v>
       </c>
       <c r="F14" t="s">
+        <v>336</v>
+      </c>
+      <c r="G14" t="s">
         <v>337</v>
-      </c>
-      <c r="G14" t="s">
-        <v>338</v>
       </c>
       <c r="H14" t="s">
         <v>138</v>
@@ -5988,10 +5991,10 @@
         <v>24</v>
       </c>
       <c r="F15" t="s">
+        <v>338</v>
+      </c>
+      <c r="G15" t="s">
         <v>339</v>
-      </c>
-      <c r="G15" t="s">
-        <v>340</v>
       </c>
       <c r="H15" t="s">
         <v>138</v>
@@ -6020,10 +6023,10 @@
         <v>28</v>
       </c>
       <c r="F16" t="s">
+        <v>340</v>
+      </c>
+      <c r="G16" t="s">
         <v>341</v>
-      </c>
-      <c r="G16" t="s">
-        <v>342</v>
       </c>
       <c r="H16" t="s">
         <v>138</v>
@@ -6052,10 +6055,10 @@
         <v>180</v>
       </c>
       <c r="F17" t="s">
+        <v>342</v>
+      </c>
+      <c r="G17" t="s">
         <v>343</v>
-      </c>
-      <c r="G17" t="s">
-        <v>344</v>
       </c>
       <c r="H17" t="s">
         <v>138</v>
@@ -6084,10 +6087,10 @@
         <v>30</v>
       </c>
       <c r="F18" t="s">
+        <v>344</v>
+      </c>
+      <c r="G18" t="s">
         <v>345</v>
-      </c>
-      <c r="G18" t="s">
-        <v>346</v>
       </c>
       <c r="H18" t="s">
         <v>138</v>
@@ -6116,10 +6119,10 @@
         <v>30</v>
       </c>
       <c r="F19" t="s">
+        <v>346</v>
+      </c>
+      <c r="G19" t="s">
         <v>347</v>
-      </c>
-      <c r="G19" t="s">
-        <v>348</v>
       </c>
       <c r="H19" t="s">
         <v>138</v>
@@ -6148,10 +6151,10 @@
         <v>99</v>
       </c>
       <c r="F20" t="s">
+        <v>348</v>
+      </c>
+      <c r="G20" t="s">
         <v>349</v>
-      </c>
-      <c r="G20" t="s">
-        <v>350</v>
       </c>
       <c r="H20" t="s">
         <v>138</v>
@@ -6160,7 +6163,7 @@
         <v>1E-3</v>
       </c>
       <c r="J20" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.35">
@@ -6180,10 +6183,10 @@
         <v>30</v>
       </c>
       <c r="F21" t="s">
+        <v>350</v>
+      </c>
+      <c r="G21" t="s">
         <v>351</v>
-      </c>
-      <c r="G21" t="s">
-        <v>352</v>
       </c>
       <c r="H21" t="s">
         <v>138</v>
@@ -6192,7 +6195,7 @@
         <v>1E-4</v>
       </c>
       <c r="J21" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.35">
@@ -6212,10 +6215,10 @@
         <v>28</v>
       </c>
       <c r="F22" t="s">
+        <v>352</v>
+      </c>
+      <c r="G22" t="s">
         <v>353</v>
-      </c>
-      <c r="G22" t="s">
-        <v>354</v>
       </c>
       <c r="H22" t="s">
         <v>138</v>
@@ -6224,7 +6227,7 @@
         <v>0.01</v>
       </c>
       <c r="J22" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.35">
@@ -6244,11 +6247,11 @@
         <v>174</v>
       </c>
       <c r="F23" t="s">
+        <v>354</v>
+      </c>
+      <c r="G23" t="s">
         <v>355</v>
       </c>
-      <c r="G23" t="s">
-        <v>356</v>
-      </c>
       <c r="H23" t="s">
         <v>138</v>
       </c>
@@ -6256,7 +6259,7 @@
         <v>1</v>
       </c>
       <c r="J23" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.35">
@@ -6276,11 +6279,11 @@
         <v>174</v>
       </c>
       <c r="F24" t="s">
+        <v>356</v>
+      </c>
+      <c r="G24" t="s">
         <v>357</v>
       </c>
-      <c r="G24" t="s">
-        <v>358</v>
-      </c>
       <c r="H24" t="s">
         <v>138</v>
       </c>
@@ -6288,7 +6291,7 @@
         <v>1</v>
       </c>
       <c r="J24" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.35">
@@ -6308,10 +6311,10 @@
         <v>24</v>
       </c>
       <c r="F25" t="s">
+        <v>358</v>
+      </c>
+      <c r="G25" t="s">
         <v>359</v>
-      </c>
-      <c r="G25" t="s">
-        <v>360</v>
       </c>
       <c r="H25" t="s">
         <v>138</v>
@@ -6340,10 +6343,10 @@
         <v>60</v>
       </c>
       <c r="F26" t="s">
+        <v>360</v>
+      </c>
+      <c r="G26" t="s">
         <v>361</v>
-      </c>
-      <c r="G26" t="s">
-        <v>362</v>
       </c>
       <c r="H26" t="s">
         <v>138</v>
@@ -6368,7 +6371,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C0D7C64-12CB-4A85-A4CD-D098869794C1}">
   <dimension ref="A1:J22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <selection sqref="A1:K22"/>
     </sheetView>
   </sheetViews>
@@ -6397,7 +6400,7 @@
         <v>135</v>
       </c>
       <c r="F1" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="G1" t="s">
         <v>136</v>
@@ -6429,10 +6432,10 @@
         <v>174</v>
       </c>
       <c r="F2" t="s">
+        <v>362</v>
+      </c>
+      <c r="G2" t="s">
         <v>363</v>
-      </c>
-      <c r="G2" t="s">
-        <v>364</v>
       </c>
       <c r="H2" t="s">
         <v>138</v>
@@ -6461,7 +6464,7 @@
         <v>38</v>
       </c>
       <c r="F3" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="G3" t="s">
         <v>182</v>
@@ -6493,11 +6496,11 @@
         <v>173</v>
       </c>
       <c r="F4" t="s">
+        <v>365</v>
+      </c>
+      <c r="G4" t="s">
         <v>366</v>
       </c>
-      <c r="G4" t="s">
-        <v>367</v>
-      </c>
       <c r="H4" t="s">
         <v>138</v>
       </c>
@@ -6505,7 +6508,7 @@
         <v>1</v>
       </c>
       <c r="J4" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.35">
@@ -6525,7 +6528,7 @@
         <v>174</v>
       </c>
       <c r="F5" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="G5" t="s">
         <v>186</v>
@@ -6557,7 +6560,7 @@
         <v>38</v>
       </c>
       <c r="F6" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="G6" t="s">
         <v>183</v>
@@ -6589,7 +6592,7 @@
         <v>173</v>
       </c>
       <c r="F7" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="G7" t="s">
         <v>184</v>
@@ -6601,7 +6604,7 @@
         <v>1</v>
       </c>
       <c r="J7" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.35">
@@ -6621,10 +6624,10 @@
         <v>174</v>
       </c>
       <c r="F8" t="s">
+        <v>370</v>
+      </c>
+      <c r="G8" t="s">
         <v>371</v>
-      </c>
-      <c r="G8" t="s">
-        <v>372</v>
       </c>
       <c r="H8" t="s">
         <v>138</v>
@@ -6653,7 +6656,7 @@
         <v>38</v>
       </c>
       <c r="F9" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="G9" t="s">
         <v>185</v>
@@ -6685,11 +6688,11 @@
         <v>173</v>
       </c>
       <c r="F10" t="s">
+        <v>373</v>
+      </c>
+      <c r="G10" t="s">
         <v>374</v>
       </c>
-      <c r="G10" t="s">
-        <v>375</v>
-      </c>
       <c r="H10" t="s">
         <v>138</v>
       </c>
@@ -6697,7 +6700,7 @@
         <v>1</v>
       </c>
       <c r="J10" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.35">
@@ -6717,10 +6720,10 @@
         <v>174</v>
       </c>
       <c r="F11" t="s">
+        <v>375</v>
+      </c>
+      <c r="G11" t="s">
         <v>376</v>
-      </c>
-      <c r="G11" t="s">
-        <v>377</v>
       </c>
       <c r="H11" t="s">
         <v>138</v>
@@ -6749,10 +6752,10 @@
         <v>38</v>
       </c>
       <c r="F12" t="s">
+        <v>377</v>
+      </c>
+      <c r="G12" t="s">
         <v>378</v>
-      </c>
-      <c r="G12" t="s">
-        <v>379</v>
       </c>
       <c r="H12" t="s">
         <v>138</v>
@@ -6781,11 +6784,11 @@
         <v>173</v>
       </c>
       <c r="F13" t="s">
+        <v>379</v>
+      </c>
+      <c r="G13" t="s">
         <v>380</v>
       </c>
-      <c r="G13" t="s">
-        <v>381</v>
-      </c>
       <c r="H13" t="s">
         <v>138</v>
       </c>
@@ -6793,7 +6796,7 @@
         <v>1</v>
       </c>
       <c r="J13" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.35">
@@ -6813,10 +6816,10 @@
         <v>174</v>
       </c>
       <c r="F14" t="s">
+        <v>381</v>
+      </c>
+      <c r="G14" t="s">
         <v>382</v>
-      </c>
-      <c r="G14" t="s">
-        <v>383</v>
       </c>
       <c r="H14" t="s">
         <v>138</v>
@@ -6845,7 +6848,7 @@
         <v>38</v>
       </c>
       <c r="F15" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="G15" t="s">
         <v>187</v>
@@ -6877,11 +6880,11 @@
         <v>173</v>
       </c>
       <c r="F16" t="s">
+        <v>384</v>
+      </c>
+      <c r="G16" t="s">
         <v>385</v>
       </c>
-      <c r="G16" t="s">
-        <v>386</v>
-      </c>
       <c r="H16" t="s">
         <v>138</v>
       </c>
@@ -6889,7 +6892,7 @@
         <v>1</v>
       </c>
       <c r="J16" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.35">
@@ -6909,10 +6912,10 @@
         <v>174</v>
       </c>
       <c r="F17" t="s">
+        <v>386</v>
+      </c>
+      <c r="G17" t="s">
         <v>387</v>
-      </c>
-      <c r="G17" t="s">
-        <v>388</v>
       </c>
       <c r="H17" t="s">
         <v>138</v>
@@ -6941,7 +6944,7 @@
         <v>38</v>
       </c>
       <c r="F18" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="G18" t="s">
         <v>188</v>
@@ -6973,11 +6976,11 @@
         <v>173</v>
       </c>
       <c r="F19" t="s">
+        <v>389</v>
+      </c>
+      <c r="G19" t="s">
         <v>390</v>
       </c>
-      <c r="G19" t="s">
-        <v>391</v>
-      </c>
       <c r="H19" t="s">
         <v>138</v>
       </c>
@@ -6985,7 +6988,7 @@
         <v>1</v>
       </c>
       <c r="J19" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.35">
@@ -7005,10 +7008,10 @@
         <v>174</v>
       </c>
       <c r="F20" t="s">
+        <v>391</v>
+      </c>
+      <c r="G20" t="s">
         <v>392</v>
-      </c>
-      <c r="G20" t="s">
-        <v>393</v>
       </c>
       <c r="H20" t="s">
         <v>138</v>
@@ -7037,7 +7040,7 @@
         <v>38</v>
       </c>
       <c r="F21" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="G21" t="s">
         <v>189</v>
@@ -7069,11 +7072,11 @@
         <v>173</v>
       </c>
       <c r="F22" t="s">
+        <v>394</v>
+      </c>
+      <c r="G22" t="s">
         <v>395</v>
       </c>
-      <c r="G22" t="s">
-        <v>396</v>
-      </c>
       <c r="H22" t="s">
         <v>138</v>
       </c>
@@ -7081,7 +7084,7 @@
         <v>1</v>
       </c>
       <c r="J22" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
   </sheetData>
@@ -7093,8 +7096,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5B46F03-BBFE-4EF0-AFCA-0F4C3592A7D1}">
   <dimension ref="A1:J33"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -7122,7 +7125,7 @@
         <v>135</v>
       </c>
       <c r="F1" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="G1" t="s">
         <v>136</v>
@@ -7141,10 +7144,10 @@
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
       <c r="H2" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="J2" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.35">
@@ -7160,7 +7163,7 @@
         <v>254</v>
       </c>
       <c r="J3" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.35">
@@ -7170,7 +7173,7 @@
         <v>255</v>
       </c>
       <c r="J4" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.35">
@@ -7190,7 +7193,7 @@
         <v>77</v>
       </c>
       <c r="F5" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="G5" t="s">
         <v>190</v>
@@ -7202,7 +7205,7 @@
         <v>1</v>
       </c>
       <c r="J5" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.35">
@@ -7222,7 +7225,7 @@
         <v>79</v>
       </c>
       <c r="F6" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="G6" t="s">
         <v>191</v>
@@ -7234,7 +7237,7 @@
         <v>1</v>
       </c>
       <c r="J6" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.35">
@@ -7254,7 +7257,7 @@
         <v>79</v>
       </c>
       <c r="F7" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="G7" t="s">
         <v>192</v>
@@ -7266,7 +7269,7 @@
         <v>1</v>
       </c>
       <c r="J7" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.35">
@@ -7286,7 +7289,7 @@
         <v>13</v>
       </c>
       <c r="F8" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="G8" t="s">
         <v>193</v>
@@ -7298,7 +7301,7 @@
         <v>1</v>
       </c>
       <c r="J8" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.35">
@@ -7318,7 +7321,7 @@
         <v>13</v>
       </c>
       <c r="F9" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="G9" t="s">
         <v>194</v>
@@ -7330,7 +7333,7 @@
         <v>1</v>
       </c>
       <c r="J9" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.35">
@@ -7340,17 +7343,17 @@
         <v>255</v>
       </c>
       <c r="J10" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="H11" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="J11" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.35">
@@ -7370,7 +7373,7 @@
         <v>79</v>
       </c>
       <c r="F12" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="G12" t="s">
         <v>195</v>
@@ -7382,7 +7385,7 @@
         <v>1</v>
       </c>
       <c r="J12" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.35">
@@ -7402,7 +7405,7 @@
         <v>79</v>
       </c>
       <c r="F13" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="G13" t="s">
         <v>235</v>
@@ -7414,7 +7417,7 @@
         <v>1</v>
       </c>
       <c r="J13" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.35">
@@ -7434,7 +7437,7 @@
         <v>60</v>
       </c>
       <c r="F14" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="G14" t="s">
         <v>206</v>
@@ -7446,33 +7449,33 @@
         <v>1E-3</v>
       </c>
       <c r="J14" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
       <c r="H15" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="J15" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
       <c r="F16" t="s">
-        <v>256</v>
+        <v>464</v>
       </c>
       <c r="G16" t="s">
-        <v>256</v>
+        <v>464</v>
       </c>
       <c r="H16" t="s">
         <v>254</v>
       </c>
       <c r="J16" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.35">
@@ -7482,7 +7485,7 @@
         <v>255</v>
       </c>
       <c r="J17" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.35">
@@ -7502,7 +7505,7 @@
         <v>86</v>
       </c>
       <c r="F18" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="G18" t="s">
         <v>198</v>
@@ -7514,7 +7517,7 @@
         <v>1</v>
       </c>
       <c r="J18" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.35">
@@ -7534,7 +7537,7 @@
         <v>79</v>
       </c>
       <c r="F19" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="G19" t="s">
         <v>196</v>
@@ -7546,7 +7549,7 @@
         <v>1</v>
       </c>
       <c r="J19" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.35">
@@ -7566,7 +7569,7 @@
         <v>79</v>
       </c>
       <c r="F20" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="G20" t="s">
         <v>197</v>
@@ -7578,7 +7581,7 @@
         <v>1</v>
       </c>
       <c r="J20" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.35">
@@ -7598,7 +7601,7 @@
         <v>13</v>
       </c>
       <c r="F21" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="G21" t="s">
         <v>199</v>
@@ -7610,7 +7613,7 @@
         <v>1</v>
       </c>
       <c r="J21" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.35">
@@ -7630,7 +7633,7 @@
         <v>13</v>
       </c>
       <c r="F22" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="G22" t="s">
         <v>200</v>
@@ -7642,7 +7645,7 @@
         <v>1</v>
       </c>
       <c r="J22" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.35">
@@ -7662,11 +7665,11 @@
         <v>13</v>
       </c>
       <c r="F23" t="s">
+        <v>409</v>
+      </c>
+      <c r="G23" t="s">
         <v>410</v>
       </c>
-      <c r="G23" t="s">
-        <v>411</v>
-      </c>
       <c r="H23" t="s">
         <v>138</v>
       </c>
@@ -7674,7 +7677,7 @@
         <v>1</v>
       </c>
       <c r="J23" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.35">
@@ -7684,17 +7687,17 @@
         <v>255</v>
       </c>
       <c r="J24" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
       <c r="H25" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="J25" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.35">
@@ -7714,7 +7717,7 @@
         <v>60</v>
       </c>
       <c r="F26" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="G26" t="s">
         <v>201</v>
@@ -7726,7 +7729,7 @@
         <v>0.01</v>
       </c>
       <c r="J26" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.35">
@@ -7746,7 +7749,7 @@
         <v>60</v>
       </c>
       <c r="F27" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="G27" t="s">
         <v>214</v>
@@ -7758,7 +7761,7 @@
         <v>0.01</v>
       </c>
       <c r="J27" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.35">
@@ -7778,7 +7781,7 @@
         <v>175</v>
       </c>
       <c r="F28" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="G28" t="s">
         <v>202</v>
@@ -7790,7 +7793,7 @@
         <v>1</v>
       </c>
       <c r="J28" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.35">
@@ -7810,7 +7813,7 @@
         <v>173</v>
       </c>
       <c r="F29" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="G29" t="s">
         <v>207</v>
@@ -7822,7 +7825,7 @@
         <v>1</v>
       </c>
       <c r="J29" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.35">
@@ -7842,11 +7845,11 @@
         <v>176</v>
       </c>
       <c r="F30" t="s">
+        <v>415</v>
+      </c>
+      <c r="G30" t="s">
         <v>416</v>
       </c>
-      <c r="G30" t="s">
-        <v>417</v>
-      </c>
       <c r="H30" t="s">
         <v>138</v>
       </c>
@@ -7854,7 +7857,7 @@
         <v>1</v>
       </c>
       <c r="J30" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.35">
@@ -7874,7 +7877,7 @@
         <v>176</v>
       </c>
       <c r="F31" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="G31" t="s">
         <v>204</v>
@@ -7886,7 +7889,7 @@
         <v>1</v>
       </c>
       <c r="J31" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.35">
@@ -7906,7 +7909,7 @@
         <v>60</v>
       </c>
       <c r="F32" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="G32" t="s">
         <v>203</v>
@@ -7918,7 +7921,7 @@
         <v>0.01</v>
       </c>
       <c r="J32" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.35">
@@ -7938,7 +7941,7 @@
         <v>60</v>
       </c>
       <c r="F33" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="G33" t="s">
         <v>205</v>
@@ -7950,7 +7953,7 @@
         <v>0.01</v>
       </c>
       <c r="J33" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
   </sheetData>
@@ -7962,8 +7965,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7AD55CD1-0195-43C4-85D0-979B3B5F4C61}">
   <dimension ref="A1:J26"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView topLeftCell="D16" workbookViewId="0">
+      <selection activeCell="D16" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -7991,7 +7994,7 @@
         <v>135</v>
       </c>
       <c r="F1" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="G1" t="s">
         <v>136</v>
@@ -8010,7 +8013,7 @@
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
       <c r="H2" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="J2" t="s">
         <v>249</v>
@@ -8020,10 +8023,10 @@
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="F3" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="G3" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="H3" t="s">
         <v>254</v>
@@ -8059,10 +8062,10 @@
         <v>60</v>
       </c>
       <c r="F5" t="s">
+        <v>422</v>
+      </c>
+      <c r="G5" t="s">
         <v>423</v>
-      </c>
-      <c r="G5" t="s">
-        <v>424</v>
       </c>
       <c r="H5" t="s">
         <v>138</v>
@@ -8091,7 +8094,7 @@
         <v>55</v>
       </c>
       <c r="F6" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="G6" t="s">
         <v>210</v>
@@ -8123,7 +8126,7 @@
         <v>55</v>
       </c>
       <c r="F7" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="G7" t="s">
         <v>211</v>
@@ -8155,7 +8158,7 @@
         <v>13</v>
       </c>
       <c r="F8" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="G8" t="s">
         <v>212</v>
@@ -8187,7 +8190,7 @@
         <v>13</v>
       </c>
       <c r="F9" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="G9" t="s">
         <v>213</v>
@@ -8216,7 +8219,7 @@
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="H11" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="J11" t="s">
         <v>249</v>
@@ -8239,7 +8242,7 @@
         <v>60</v>
       </c>
       <c r="F12" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="G12" t="s">
         <v>216</v>
@@ -8271,7 +8274,7 @@
         <v>60</v>
       </c>
       <c r="F13" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="G13" t="s">
         <v>215</v>
@@ -8303,7 +8306,7 @@
         <v>60</v>
       </c>
       <c r="F14" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="G14" t="s">
         <v>221</v>
@@ -8322,7 +8325,7 @@
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
       <c r="H15" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="J15" t="s">
         <v>249</v>
@@ -8332,10 +8335,10 @@
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
       <c r="F16" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="G16" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="H16" t="s">
         <v>254</v>
@@ -8371,7 +8374,7 @@
         <v>60</v>
       </c>
       <c r="F18" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="G18" t="s">
         <v>222</v>
@@ -8403,7 +8406,7 @@
         <v>79</v>
       </c>
       <c r="F19" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="G19" t="s">
         <v>220</v>
@@ -8435,7 +8438,7 @@
         <v>79</v>
       </c>
       <c r="F20" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="G20" t="s">
         <v>219</v>
@@ -8467,7 +8470,7 @@
         <v>13</v>
       </c>
       <c r="F21" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="G21" t="s">
         <v>217</v>
@@ -8499,7 +8502,7 @@
         <v>13</v>
       </c>
       <c r="F22" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="G22" t="s">
         <v>218</v>
@@ -8528,7 +8531,7 @@
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
       <c r="H24" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="J24" t="s">
         <v>249</v>
@@ -8551,7 +8554,7 @@
         <v>60</v>
       </c>
       <c r="F25" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="G25" t="s">
         <v>208</v>
@@ -8583,7 +8586,7 @@
         <v>55</v>
       </c>
       <c r="F26" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="G26" t="s">
         <v>209</v>
@@ -8609,7 +8612,7 @@
   <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD4"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -8638,7 +8641,7 @@
         <v>135</v>
       </c>
       <c r="F1" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="G1" t="s">
         <v>136</v>
@@ -8670,7 +8673,7 @@
         <v>171</v>
       </c>
       <c r="F2" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="G2" t="s">
         <v>223</v>
@@ -8682,7 +8685,7 @@
         <v>1</v>
       </c>
       <c r="J2" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added tree mortality probability
</commit_message>
<xml_diff>
--- a/data/Walnut_grain_veg_tub.xlsx
+++ b/data/Walnut_grain_veg_tub.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mjimenez\Documents\ReForest\Living Labs for Mitigating Climate Change in Agriculture\DualPurpose_Trees\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06417455-764A-4C7D-86E9-0B56CE35ED1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB983E39-DB2D-4E1D-A9A5-0C97F402633D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" firstSheet="5" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" firstSheet="5" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sheet_names" sheetId="17" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1079" uniqueCount="465">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1086" uniqueCount="468">
   <si>
     <t>variable</t>
   </si>
@@ -1427,6 +1427,15 @@
   </si>
   <si>
     <t>Nuts/fruit yield model</t>
+  </si>
+  <si>
+    <t>tree_mortality_chance</t>
+  </si>
+  <si>
+    <t>Annual probability of tree mortality</t>
+  </si>
+  <si>
+    <t>Probability of a tree to die sometime before it can be harvested, making its wood to lose value</t>
   </si>
 </sst>
 </file>
@@ -3846,7 +3855,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0AACA546-DF26-443B-AA33-3E83721C2724}">
   <dimension ref="A1:J5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+    <sheetView topLeftCell="D1" workbookViewId="0">
       <selection activeCell="D1" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
@@ -7094,10 +7103,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5B46F03-BBFE-4EF0-AFCA-0F4C3592A7D1}">
-  <dimension ref="A1:J33"/>
+  <dimension ref="A1:J34"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -7178,25 +7187,25 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>76</v>
+        <v>84</v>
       </c>
       <c r="B5" s="1">
-        <v>105</v>
+        <v>50</v>
       </c>
       <c r="C5" s="1">
-        <v>120</v>
+        <v>70</v>
       </c>
       <c r="D5" t="s">
         <v>12</v>
       </c>
       <c r="E5" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="F5" t="s">
-        <v>396</v>
+        <v>402</v>
       </c>
       <c r="G5" t="s">
-        <v>190</v>
+        <v>235</v>
       </c>
       <c r="H5" t="s">
         <v>138</v>
@@ -7210,28 +7219,28 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B6" s="1">
-        <v>10</v>
+        <v>105</v>
       </c>
       <c r="C6" s="1">
-        <v>10</v>
+        <v>120</v>
       </c>
       <c r="D6" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="E6" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="F6" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="G6" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="H6" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="I6">
         <v>1</v>
@@ -7242,13 +7251,13 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B7" s="1">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="C7" s="1">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="D7" t="s">
         <v>5</v>
@@ -7257,10 +7266,10 @@
         <v>79</v>
       </c>
       <c r="F7" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="G7" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="H7" t="s">
         <v>140</v>
@@ -7274,28 +7283,28 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B8" s="1">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="C8" s="1">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D8" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="E8" t="s">
-        <v>13</v>
+        <v>79</v>
       </c>
       <c r="F8" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="G8" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="H8" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="I8">
         <v>1</v>
@@ -7306,10 +7315,10 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B9" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C9" s="1">
         <v>18</v>
@@ -7321,10 +7330,10 @@
         <v>13</v>
       </c>
       <c r="F9" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="G9" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="H9" t="s">
         <v>138</v>
@@ -7337,10 +7346,32 @@
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
+      <c r="A10" t="s">
+        <v>82</v>
+      </c>
+      <c r="B10" s="1">
+        <v>1</v>
+      </c>
+      <c r="C10" s="1">
+        <v>18</v>
+      </c>
+      <c r="D10" t="s">
+        <v>12</v>
+      </c>
+      <c r="E10" t="s">
+        <v>13</v>
+      </c>
+      <c r="F10" t="s">
+        <v>400</v>
+      </c>
+      <c r="G10" t="s">
+        <v>194</v>
+      </c>
       <c r="H10" t="s">
-        <v>255</v>
+        <v>138</v>
+      </c>
+      <c r="I10">
+        <v>1</v>
       </c>
       <c r="J10" t="s">
         <v>278</v>
@@ -7350,39 +7381,17 @@
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="H11" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
       <c r="J11" t="s">
         <v>278</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
-        <v>83</v>
-      </c>
-      <c r="B12" s="1">
-        <v>1</v>
-      </c>
-      <c r="C12" s="1">
-        <v>4</v>
-      </c>
-      <c r="D12" t="s">
-        <v>12</v>
-      </c>
-      <c r="E12" t="s">
-        <v>79</v>
-      </c>
-      <c r="F12" t="s">
-        <v>401</v>
-      </c>
-      <c r="G12" t="s">
-        <v>195</v>
-      </c>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
       <c r="H12" t="s">
-        <v>138</v>
-      </c>
-      <c r="I12">
-        <v>1</v>
+        <v>260</v>
       </c>
       <c r="J12" t="s">
         <v>278</v>
@@ -7390,13 +7399,13 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B13" s="1">
-        <v>50</v>
+        <v>1</v>
       </c>
       <c r="C13" s="1">
-        <v>70</v>
+        <v>4</v>
       </c>
       <c r="D13" t="s">
         <v>12</v>
@@ -7405,10 +7414,10 @@
         <v>79</v>
       </c>
       <c r="F13" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="G13" t="s">
-        <v>235</v>
+        <v>195</v>
       </c>
       <c r="H13" t="s">
         <v>138</v>
@@ -7453,26 +7462,42 @@
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
+      <c r="A15" t="s">
+        <v>465</v>
+      </c>
+      <c r="B15">
+        <v>0.05</v>
+      </c>
+      <c r="C15">
+        <v>0.25</v>
+      </c>
+      <c r="D15" t="s">
+        <v>91</v>
+      </c>
+      <c r="E15" t="s">
+        <v>60</v>
+      </c>
+      <c r="F15" t="s">
+        <v>466</v>
+      </c>
+      <c r="G15" t="s">
+        <v>467</v>
+      </c>
       <c r="H15" t="s">
-        <v>260</v>
+        <v>138</v>
+      </c>
+      <c r="I15">
+        <v>1</v>
       </c>
       <c r="J15" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
-      <c r="F16" t="s">
-        <v>464</v>
-      </c>
-      <c r="G16" t="s">
-        <v>464</v>
-      </c>
       <c r="H16" t="s">
-        <v>254</v>
+        <v>260</v>
       </c>
       <c r="J16" t="s">
         <v>280</v>
@@ -7481,69 +7506,53 @@
     <row r="17" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
+      <c r="F17" t="s">
+        <v>464</v>
+      </c>
+      <c r="G17" t="s">
+        <v>464</v>
+      </c>
       <c r="H17" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="J17" t="s">
         <v>280</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
-        <v>85</v>
-      </c>
-      <c r="B18" s="1">
-        <v>14</v>
-      </c>
-      <c r="C18" s="1">
-        <v>26</v>
-      </c>
-      <c r="D18" t="s">
-        <v>12</v>
-      </c>
-      <c r="E18" t="s">
-        <v>86</v>
-      </c>
-      <c r="F18" t="s">
-        <v>404</v>
-      </c>
-      <c r="G18" t="s">
-        <v>198</v>
-      </c>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
       <c r="H18" t="s">
-        <v>138</v>
-      </c>
-      <c r="I18">
-        <v>1</v>
+        <v>255</v>
       </c>
       <c r="J18" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B19" s="1">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="C19" s="1">
-        <v>4</v>
+        <v>26</v>
       </c>
       <c r="D19" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="E19" t="s">
-        <v>79</v>
+        <v>86</v>
       </c>
       <c r="F19" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="G19" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="H19" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="I19">
         <v>1</v>
@@ -7554,13 +7563,13 @@
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B20" s="1">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="C20" s="1">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="D20" t="s">
         <v>5</v>
@@ -7569,10 +7578,10 @@
         <v>79</v>
       </c>
       <c r="F20" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="G20" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="H20" t="s">
         <v>140</v>
@@ -7586,28 +7595,28 @@
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B21" s="1">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="C21" s="1">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D21" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="E21" t="s">
-        <v>13</v>
+        <v>79</v>
       </c>
       <c r="F21" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="G21" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="H21" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="I21">
         <v>1</v>
@@ -7618,13 +7627,13 @@
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B22" s="1">
-        <v>40</v>
+        <v>6</v>
       </c>
       <c r="C22" s="1">
-        <v>60</v>
+        <v>11</v>
       </c>
       <c r="D22" t="s">
         <v>12</v>
@@ -7633,10 +7642,10 @@
         <v>13</v>
       </c>
       <c r="F22" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="G22" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="H22" t="s">
         <v>138</v>
@@ -7650,13 +7659,13 @@
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B23" s="1">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="C23" s="1">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="D23" t="s">
         <v>12</v>
@@ -7665,26 +7674,48 @@
         <v>13</v>
       </c>
       <c r="F23" t="s">
+        <v>408</v>
+      </c>
+      <c r="G23" t="s">
+        <v>200</v>
+      </c>
+      <c r="H23" t="s">
+        <v>138</v>
+      </c>
+      <c r="I23">
+        <v>1</v>
+      </c>
+      <c r="J23" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>92</v>
+      </c>
+      <c r="B24" s="1">
+        <v>20</v>
+      </c>
+      <c r="C24" s="1">
+        <v>50</v>
+      </c>
+      <c r="D24" t="s">
+        <v>12</v>
+      </c>
+      <c r="E24" t="s">
+        <v>13</v>
+      </c>
+      <c r="F24" t="s">
         <v>409</v>
       </c>
-      <c r="G23" t="s">
+      <c r="G24" t="s">
         <v>410</v>
       </c>
-      <c r="H23" t="s">
-        <v>138</v>
-      </c>
-      <c r="I23">
-        <v>1</v>
-      </c>
-      <c r="J23" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B24" s="1"/>
-      <c r="C24" s="1"/>
       <c r="H24" t="s">
-        <v>255</v>
+        <v>138</v>
+      </c>
+      <c r="I24">
+        <v>1</v>
       </c>
       <c r="J24" t="s">
         <v>280</v>
@@ -7694,53 +7725,31 @@
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
       <c r="H25" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
       <c r="J25" t="s">
         <v>280</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A26" t="s">
-        <v>153</v>
-      </c>
-      <c r="B26" s="1">
-        <v>0.1</v>
-      </c>
-      <c r="C26" s="1">
-        <v>0.3</v>
-      </c>
-      <c r="D26" t="s">
-        <v>91</v>
-      </c>
-      <c r="E26" t="s">
-        <v>60</v>
-      </c>
-      <c r="F26" t="s">
-        <v>411</v>
-      </c>
-      <c r="G26" t="s">
-        <v>201</v>
-      </c>
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
       <c r="H26" t="s">
-        <v>138</v>
-      </c>
-      <c r="I26">
-        <v>0.01</v>
+        <v>260</v>
       </c>
       <c r="J26" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B27" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="C27" s="1">
         <v>0.3</v>
-      </c>
-      <c r="C27" s="1">
-        <v>0.7</v>
       </c>
       <c r="D27" t="s">
         <v>91</v>
@@ -7749,10 +7758,10 @@
         <v>60</v>
       </c>
       <c r="F27" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="G27" t="s">
-        <v>214</v>
+        <v>201</v>
       </c>
       <c r="H27" t="s">
         <v>138</v>
@@ -7766,57 +7775,57 @@
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>93</v>
+        <v>154</v>
       </c>
       <c r="B28" s="1">
-        <v>1</v>
+        <v>0.3</v>
       </c>
       <c r="C28" s="1">
-        <v>5</v>
+        <v>0.7</v>
       </c>
       <c r="D28" t="s">
-        <v>12</v>
+        <v>91</v>
       </c>
       <c r="E28" t="s">
-        <v>175</v>
+        <v>60</v>
       </c>
       <c r="F28" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="G28" t="s">
-        <v>202</v>
+        <v>214</v>
       </c>
       <c r="H28" t="s">
         <v>138</v>
       </c>
       <c r="I28">
-        <v>1</v>
+        <v>0.01</v>
       </c>
       <c r="J28" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B29" s="1">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="C29" s="1">
-        <v>130</v>
+        <v>5</v>
       </c>
       <c r="D29" t="s">
         <v>12</v>
       </c>
       <c r="E29" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="F29" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="G29" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="H29" t="s">
         <v>138</v>
@@ -7825,30 +7834,30 @@
         <v>1</v>
       </c>
       <c r="J29" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B30" s="1">
-        <v>70</v>
+        <v>20</v>
       </c>
       <c r="C30" s="1">
-        <v>320</v>
+        <v>130</v>
       </c>
       <c r="D30" t="s">
         <v>12</v>
       </c>
       <c r="E30" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="F30" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="G30" t="s">
-        <v>416</v>
+        <v>207</v>
       </c>
       <c r="H30" t="s">
         <v>138</v>
@@ -7862,13 +7871,13 @@
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B31" s="1">
-        <v>400</v>
+        <v>70</v>
       </c>
       <c r="C31" s="1">
-        <v>1300</v>
+        <v>320</v>
       </c>
       <c r="D31" t="s">
         <v>12</v>
@@ -7877,10 +7886,10 @@
         <v>176</v>
       </c>
       <c r="F31" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="G31" t="s">
-        <v>204</v>
+        <v>416</v>
       </c>
       <c r="H31" t="s">
         <v>138</v>
@@ -7894,45 +7903,45 @@
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>152</v>
+        <v>94</v>
       </c>
       <c r="B32" s="1">
-        <v>0.1</v>
+        <v>400</v>
       </c>
       <c r="C32" s="1">
-        <v>0.6</v>
+        <v>1300</v>
       </c>
       <c r="D32" t="s">
-        <v>91</v>
+        <v>12</v>
       </c>
       <c r="E32" t="s">
-        <v>60</v>
+        <v>176</v>
       </c>
       <c r="F32" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="G32" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="H32" t="s">
         <v>138</v>
       </c>
       <c r="I32">
-        <v>0.01</v>
+        <v>1</v>
       </c>
       <c r="J32" t="s">
-        <v>278</v>
+        <v>282</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B33" s="1">
         <v>0.1</v>
       </c>
       <c r="C33" s="1">
-        <v>0.9</v>
+        <v>0.6</v>
       </c>
       <c r="D33" t="s">
         <v>91</v>
@@ -7941,10 +7950,10 @@
         <v>60</v>
       </c>
       <c r="F33" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="G33" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="H33" t="s">
         <v>138</v>
@@ -7953,6 +7962,38 @@
         <v>0.01</v>
       </c>
       <c r="J33" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
+        <v>151</v>
+      </c>
+      <c r="B34" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="C34" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="D34" t="s">
+        <v>91</v>
+      </c>
+      <c r="E34" t="s">
+        <v>60</v>
+      </c>
+      <c r="F34" t="s">
+        <v>419</v>
+      </c>
+      <c r="G34" t="s">
+        <v>205</v>
+      </c>
+      <c r="H34" t="s">
+        <v>138</v>
+      </c>
+      <c r="I34">
+        <v>0.01</v>
+      </c>
+      <c r="J34" t="s">
         <v>278</v>
       </c>
     </row>
@@ -7965,7 +8006,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7AD55CD1-0195-43C4-85D0-979B3B5F4C61}">
   <dimension ref="A1:J26"/>
   <sheetViews>
-    <sheetView topLeftCell="D16" workbookViewId="0">
+    <sheetView topLeftCell="D1" workbookViewId="0">
       <selection activeCell="D16" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
rearrange EVPI message in three rows
</commit_message>
<xml_diff>
--- a/data/Walnut_grain_veg_tub.xlsx
+++ b/data/Walnut_grain_veg_tub.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mjimenez\Documents\ReForest\Living Labs for Mitigating Climate Change in Agriculture\DualPurpose_Trees\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E50B32E-216D-4831-9403-335652412C85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C080712-54F1-4D6A-B5E4-D025D44EEDFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-80" yWindow="-80" windowWidth="19360" windowHeight="11440" firstSheet="1" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-80" yWindow="-80" windowWidth="19360" windowHeight="11440" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sheet_names" sheetId="17" r:id="rId1"/>
@@ -4036,8 +4036,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06826C72-96B8-4DB0-B8A1-5FBF5F35F3F2}">
   <dimension ref="A1:J121"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4086,10 +4086,10 @@
         <v>7</v>
       </c>
       <c r="B2" s="1">
-        <v>40</v>
+        <v>80</v>
       </c>
       <c r="C2" s="1">
-        <v>40</v>
+        <v>80</v>
       </c>
       <c r="D2" t="s">
         <v>5</v>
@@ -4739,7 +4739,7 @@
   <dimension ref="A1:K118"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:J5"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -7105,7 +7105,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5B46F03-BBFE-4EF0-AFCA-0F4C3592A7D1}">
   <dimension ref="A1:J34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Titles and footnotes added to the plots "app.R" file
</commit_message>
<xml_diff>
--- a/data/Walnut_grain_veg_tub.xlsx
+++ b/data/Walnut_grain_veg_tub.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mjimenez\Documents\ReForest\Living Labs for Mitigating Climate Change in Agriculture\DualPurpose_Trees\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C080712-54F1-4D6A-B5E4-D025D44EEDFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{957E4CFC-08D0-4541-9F98-45EFBF109197}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-80" yWindow="-80" windowWidth="19360" windowHeight="11440" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="1650" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sheet_names" sheetId="17" r:id="rId1"/>
@@ -2411,7 +2411,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E807E7F-DCAE-400C-B9F4-3C0EDF692711}">
   <dimension ref="A1:J5"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D1" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
@@ -2593,7 +2593,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{724F1830-3430-4657-920D-E95506196AA8}">
   <dimension ref="A1:J29"/>
   <sheetViews>
-    <sheetView topLeftCell="B19" workbookViewId="0">
+    <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="B19" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
@@ -3291,7 +3291,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2682F285-7B44-4D8F-A7EA-4445FB570320}">
   <dimension ref="A1:J122"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C1" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
@@ -3855,7 +3855,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0AACA546-DF26-443B-AA33-3E83721C2724}">
   <dimension ref="A1:J5"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D1" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
@@ -4036,8 +4036,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06826C72-96B8-4DB0-B8A1-5FBF5F35F3F2}">
   <dimension ref="A1:J121"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4214,10 +4214,10 @@
         <v>4</v>
       </c>
       <c r="B6" s="1">
-        <v>10000</v>
+        <v>1000</v>
       </c>
       <c r="C6" s="1">
-        <v>10000</v>
+        <v>1000</v>
       </c>
       <c r="D6" t="s">
         <v>5</v>
@@ -5521,8 +5521,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8D4214A-8AE9-4396-ABE5-C95E3D310602}">
   <dimension ref="A1:J27"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A24" sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5895,7 +5895,7 @@
         <v>1</v>
       </c>
       <c r="C12" s="1">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="D12" t="s">
         <v>12</v>
@@ -6380,7 +6380,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C0D7C64-12CB-4A85-A4CD-D098869794C1}">
   <dimension ref="A1:J22"/>
   <sheetViews>
-    <sheetView topLeftCell="C10" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:K22"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
bigger update - clean up of code. save/load/delte/download functionality dynamic crop rotation test (commented out).
</commit_message>
<xml_diff>
--- a/data/Walnut_grain_veg_tub.xlsx
+++ b/data/Walnut_grain_veg_tub.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mjimenez\Documents\ReForest\Living Labs for Mitigating Climate Change in Agriculture\DualPurpose_Trees\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\belgium_app\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E69EF1A-F279-47EC-8BAE-E95DCEFA7E40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B826A9BA-35D4-485D-9C7F-296621A6C972}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="1650" windowWidth="29040" windowHeight="15720" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sheet_names" sheetId="17" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1086" uniqueCount="468">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1099" uniqueCount="469">
   <si>
     <t>variable</t>
   </si>
@@ -1436,6 +1436,9 @@
   </si>
   <si>
     <t>tree_mortality_chance_t</t>
+  </si>
+  <si>
+    <t>Crop_rotation</t>
   </si>
 </sst>
 </file>
@@ -1933,48 +1936,48 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
-    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="20 % - Akzent1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20 % - Akzent2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20 % - Akzent3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20 % - Akzent4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20 % - Akzent5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20 % - Akzent6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40 % - Akzent1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40 % - Akzent2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40 % - Akzent3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40 % - Akzent4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40 % - Akzent5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40 % - Akzent6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60 % - Akzent1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60 % - Akzent2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60 % - Akzent3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60 % - Akzent4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60 % - Akzent5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60 % - Akzent6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Akzent1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Akzent2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Akzent3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Akzent4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Akzent5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Akzent6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Ausgabe" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Berechnung" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Eingabe" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Ergebnis" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Erklärender Text" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Gut" xfId="6" builtinId="26" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="Notiz" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Schlecht" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Überschrift" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Überschrift 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Überschrift 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Überschrift 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Überschrift 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Verknüpfte Zelle" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Warnender Text" xfId="14" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="Zelle überprüfen" xfId="13" builtinId="23" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1990,7 +1993,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -2289,15 +2292,15 @@
   <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B13"/>
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="37.1796875" customWidth="1"/>
+    <col min="1" max="1" width="37.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>158</v>
       </c>
@@ -2305,7 +2308,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>159</v>
       </c>
@@ -2313,7 +2316,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>163</v>
       </c>
@@ -2321,7 +2324,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>164</v>
       </c>
@@ -2329,7 +2332,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>160</v>
       </c>
@@ -2337,7 +2340,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>167</v>
       </c>
@@ -2345,7 +2348,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>165</v>
       </c>
@@ -2353,7 +2356,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>166</v>
       </c>
@@ -2361,7 +2364,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>168</v>
       </c>
@@ -2369,7 +2372,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>169</v>
       </c>
@@ -2377,7 +2380,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>161</v>
       </c>
@@ -2385,7 +2388,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>170</v>
       </c>
@@ -2393,7 +2396,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>162</v>
       </c>
@@ -2409,22 +2412,23 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E807E7F-DCAE-400C-B9F4-3C0EDF692711}">
-  <dimension ref="A1:J5"/>
+  <dimension ref="A1:K5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.26953125" customWidth="1"/>
-    <col min="2" max="2" width="11.453125" customWidth="1"/>
-    <col min="3" max="3" width="10.81640625" customWidth="1"/>
-    <col min="6" max="6" width="94.1796875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.453125" customWidth="1"/>
+    <col min="1" max="1" width="28.28515625" customWidth="1"/>
+    <col min="2" max="2" width="11.42578125" customWidth="1"/>
+    <col min="3" max="3" width="10.85546875" customWidth="1"/>
+    <col min="6" max="6" width="94.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.42578125" customWidth="1"/>
+    <col min="10" max="10" width="33.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2455,8 +2459,11 @@
       <c r="J1" t="s">
         <v>247</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K1" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>57</v>
       </c>
@@ -2488,7 +2495,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>61</v>
       </c>
@@ -2520,7 +2527,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>59</v>
       </c>
@@ -2552,7 +2559,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>58</v>
       </c>
@@ -2591,20 +2598,20 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{724F1830-3430-4657-920D-E95506196AA8}">
-  <dimension ref="A1:J29"/>
+  <dimension ref="A1:K29"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B19" sqref="A1:XFD1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="38.81640625" customWidth="1"/>
-    <col min="6" max="6" width="80.1796875" customWidth="1"/>
-    <col min="9" max="9" width="18.453125" customWidth="1"/>
+    <col min="1" max="1" width="38.85546875" customWidth="1"/>
+    <col min="6" max="6" width="80.140625" customWidth="1"/>
+    <col min="9" max="9" width="18.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2635,8 +2642,11 @@
       <c r="J1" t="s">
         <v>247</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K1" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>104</v>
       </c>
@@ -2668,7 +2678,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>111</v>
       </c>
@@ -2700,7 +2710,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="H4" t="s">
@@ -2710,7 +2720,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
       <c r="F5" t="s">
@@ -2726,7 +2736,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
       <c r="H6" t="s">
@@ -2736,7 +2746,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>106</v>
       </c>
@@ -2762,13 +2772,13 @@
         <v>138</v>
       </c>
       <c r="I7">
-        <v>1</v>
+        <v>1E-3</v>
       </c>
       <c r="J7" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>107</v>
       </c>
@@ -2793,11 +2803,14 @@
       <c r="H8" t="s">
         <v>138</v>
       </c>
+      <c r="I8">
+        <v>0.01</v>
+      </c>
       <c r="J8" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>108</v>
       </c>
@@ -2822,11 +2835,14 @@
       <c r="H9" t="s">
         <v>138</v>
       </c>
+      <c r="I9">
+        <v>0.1</v>
+      </c>
       <c r="J9" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>150</v>
       </c>
@@ -2851,11 +2867,14 @@
       <c r="H10" t="s">
         <v>138</v>
       </c>
+      <c r="I10">
+        <v>0.1</v>
+      </c>
       <c r="J10" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="H11" t="s">
@@ -2865,7 +2884,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="F12" t="s">
@@ -2881,7 +2900,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="H13" t="s">
@@ -2891,7 +2910,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>112</v>
       </c>
@@ -2923,7 +2942,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>113</v>
       </c>
@@ -2955,7 +2974,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>114</v>
       </c>
@@ -2981,13 +3000,13 @@
         <v>138</v>
       </c>
       <c r="I16">
-        <v>1</v>
+        <v>1E-3</v>
       </c>
       <c r="J16" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>116</v>
       </c>
@@ -3013,13 +3032,13 @@
         <v>138</v>
       </c>
       <c r="I17">
-        <v>1</v>
+        <v>1E-4</v>
       </c>
       <c r="J17" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>117</v>
       </c>
@@ -3044,11 +3063,14 @@
       <c r="H18" t="s">
         <v>138</v>
       </c>
+      <c r="I18">
+        <v>1</v>
+      </c>
       <c r="J18" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>118</v>
       </c>
@@ -3073,11 +3095,14 @@
       <c r="H19" t="s">
         <v>138</v>
       </c>
+      <c r="I19">
+        <v>1</v>
+      </c>
       <c r="J19" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>119</v>
       </c>
@@ -3109,7 +3134,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>149</v>
       </c>
@@ -3141,7 +3166,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>148</v>
       </c>
@@ -3173,7 +3198,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>121</v>
       </c>
@@ -3198,11 +3223,14 @@
       <c r="H23" t="s">
         <v>138</v>
       </c>
+      <c r="I23">
+        <v>0.01</v>
+      </c>
       <c r="J23" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>123</v>
       </c>
@@ -3227,11 +3255,14 @@
       <c r="H24" t="s">
         <v>138</v>
       </c>
+      <c r="I24">
+        <v>0.01</v>
+      </c>
       <c r="J24" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>147</v>
       </c>
@@ -3256,29 +3287,32 @@
       <c r="H25" t="s">
         <v>138</v>
       </c>
+      <c r="I25">
+        <v>1E-3</v>
+      </c>
       <c r="J25" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
       <c r="H26" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
       <c r="H27" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
     </row>
@@ -3289,20 +3323,20 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2682F285-7B44-4D8F-A7EA-4445FB570320}">
-  <dimension ref="A1:J122"/>
+  <dimension ref="A1:K122"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="A1:XFD1048576"/>
+      <selection activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="29.1796875" customWidth="1"/>
-    <col min="6" max="6" width="52.81640625" customWidth="1"/>
-    <col min="9" max="9" width="18.453125" customWidth="1"/>
+    <col min="1" max="1" width="29.140625" customWidth="1"/>
+    <col min="6" max="6" width="52.85546875" customWidth="1"/>
+    <col min="9" max="9" width="18.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3333,8 +3367,11 @@
       <c r="J1" t="s">
         <v>247</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K1" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>157</v>
       </c>
@@ -3366,483 +3403,483 @@
         <v>284</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
     </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
     </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
     </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
     </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
     </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
     </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
     </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
     </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
     </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
     </row>
-    <row r="27" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
     </row>
-    <row r="28" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
     </row>
-    <row r="29" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
     </row>
-    <row r="30" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
     </row>
-    <row r="31" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="31" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
     </row>
-    <row r="32" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="32" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
     </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
     </row>
-    <row r="34" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
     </row>
-    <row r="35" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
     </row>
-    <row r="36" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="36" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
     </row>
-    <row r="37" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="37" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
     </row>
-    <row r="38" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="38" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
     </row>
-    <row r="39" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="39" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
     </row>
-    <row r="40" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="40" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
     </row>
-    <row r="41" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="41" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
     </row>
-    <row r="42" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="42" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
     </row>
-    <row r="43" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="43" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
     </row>
-    <row r="44" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="44" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
     </row>
-    <row r="45" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="45" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
     </row>
-    <row r="46" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="46" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>
     </row>
-    <row r="47" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="47" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
     </row>
-    <row r="48" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="48" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B48" s="1"/>
       <c r="C48" s="1"/>
     </row>
-    <row r="49" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="49" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B49" s="1"/>
       <c r="C49" s="1"/>
     </row>
-    <row r="50" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="50" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B50" s="1"/>
       <c r="C50" s="1"/>
     </row>
-    <row r="51" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="51" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B51" s="1"/>
       <c r="C51" s="1"/>
     </row>
-    <row r="52" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="52" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B52" s="1"/>
       <c r="C52" s="1"/>
     </row>
-    <row r="53" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="53" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B53" s="1"/>
       <c r="C53" s="1"/>
     </row>
-    <row r="54" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="54" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B54" s="1"/>
       <c r="C54" s="1"/>
     </row>
-    <row r="55" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="55" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B55" s="1"/>
       <c r="C55" s="1"/>
     </row>
-    <row r="56" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="56" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B56" s="1"/>
       <c r="C56" s="1"/>
     </row>
-    <row r="57" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="57" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B57" s="1"/>
       <c r="C57" s="1"/>
     </row>
-    <row r="58" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="58" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B58" s="1"/>
       <c r="C58" s="1"/>
     </row>
-    <row r="59" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="59" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B59" s="1"/>
       <c r="C59" s="1"/>
     </row>
-    <row r="60" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="60" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B60" s="1"/>
       <c r="C60" s="1"/>
     </row>
-    <row r="61" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="61" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B61" s="1"/>
       <c r="C61" s="1"/>
     </row>
-    <row r="62" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="62" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B62" s="1"/>
       <c r="C62" s="1"/>
     </row>
-    <row r="63" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="63" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B63" s="1"/>
       <c r="C63" s="1"/>
     </row>
-    <row r="64" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="64" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B64" s="1"/>
       <c r="C64" s="1"/>
     </row>
-    <row r="65" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="65" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B65" s="1"/>
       <c r="C65" s="1"/>
     </row>
-    <row r="66" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="66" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B66" s="1"/>
       <c r="C66" s="1"/>
     </row>
-    <row r="67" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="67" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B67" s="1"/>
       <c r="C67" s="1"/>
     </row>
-    <row r="68" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="68" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B68" s="1"/>
       <c r="C68" s="1"/>
     </row>
-    <row r="69" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="69" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B69" s="1"/>
       <c r="C69" s="1"/>
     </row>
-    <row r="70" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="70" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B70" s="1"/>
       <c r="C70" s="1"/>
     </row>
-    <row r="71" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="71" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B71" s="1"/>
       <c r="C71" s="1"/>
     </row>
-    <row r="72" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="72" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B72" s="1"/>
       <c r="C72" s="1"/>
     </row>
-    <row r="73" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="73" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B73" s="1"/>
       <c r="C73" s="1"/>
     </row>
-    <row r="74" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="74" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B74" s="1"/>
       <c r="C74" s="1"/>
     </row>
-    <row r="75" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="75" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B75" s="1"/>
       <c r="C75" s="1"/>
     </row>
-    <row r="76" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="76" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B76" s="1"/>
       <c r="C76" s="1"/>
     </row>
-    <row r="77" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="77" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B77" s="1"/>
       <c r="C77" s="1"/>
     </row>
-    <row r="78" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="78" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B78" s="1"/>
       <c r="C78" s="1"/>
     </row>
-    <row r="79" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="79" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B79" s="1"/>
       <c r="C79" s="1"/>
     </row>
-    <row r="80" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="80" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B80" s="1"/>
       <c r="C80" s="1"/>
     </row>
-    <row r="81" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="81" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B81" s="1"/>
       <c r="C81" s="1"/>
     </row>
-    <row r="82" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="82" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B82" s="1"/>
       <c r="C82" s="1"/>
     </row>
-    <row r="83" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="83" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B83" s="1"/>
       <c r="C83" s="1"/>
     </row>
-    <row r="84" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="84" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B84" s="1"/>
       <c r="C84" s="1"/>
     </row>
-    <row r="85" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="85" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B85" s="1"/>
       <c r="C85" s="1"/>
     </row>
-    <row r="86" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="86" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B86" s="1"/>
       <c r="C86" s="1"/>
     </row>
-    <row r="87" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="87" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B87" s="1"/>
       <c r="C87" s="1"/>
     </row>
-    <row r="88" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="88" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B88" s="1"/>
       <c r="C88" s="1"/>
     </row>
-    <row r="89" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="89" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B89" s="1"/>
       <c r="C89" s="1"/>
     </row>
-    <row r="90" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="90" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B90" s="1"/>
       <c r="C90" s="1"/>
     </row>
-    <row r="91" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="91" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B91" s="1"/>
       <c r="C91" s="1"/>
     </row>
-    <row r="92" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="92" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B92" s="1"/>
       <c r="C92" s="1"/>
     </row>
-    <row r="93" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="93" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B93" s="1"/>
       <c r="C93" s="1"/>
     </row>
-    <row r="94" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="94" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B94" s="1"/>
       <c r="C94" s="1"/>
     </row>
-    <row r="95" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="95" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B95" s="1"/>
       <c r="C95" s="1"/>
     </row>
-    <row r="96" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="96" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B96" s="1"/>
       <c r="C96" s="1"/>
     </row>
-    <row r="97" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="97" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B97" s="1"/>
       <c r="C97" s="1"/>
     </row>
-    <row r="98" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="98" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B98" s="1"/>
       <c r="C98" s="1"/>
     </row>
-    <row r="99" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="99" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B99" s="1"/>
       <c r="C99" s="1"/>
     </row>
-    <row r="100" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="100" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B100" s="1"/>
       <c r="C100" s="1"/>
     </row>
-    <row r="101" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="101" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B101" s="1"/>
       <c r="C101" s="1"/>
     </row>
-    <row r="102" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="102" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B102" s="1"/>
       <c r="C102" s="1"/>
     </row>
-    <row r="103" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="103" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B103" s="1"/>
       <c r="C103" s="1"/>
     </row>
-    <row r="104" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="104" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B104" s="1"/>
       <c r="C104" s="1"/>
     </row>
-    <row r="105" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="105" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B105" s="1"/>
       <c r="C105" s="1"/>
     </row>
-    <row r="106" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="106" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B106" s="1"/>
       <c r="C106" s="1"/>
     </row>
-    <row r="107" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="107" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B107" s="1"/>
       <c r="C107" s="1"/>
     </row>
-    <row r="108" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="108" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B108" s="1"/>
       <c r="C108" s="1"/>
     </row>
-    <row r="109" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="109" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B109" s="1"/>
       <c r="C109" s="1"/>
     </row>
-    <row r="110" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="110" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B110" s="1"/>
       <c r="C110" s="1"/>
     </row>
-    <row r="111" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="111" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B111" s="1"/>
       <c r="C111" s="1"/>
     </row>
-    <row r="112" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="112" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B112" s="1"/>
       <c r="C112" s="1"/>
     </row>
-    <row r="113" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="113" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B113" s="1"/>
       <c r="C113" s="1"/>
     </row>
-    <row r="114" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="114" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B114" s="1"/>
       <c r="C114" s="1"/>
     </row>
-    <row r="115" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="115" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B115" s="1"/>
       <c r="C115" s="1"/>
     </row>
-    <row r="116" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="116" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B116" s="1"/>
       <c r="C116" s="1"/>
     </row>
-    <row r="117" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="117" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B117" s="1"/>
       <c r="C117" s="1"/>
     </row>
-    <row r="118" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="118" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B118" s="1"/>
       <c r="C118" s="1"/>
     </row>
-    <row r="119" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="119" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B119" s="1"/>
       <c r="C119" s="1"/>
     </row>
-    <row r="120" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="120" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B120" s="1"/>
       <c r="C120" s="1"/>
     </row>
-    <row r="121" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="121" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B121" s="1"/>
       <c r="C121" s="1"/>
     </row>
-    <row r="122" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="122" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B122" s="1"/>
       <c r="C122" s="1"/>
     </row>
@@ -3853,23 +3890,23 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0AACA546-DF26-443B-AA33-3E83721C2724}">
-  <dimension ref="A1:J5"/>
+  <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="A1:XFD1048576"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="27" customWidth="1"/>
-    <col min="2" max="2" width="13.1796875" customWidth="1"/>
-    <col min="3" max="3" width="8.7265625" customWidth="1"/>
-    <col min="6" max="6" width="59.453125" customWidth="1"/>
-    <col min="7" max="7" width="33.54296875" customWidth="1"/>
+    <col min="2" max="2" width="13.140625" customWidth="1"/>
+    <col min="3" max="3" width="8.7109375" customWidth="1"/>
+    <col min="6" max="6" width="59.42578125" customWidth="1"/>
+    <col min="7" max="7" width="33.5703125" customWidth="1"/>
     <col min="9" max="9" width="37" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3885,6 +3922,9 @@
       <c r="E1" t="s">
         <v>135</v>
       </c>
+      <c r="F1" t="s">
+        <v>286</v>
+      </c>
       <c r="G1" t="s">
         <v>136</v>
       </c>
@@ -3897,8 +3937,11 @@
       <c r="J1" t="s">
         <v>247</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K1" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>37</v>
       </c>
@@ -3930,7 +3973,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>39</v>
       </c>
@@ -3962,7 +4005,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>156</v>
       </c>
@@ -3994,7 +4037,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>155</v>
       </c>
@@ -4034,22 +4077,22 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06826C72-96B8-4DB0-B8A1-5FBF5F35F3F2}">
-  <dimension ref="A1:J121"/>
+  <dimension ref="A1:K121"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="36.7265625" customWidth="1"/>
-    <col min="2" max="3" width="10.453125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="31.90625" customWidth="1"/>
-    <col min="7" max="7" width="30.453125" customWidth="1"/>
-    <col min="9" max="9" width="18.453125" customWidth="1"/>
+    <col min="1" max="1" width="36.7109375" customWidth="1"/>
+    <col min="2" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="31.85546875" customWidth="1"/>
+    <col min="7" max="7" width="73.5703125" customWidth="1"/>
+    <col min="9" max="9" width="18.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4080,8 +4123,11 @@
       <c r="J1" t="s">
         <v>247</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K1" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -4113,7 +4159,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -4145,7 +4191,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>54</v>
       </c>
@@ -4177,7 +4223,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>56</v>
       </c>
@@ -4209,7 +4255,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -4241,7 +4287,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -4273,459 +4319,459 @@
         <v>251</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
     </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
     </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
     </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
     </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
     </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
     </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
     </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
     </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
     </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
     </row>
-    <row r="27" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
     </row>
-    <row r="28" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
     </row>
-    <row r="29" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
     </row>
-    <row r="30" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
     </row>
-    <row r="31" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="31" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
     </row>
-    <row r="32" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="32" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
     </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
     </row>
-    <row r="34" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
     </row>
-    <row r="35" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
     </row>
-    <row r="36" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="36" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
     </row>
-    <row r="37" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="37" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
     </row>
-    <row r="38" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="38" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
     </row>
-    <row r="39" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="39" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
     </row>
-    <row r="40" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="40" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
     </row>
-    <row r="41" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="41" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
     </row>
-    <row r="42" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="42" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
     </row>
-    <row r="43" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="43" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
     </row>
-    <row r="44" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="44" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
     </row>
-    <row r="45" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="45" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
     </row>
-    <row r="46" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="46" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>
     </row>
-    <row r="47" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="47" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
     </row>
-    <row r="48" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="48" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B48" s="1"/>
       <c r="C48" s="1"/>
     </row>
-    <row r="49" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="49" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B49" s="1"/>
       <c r="C49" s="1"/>
     </row>
-    <row r="50" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="50" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B50" s="1"/>
       <c r="C50" s="1"/>
     </row>
-    <row r="51" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="51" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B51" s="1"/>
       <c r="C51" s="1"/>
     </row>
-    <row r="52" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="52" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B52" s="1"/>
       <c r="C52" s="1"/>
     </row>
-    <row r="53" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="53" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B53" s="1"/>
       <c r="C53" s="1"/>
     </row>
-    <row r="54" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="54" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B54" s="1"/>
       <c r="C54" s="1"/>
     </row>
-    <row r="55" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="55" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B55" s="1"/>
       <c r="C55" s="1"/>
     </row>
-    <row r="56" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="56" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B56" s="1"/>
       <c r="C56" s="1"/>
     </row>
-    <row r="57" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="57" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B57" s="1"/>
       <c r="C57" s="1"/>
     </row>
-    <row r="58" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="58" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B58" s="1"/>
       <c r="C58" s="1"/>
     </row>
-    <row r="59" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="59" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B59" s="1"/>
       <c r="C59" s="1"/>
     </row>
-    <row r="60" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="60" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B60" s="1"/>
       <c r="C60" s="1"/>
     </row>
-    <row r="61" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="61" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B61" s="1"/>
       <c r="C61" s="1"/>
     </row>
-    <row r="62" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="62" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B62" s="1"/>
       <c r="C62" s="1"/>
     </row>
-    <row r="63" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="63" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B63" s="1"/>
       <c r="C63" s="1"/>
     </row>
-    <row r="64" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="64" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B64" s="1"/>
       <c r="C64" s="1"/>
     </row>
-    <row r="65" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="65" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B65" s="1"/>
       <c r="C65" s="1"/>
     </row>
-    <row r="66" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="66" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B66" s="1"/>
       <c r="C66" s="1"/>
     </row>
-    <row r="67" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="67" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B67" s="1"/>
       <c r="C67" s="1"/>
     </row>
-    <row r="68" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="68" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B68" s="1"/>
       <c r="C68" s="1"/>
     </row>
-    <row r="69" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="69" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B69" s="1"/>
       <c r="C69" s="1"/>
     </row>
-    <row r="70" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="70" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B70" s="1"/>
       <c r="C70" s="1"/>
     </row>
-    <row r="71" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="71" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B71" s="1"/>
       <c r="C71" s="1"/>
     </row>
-    <row r="72" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="72" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B72" s="1"/>
       <c r="C72" s="1"/>
     </row>
-    <row r="73" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="73" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B73" s="1"/>
       <c r="C73" s="1"/>
     </row>
-    <row r="74" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="74" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B74" s="1"/>
       <c r="C74" s="1"/>
     </row>
-    <row r="75" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="75" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B75" s="1"/>
       <c r="C75" s="1"/>
     </row>
-    <row r="76" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="76" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B76" s="1"/>
       <c r="C76" s="1"/>
     </row>
-    <row r="77" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="77" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B77" s="1"/>
       <c r="C77" s="1"/>
     </row>
-    <row r="78" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="78" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B78" s="1"/>
       <c r="C78" s="1"/>
     </row>
-    <row r="79" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="79" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B79" s="1"/>
       <c r="C79" s="1"/>
     </row>
-    <row r="80" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="80" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B80" s="1"/>
       <c r="C80" s="1"/>
     </row>
-    <row r="81" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="81" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B81" s="1"/>
       <c r="C81" s="1"/>
     </row>
-    <row r="82" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="82" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B82" s="1"/>
       <c r="C82" s="1"/>
     </row>
-    <row r="83" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="83" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B83" s="1"/>
       <c r="C83" s="1"/>
     </row>
-    <row r="84" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="84" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B84" s="1"/>
       <c r="C84" s="1"/>
     </row>
-    <row r="85" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="85" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B85" s="1"/>
       <c r="C85" s="1"/>
     </row>
-    <row r="86" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="86" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B86" s="1"/>
       <c r="C86" s="1"/>
     </row>
-    <row r="87" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="87" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B87" s="1"/>
       <c r="C87" s="1"/>
     </row>
-    <row r="88" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="88" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B88" s="1"/>
       <c r="C88" s="1"/>
     </row>
-    <row r="89" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="89" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B89" s="1"/>
       <c r="C89" s="1"/>
     </row>
-    <row r="90" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="90" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B90" s="1"/>
       <c r="C90" s="1"/>
     </row>
-    <row r="91" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="91" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B91" s="1"/>
       <c r="C91" s="1"/>
     </row>
-    <row r="92" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="92" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B92" s="1"/>
       <c r="C92" s="1"/>
     </row>
-    <row r="93" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="93" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B93" s="1"/>
       <c r="C93" s="1"/>
     </row>
-    <row r="94" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="94" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B94" s="1"/>
       <c r="C94" s="1"/>
     </row>
-    <row r="95" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="95" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B95" s="1"/>
       <c r="C95" s="1"/>
     </row>
-    <row r="96" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="96" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B96" s="1"/>
       <c r="C96" s="1"/>
     </row>
-    <row r="97" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="97" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B97" s="1"/>
       <c r="C97" s="1"/>
     </row>
-    <row r="98" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="98" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B98" s="1"/>
       <c r="C98" s="1"/>
     </row>
-    <row r="99" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="99" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B99" s="1"/>
       <c r="C99" s="1"/>
     </row>
-    <row r="100" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="100" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B100" s="1"/>
       <c r="C100" s="1"/>
     </row>
-    <row r="101" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="101" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B101" s="1"/>
       <c r="C101" s="1"/>
     </row>
-    <row r="102" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="102" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B102" s="1"/>
       <c r="C102" s="1"/>
     </row>
-    <row r="103" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="103" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B103" s="1"/>
       <c r="C103" s="1"/>
     </row>
-    <row r="104" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="104" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B104" s="1"/>
       <c r="C104" s="1"/>
     </row>
-    <row r="105" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="105" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B105" s="1"/>
       <c r="C105" s="1"/>
     </row>
-    <row r="106" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="106" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B106" s="1"/>
       <c r="C106" s="1"/>
     </row>
-    <row r="107" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="107" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B107" s="1"/>
       <c r="C107" s="1"/>
     </row>
-    <row r="108" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="108" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B108" s="1"/>
       <c r="C108" s="1"/>
     </row>
-    <row r="109" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="109" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B109" s="1"/>
       <c r="C109" s="1"/>
     </row>
-    <row r="110" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="110" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B110" s="1"/>
       <c r="C110" s="1"/>
     </row>
-    <row r="111" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="111" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B111" s="1"/>
       <c r="C111" s="1"/>
     </row>
-    <row r="112" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="112" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B112" s="1"/>
       <c r="C112" s="1"/>
     </row>
-    <row r="113" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="113" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B113" s="1"/>
       <c r="C113" s="1"/>
     </row>
-    <row r="114" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="114" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B114" s="1"/>
       <c r="C114" s="1"/>
     </row>
-    <row r="115" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="115" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B115" s="1"/>
       <c r="C115" s="1"/>
     </row>
-    <row r="116" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="116" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B116" s="1"/>
       <c r="C116" s="1"/>
     </row>
-    <row r="117" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="117" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B117" s="1"/>
       <c r="C117" s="1"/>
     </row>
-    <row r="118" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="118" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B118" s="1"/>
       <c r="C118" s="1"/>
     </row>
-    <row r="119" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="119" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B119" s="1"/>
       <c r="C119" s="1"/>
     </row>
-    <row r="120" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="120" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B120" s="1"/>
       <c r="C120" s="1"/>
     </row>
-    <row r="121" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="121" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B121" s="1"/>
       <c r="C121" s="1"/>
     </row>
@@ -4739,17 +4785,17 @@
   <dimension ref="A1:K118"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="42.26953125" customWidth="1"/>
-    <col min="6" max="6" width="68.453125" customWidth="1"/>
-    <col min="9" max="9" width="18.453125" customWidth="1"/>
+    <col min="1" max="1" width="42.28515625" customWidth="1"/>
+    <col min="6" max="6" width="68.42578125" customWidth="1"/>
+    <col min="9" max="9" width="18.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4780,8 +4826,11 @@
       <c r="J1" t="s">
         <v>247</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="K1" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -4813,7 +4862,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -4846,7 +4895,7 @@
       </c>
       <c r="K3" s="1"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>17</v>
       </c>
@@ -4878,7 +4927,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -4910,455 +4959,455 @@
         <v>250</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
     </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
     </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
     </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
     </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
     </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
     </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
     </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
     </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
     </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
     </row>
-    <row r="27" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
     </row>
-    <row r="28" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
     </row>
-    <row r="29" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
     </row>
-    <row r="30" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
     </row>
-    <row r="31" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="31" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
     </row>
-    <row r="32" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="32" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
     </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
     </row>
-    <row r="34" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
     </row>
-    <row r="35" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
     </row>
-    <row r="36" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="36" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
     </row>
-    <row r="37" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="37" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
     </row>
-    <row r="38" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="38" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
     </row>
-    <row r="39" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="39" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
     </row>
-    <row r="40" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="40" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
     </row>
-    <row r="41" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="41" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
     </row>
-    <row r="42" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="42" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
     </row>
-    <row r="43" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="43" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
     </row>
-    <row r="44" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="44" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
     </row>
-    <row r="45" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="45" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
     </row>
-    <row r="46" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="46" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>
     </row>
-    <row r="47" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="47" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
     </row>
-    <row r="48" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="48" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B48" s="1"/>
       <c r="C48" s="1"/>
     </row>
-    <row r="49" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="49" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B49" s="1"/>
       <c r="C49" s="1"/>
     </row>
-    <row r="50" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="50" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B50" s="1"/>
       <c r="C50" s="1"/>
     </row>
-    <row r="51" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="51" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B51" s="1"/>
       <c r="C51" s="1"/>
     </row>
-    <row r="52" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="52" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B52" s="1"/>
       <c r="C52" s="1"/>
     </row>
-    <row r="53" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="53" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B53" s="1"/>
       <c r="C53" s="1"/>
     </row>
-    <row r="54" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="54" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B54" s="1"/>
       <c r="C54" s="1"/>
     </row>
-    <row r="55" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="55" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B55" s="1"/>
       <c r="C55" s="1"/>
     </row>
-    <row r="56" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="56" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B56" s="1"/>
       <c r="C56" s="1"/>
     </row>
-    <row r="57" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="57" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B57" s="1"/>
       <c r="C57" s="1"/>
     </row>
-    <row r="58" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="58" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B58" s="1"/>
       <c r="C58" s="1"/>
     </row>
-    <row r="59" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="59" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B59" s="1"/>
       <c r="C59" s="1"/>
     </row>
-    <row r="60" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="60" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B60" s="1"/>
       <c r="C60" s="1"/>
     </row>
-    <row r="61" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="61" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B61" s="1"/>
       <c r="C61" s="1"/>
     </row>
-    <row r="62" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="62" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B62" s="1"/>
       <c r="C62" s="1"/>
     </row>
-    <row r="63" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="63" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B63" s="1"/>
       <c r="C63" s="1"/>
     </row>
-    <row r="64" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="64" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B64" s="1"/>
       <c r="C64" s="1"/>
     </row>
-    <row r="65" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="65" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B65" s="1"/>
       <c r="C65" s="1"/>
     </row>
-    <row r="66" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="66" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B66" s="1"/>
       <c r="C66" s="1"/>
     </row>
-    <row r="67" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="67" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B67" s="1"/>
       <c r="C67" s="1"/>
     </row>
-    <row r="68" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="68" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B68" s="1"/>
       <c r="C68" s="1"/>
     </row>
-    <row r="69" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="69" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B69" s="1"/>
       <c r="C69" s="1"/>
     </row>
-    <row r="70" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="70" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B70" s="1"/>
       <c r="C70" s="1"/>
     </row>
-    <row r="71" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="71" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B71" s="1"/>
       <c r="C71" s="1"/>
     </row>
-    <row r="72" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="72" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B72" s="1"/>
       <c r="C72" s="1"/>
     </row>
-    <row r="73" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="73" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B73" s="1"/>
       <c r="C73" s="1"/>
     </row>
-    <row r="74" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="74" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B74" s="1"/>
       <c r="C74" s="1"/>
     </row>
-    <row r="75" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="75" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B75" s="1"/>
       <c r="C75" s="1"/>
     </row>
-    <row r="76" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="76" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B76" s="1"/>
       <c r="C76" s="1"/>
     </row>
-    <row r="77" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="77" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B77" s="1"/>
       <c r="C77" s="1"/>
     </row>
-    <row r="78" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="78" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B78" s="1"/>
       <c r="C78" s="1"/>
     </row>
-    <row r="79" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="79" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B79" s="1"/>
       <c r="C79" s="1"/>
     </row>
-    <row r="80" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="80" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B80" s="1"/>
       <c r="C80" s="1"/>
     </row>
-    <row r="81" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="81" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B81" s="1"/>
       <c r="C81" s="1"/>
     </row>
-    <row r="82" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="82" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B82" s="1"/>
       <c r="C82" s="1"/>
     </row>
-    <row r="83" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="83" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B83" s="1"/>
       <c r="C83" s="1"/>
     </row>
-    <row r="84" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="84" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B84" s="1"/>
       <c r="C84" s="1"/>
     </row>
-    <row r="85" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="85" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B85" s="1"/>
       <c r="C85" s="1"/>
     </row>
-    <row r="86" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="86" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B86" s="1"/>
       <c r="C86" s="1"/>
     </row>
-    <row r="87" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="87" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B87" s="1"/>
       <c r="C87" s="1"/>
     </row>
-    <row r="88" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="88" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B88" s="1"/>
       <c r="C88" s="1"/>
     </row>
-    <row r="89" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="89" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B89" s="1"/>
       <c r="C89" s="1"/>
     </row>
-    <row r="90" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="90" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B90" s="1"/>
       <c r="C90" s="1"/>
     </row>
-    <row r="91" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="91" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B91" s="1"/>
       <c r="C91" s="1"/>
     </row>
-    <row r="92" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="92" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B92" s="1"/>
       <c r="C92" s="1"/>
     </row>
-    <row r="93" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="93" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B93" s="1"/>
       <c r="C93" s="1"/>
     </row>
-    <row r="94" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="94" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B94" s="1"/>
       <c r="C94" s="1"/>
     </row>
-    <row r="95" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="95" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B95" s="1"/>
       <c r="C95" s="1"/>
     </row>
-    <row r="96" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="96" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B96" s="1"/>
       <c r="C96" s="1"/>
     </row>
-    <row r="97" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="97" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B97" s="1"/>
       <c r="C97" s="1"/>
     </row>
-    <row r="98" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="98" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B98" s="1"/>
       <c r="C98" s="1"/>
     </row>
-    <row r="99" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="99" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B99" s="1"/>
       <c r="C99" s="1"/>
     </row>
-    <row r="100" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="100" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B100" s="1"/>
       <c r="C100" s="1"/>
     </row>
-    <row r="101" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="101" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B101" s="1"/>
       <c r="C101" s="1"/>
     </row>
-    <row r="102" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="102" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B102" s="1"/>
       <c r="C102" s="1"/>
     </row>
-    <row r="103" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="103" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B103" s="1"/>
       <c r="C103" s="1"/>
     </row>
-    <row r="104" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="104" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B104" s="1"/>
       <c r="C104" s="1"/>
     </row>
-    <row r="105" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="105" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B105" s="1"/>
       <c r="C105" s="1"/>
     </row>
-    <row r="106" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="106" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B106" s="1"/>
       <c r="C106" s="1"/>
     </row>
-    <row r="107" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="107" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B107" s="1"/>
       <c r="C107" s="1"/>
     </row>
-    <row r="108" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="108" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B108" s="1"/>
       <c r="C108" s="1"/>
     </row>
-    <row r="109" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="109" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B109" s="1"/>
       <c r="C109" s="1"/>
     </row>
-    <row r="110" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="110" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B110" s="1"/>
       <c r="C110" s="1"/>
     </row>
-    <row r="111" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="111" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B111" s="1"/>
       <c r="C111" s="1"/>
     </row>
-    <row r="112" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="112" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B112" s="1"/>
       <c r="C112" s="1"/>
     </row>
-    <row r="113" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="113" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B113" s="1"/>
       <c r="C113" s="1"/>
     </row>
-    <row r="114" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="114" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B114" s="1"/>
       <c r="C114" s="1"/>
     </row>
-    <row r="115" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="115" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B115" s="1"/>
       <c r="C115" s="1"/>
     </row>
-    <row r="116" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="116" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B116" s="1"/>
       <c r="C116" s="1"/>
     </row>
-    <row r="117" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="117" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B117" s="1"/>
       <c r="C117" s="1"/>
     </row>
-    <row r="118" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="118" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B118" s="1"/>
       <c r="C118" s="1"/>
     </row>
@@ -5369,22 +5418,24 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FF733DD-E084-451A-AEBD-87D8A1F2D1F6}">
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="32.54296875" customWidth="1"/>
-    <col min="2" max="2" width="14.1796875" customWidth="1"/>
-    <col min="3" max="3" width="10.81640625" customWidth="1"/>
-    <col min="6" max="6" width="128.81640625" customWidth="1"/>
-    <col min="9" max="9" width="18.453125" customWidth="1"/>
+    <col min="1" max="1" width="32.5703125" customWidth="1"/>
+    <col min="2" max="2" width="14.140625" customWidth="1"/>
+    <col min="3" max="3" width="10.85546875" customWidth="1"/>
+    <col min="6" max="6" width="128.85546875" customWidth="1"/>
+    <col min="7" max="7" width="69.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.42578125" customWidth="1"/>
+    <col min="10" max="10" width="30.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -5415,8 +5466,11 @@
       <c r="J1" t="s">
         <v>247</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K1" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>19</v>
       </c>
@@ -5448,7 +5502,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -5480,7 +5534,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>21</v>
       </c>
@@ -5519,23 +5573,23 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8D4214A-8AE9-4396-ABE5-C95E3D310602}">
-  <dimension ref="A1:J27"/>
+  <dimension ref="A1:K27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="F35" sqref="F35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="47.453125" customWidth="1"/>
-    <col min="2" max="2" width="11.54296875" customWidth="1"/>
-    <col min="3" max="3" width="12.26953125" customWidth="1"/>
-    <col min="4" max="4" width="12.1796875" customWidth="1"/>
-    <col min="6" max="6" width="63.7265625" customWidth="1"/>
-    <col min="9" max="9" width="18.453125" customWidth="1"/>
+    <col min="1" max="1" width="47.42578125" customWidth="1"/>
+    <col min="2" max="2" width="11.5703125" customWidth="1"/>
+    <col min="3" max="3" width="12.28515625" customWidth="1"/>
+    <col min="4" max="4" width="12.140625" customWidth="1"/>
+    <col min="6" max="6" width="63.7109375" customWidth="1"/>
+    <col min="9" max="9" width="18.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -5566,8 +5620,11 @@
       <c r="J1" t="s">
         <v>247</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K1" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>22</v>
       </c>
@@ -5599,7 +5656,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>63</v>
       </c>
@@ -5631,7 +5688,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>65</v>
       </c>
@@ -5663,7 +5720,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>67</v>
       </c>
@@ -5695,7 +5752,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>69</v>
       </c>
@@ -5727,7 +5784,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>71</v>
       </c>
@@ -5759,7 +5816,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>73</v>
       </c>
@@ -5791,7 +5848,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>75</v>
       </c>
@@ -5823,7 +5880,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>36</v>
       </c>
@@ -5855,7 +5912,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>23</v>
       </c>
@@ -5887,7 +5944,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>26</v>
       </c>
@@ -5919,7 +5976,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>27</v>
       </c>
@@ -5945,13 +6002,13 @@
         <v>138</v>
       </c>
       <c r="I13">
-        <v>1</v>
+        <v>1E-3</v>
       </c>
       <c r="J13" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>29</v>
       </c>
@@ -5983,7 +6040,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>31</v>
       </c>
@@ -6015,7 +6072,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>32</v>
       </c>
@@ -6047,7 +6104,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>33</v>
       </c>
@@ -6079,7 +6136,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>34</v>
       </c>
@@ -6111,7 +6168,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>35</v>
       </c>
@@ -6143,7 +6200,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>98</v>
       </c>
@@ -6175,7 +6232,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>100</v>
       </c>
@@ -6207,7 +6264,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>101</v>
       </c>
@@ -6239,7 +6296,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>102</v>
       </c>
@@ -6271,7 +6328,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>103</v>
       </c>
@@ -6303,7 +6360,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>134</v>
       </c>
@@ -6335,7 +6392,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>143</v>
       </c>
@@ -6367,7 +6424,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
     </row>
@@ -6378,21 +6435,22 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C0D7C64-12CB-4A85-A4CD-D098869794C1}">
-  <dimension ref="A1:J22"/>
+  <dimension ref="A1:K22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:K22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K2" sqref="K2:K22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.453125" customWidth="1"/>
-    <col min="2" max="3" width="12.54296875" customWidth="1"/>
+    <col min="1" max="1" width="23.42578125" customWidth="1"/>
+    <col min="2" max="3" width="12.5703125" customWidth="1"/>
     <col min="6" max="6" width="87" customWidth="1"/>
-    <col min="9" max="9" width="18.453125" customWidth="1"/>
+    <col min="9" max="9" width="18.42578125" customWidth="1"/>
+    <col min="10" max="10" width="30.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -6423,8 +6481,11 @@
       <c r="J1" t="s">
         <v>247</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K1" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>64</v>
       </c>
@@ -6456,7 +6517,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>42</v>
       </c>
@@ -6488,7 +6549,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>43</v>
       </c>
@@ -6520,7 +6581,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>66</v>
       </c>
@@ -6552,7 +6613,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>44</v>
       </c>
@@ -6584,7 +6645,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>45</v>
       </c>
@@ -6616,7 +6677,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>68</v>
       </c>
@@ -6648,7 +6709,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>46</v>
       </c>
@@ -6680,7 +6741,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>47</v>
       </c>
@@ -6712,7 +6773,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>70</v>
       </c>
@@ -6744,7 +6805,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>48</v>
       </c>
@@ -6776,7 +6837,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>49</v>
       </c>
@@ -6808,7 +6869,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>72</v>
       </c>
@@ -6840,7 +6901,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>50</v>
       </c>
@@ -6872,7 +6933,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>51</v>
       </c>
@@ -6904,7 +6965,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>74</v>
       </c>
@@ -6936,7 +6997,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>52</v>
       </c>
@@ -6968,7 +7029,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>53</v>
       </c>
@@ -7000,7 +7061,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>62</v>
       </c>
@@ -7032,7 +7093,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>40</v>
       </c>
@@ -7064,7 +7125,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>41</v>
       </c>
@@ -7103,21 +7164,21 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5B46F03-BBFE-4EF0-AFCA-0F4C3592A7D1}">
-  <dimension ref="A1:J34"/>
+  <dimension ref="A1:K34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.1796875" customWidth="1"/>
-    <col min="3" max="4" width="12.453125" customWidth="1"/>
-    <col min="6" max="6" width="107.453125" customWidth="1"/>
-    <col min="9" max="9" width="18.453125" customWidth="1"/>
+    <col min="1" max="1" width="35.42578125" customWidth="1"/>
+    <col min="3" max="4" width="12.42578125" customWidth="1"/>
+    <col min="6" max="6" width="107.42578125" customWidth="1"/>
+    <col min="9" max="9" width="18.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -7148,8 +7209,11 @@
       <c r="J1" t="s">
         <v>247</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K1" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
       <c r="H2" t="s">
@@ -7159,7 +7223,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="F3" t="s">
@@ -7175,7 +7239,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="H4" t="s">
@@ -7185,7 +7249,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>84</v>
       </c>
@@ -7217,7 +7281,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>76</v>
       </c>
@@ -7249,7 +7313,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>78</v>
       </c>
@@ -7281,7 +7345,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>80</v>
       </c>
@@ -7313,7 +7377,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>81</v>
       </c>
@@ -7345,7 +7409,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>82</v>
       </c>
@@ -7377,7 +7441,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="H11" t="s">
@@ -7387,7 +7451,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="H12" t="s">
@@ -7397,7 +7461,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>83</v>
       </c>
@@ -7429,7 +7493,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>97</v>
       </c>
@@ -7461,7 +7525,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>467</v>
       </c>
@@ -7493,7 +7557,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
       <c r="H16" t="s">
@@ -7503,7 +7567,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
       <c r="F17" t="s">
@@ -7519,7 +7583,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
       <c r="H18" t="s">
@@ -7529,7 +7593,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>85</v>
       </c>
@@ -7561,7 +7625,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>87</v>
       </c>
@@ -7593,7 +7657,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>88</v>
       </c>
@@ -7625,7 +7689,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>89</v>
       </c>
@@ -7657,7 +7721,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>90</v>
       </c>
@@ -7689,7 +7753,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>92</v>
       </c>
@@ -7721,7 +7785,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
       <c r="H25" t="s">
@@ -7731,7 +7795,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
       <c r="H26" t="s">
@@ -7741,7 +7805,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>153</v>
       </c>
@@ -7773,7 +7837,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>154</v>
       </c>
@@ -7805,7 +7869,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>93</v>
       </c>
@@ -7837,7 +7901,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>96</v>
       </c>
@@ -7869,7 +7933,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>95</v>
       </c>
@@ -7901,7 +7965,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>94</v>
       </c>
@@ -7933,7 +7997,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>152</v>
       </c>
@@ -7965,7 +8029,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>151</v>
       </c>
@@ -8004,21 +8068,21 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7AD55CD1-0195-43C4-85D0-979B3B5F4C61}">
-  <dimension ref="A1:J26"/>
+  <dimension ref="A1:K26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A33" sqref="A33"/>
+      <selection activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="39.81640625" customWidth="1"/>
-    <col min="4" max="4" width="12.26953125" customWidth="1"/>
-    <col min="6" max="6" width="77.90625" customWidth="1"/>
-    <col min="9" max="9" width="18.453125" customWidth="1"/>
+    <col min="1" max="1" width="39.85546875" customWidth="1"/>
+    <col min="4" max="4" width="12.28515625" customWidth="1"/>
+    <col min="6" max="6" width="77.85546875" customWidth="1"/>
+    <col min="9" max="9" width="18.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -8049,8 +8113,11 @@
       <c r="J1" t="s">
         <v>247</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K1" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
       <c r="H2" t="s">
@@ -8060,7 +8127,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="F3" t="s">
@@ -8076,7 +8143,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="H4" t="s">
@@ -8086,7 +8153,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>124</v>
       </c>
@@ -8118,7 +8185,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>125</v>
       </c>
@@ -8150,7 +8217,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>126</v>
       </c>
@@ -8182,7 +8249,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>127</v>
       </c>
@@ -8214,7 +8281,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>128</v>
       </c>
@@ -8246,7 +8313,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="H10" t="s">
@@ -8256,7 +8323,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="H11" t="s">
@@ -8266,7 +8333,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>146</v>
       </c>
@@ -8298,7 +8365,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>129</v>
       </c>
@@ -8330,7 +8397,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>145</v>
       </c>
@@ -8362,7 +8429,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
       <c r="H15" t="s">
@@ -8372,7 +8439,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
       <c r="F16" t="s">
@@ -8388,7 +8455,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
       <c r="H17" t="s">
@@ -8398,7 +8465,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>144</v>
       </c>
@@ -8430,7 +8497,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>130</v>
       </c>
@@ -8462,7 +8529,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>131</v>
       </c>
@@ -8494,7 +8561,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>132</v>
       </c>
@@ -8526,7 +8593,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>133</v>
       </c>
@@ -8558,7 +8625,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
       <c r="H23" t="s">
@@ -8568,7 +8635,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
       <c r="H24" t="s">
@@ -8578,7 +8645,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>141</v>
       </c>
@@ -8610,7 +8677,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>142</v>
       </c>
@@ -8650,22 +8717,22 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E18C2264-89B4-41CF-A7EB-F2121007945D}">
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.26953125" customWidth="1"/>
-    <col min="2" max="2" width="10.54296875" customWidth="1"/>
-    <col min="3" max="3" width="11.54296875" customWidth="1"/>
-    <col min="6" max="6" width="47.81640625" customWidth="1"/>
-    <col min="9" max="9" width="18.453125" customWidth="1"/>
+    <col min="1" max="1" width="21.28515625" customWidth="1"/>
+    <col min="2" max="2" width="10.5703125" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" customWidth="1"/>
+    <col min="6" max="6" width="47.85546875" customWidth="1"/>
+    <col min="9" max="9" width="18.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -8696,8 +8763,11 @@
       <c r="J1" t="s">
         <v>247</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K1" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>25</v>
       </c>

</xml_diff>